<commit_message>
added nouns semantic classes
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD47ADB-E818-4665-AE3B-194B887191CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC496E17-2741-4EA9-98C1-117ED9D62C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="545">
   <si>
     <t>Feature</t>
   </si>
@@ -16762,6 +16762,455 @@
       </rPr>
       <t>apparent, certain, clear, confident, convinced, correct, evident, false, impossible, inevitable, obvious, positive, right, sure, true, well-known, doubtful, likely, possible, probable, unlikely</t>
     </r>
+  </si>
+  <si>
+    <t>NNABSPROC</t>
+  </si>
+  <si>
+    <t>NNCOG</t>
+  </si>
+  <si>
+    <t>Nouns cognitive</t>
+  </si>
+  <si>
+    <t>NNCONC</t>
+  </si>
+  <si>
+    <t>Nouns concrete</t>
+  </si>
+  <si>
+    <t>NNGRP</t>
+  </si>
+  <si>
+    <t>Nouns group</t>
+  </si>
+  <si>
+    <t>NNHUMAN</t>
+  </si>
+  <si>
+    <t>Nouns human</t>
+  </si>
+  <si>
+    <t>NNPLACE</t>
+  </si>
+  <si>
+    <t>Nouns place</t>
+  </si>
+  <si>
+    <t>NNQUANT</t>
+  </si>
+  <si>
+    <t>Nouns quantity</t>
+  </si>
+  <si>
+    <t>NNTECH</t>
+  </si>
+  <si>
+    <t>NOMZ</t>
+  </si>
+  <si>
+    <t>NSTNCother</t>
+  </si>
+  <si>
+    <t>Stance nouns without prepositions</t>
+  </si>
+  <si>
+    <t>Nouns abstract and process</t>
+  </si>
+  <si>
+    <t>Nominalizations</t>
+  </si>
+  <si>
+    <t>Nouns technical</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>airline, airlines, institute, institutes, colony, colonies, bank, banks, flight, flights, church, churches, hotel, hotels, firm, firms, hospital, hospitals, household, households, college, colleges, institution, institutions, house, houses, lab, labs, laboratory, laboratories, community, communities, company, companies, government, governments, university, universities, school, schools, home, homes, congress, congresses, committee, committees</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>action, actions, activity, activities, application, applications, argument, arguments, development, developments, education, educations, effect, effects, function, functions, method, methods, research, researches, result, results, process, processes, accounting, accountings, achievement, achievements, addition, additions, administration, administrations, approach, approaches, arrangement, arrangements, assignment, assignments, competition, competitions, construction, constructions, consumption, consumptions, contribution, contributions, counseling, counselings, criticism, criticisms, definition, definitions, discrimination, discriminations, description, descriptions, discussion, discussions, distribution, distributions, division, divisions, eruption, eruptions, evolution, evolutions, exchange, exchanges, exercise, exercises, experiment, experiments, explanation, explanations, expression, expressions, formation, formations, generation, generations, graduation, graduations, management, managements, marketing, marketings, marriage, marriages, mechanism, mechanisms, meeting, meetings, operation, operations, orientation, orientations, performance, performances, practice, practices, presentation, presentations, procedure, procedures, production, productions, progress, progresses, reaction, reactions, registration, registrations, regulation, regulations, revolution, revolutions, selection, selections, session, sessions, strategy, strategies, teaching, teachings, technique, techniques, tradition, traditions, training, trainings, transition, transitions, treatment, treatments, trial, trials, act, acts, agreement, agreements, attempt, attempts, attendance, attendances, birth, births, break, breaks, claim, claims, comment, comments, comparison, comparisons, conflict, conflicts, deal, deals, death, deaths, debate, debates, demand, demands, answer, answers, control, controls, flow, flows, service, services, work, works, test, tests, use, uses, war, wars, change, changes, question, questions, study, studies, talk, talks, task, tasks, trade, trades, transfer, transfers, admission, admissions, design, designs, detail, details, dimension, dimensions, direction, directions, disorder, disorders, diversity, diversities, economy, economies, emergency, emergencies, emphasis, emphases, employment, employments, equilibrium, equilibriums, equity, equities, error, errors, expense, expenses, facility, facilities, failure, failures, fallacy, fallacies, feature, features, format, formats, freedom, freedoms, fun, funs, gender, genders, goal, goals, grammar, grammars, health, healths, heat, heats, help, helps, identity, identities, image, images, impact, impacts, importance, importances, influence, influences, input, inputs, labor, labors, leadership, leaderships, link, links, manner, manners, math, maths, matrix, matrices, meaning, meanings, music, musics, network, networks, objective, objectives, opportunity, opportunities, option, options, origin, origins, output, outputs, past, pasts, pattern, patterns, phase, phases, philosophy, philosophies, plan, plans, potential, potentials, prerequisite, prerequisites, presence, presences, principle, principles, success, successes, profile, profiles, profit, profits, proposal, proposals, psychology, psychologies, quality, qualities, quiz, quizzes, race, races, reality, realities, religion, religions, resource, resources, respect, respects, rest, rests, return, returns, risk, risks, substance, substances, scene, scenes, security, securities, series, series, set, sets, setting, settings, sex, sexes, shape, shapes, share, shares, show, shows, sign, signs, signal, signals, sort, sorts, sound, sounds, spring, springs, stage, stages, standard, standards, start, starts, stimulus, stimuli, strength, strengths, stress, stresses, style, styles, support, supports, survey, surveys, symbol, symbols, topic, topics, track, tracks, trait, traits, trouble, troubles, truth, truths, variation, variations, variety, varieties, velocity, velocities, version, versions, whole, wholes, action, actions, account, accounts, condition, conditions, culture, cultures, end, ends, factor, factors, grade, grades, interest, interests, issue, issues, job, jobs, kind, kinds, language, languages, law, laws, level, levels, life, lives, model, models, name, names, nature, natures, order, orders, policy, policies, position, positions, power, powers, pressure, pressures, relationship, relationships, requirement, requirements, role, roles, rule, rules, science, sciences, side, sides, situation, situations, skill, skills, source, sources, structure, structures, subject, subjects, type, types, information, informations, right, rights, state, states, system, systems, value, values, way, ways, address, addresses, absence, absences, advantage, advantages, aid, aids, alternative, alternatives, aspect, aspects, authority, authorities, axis, axes, background, backgrounds, balance, balances, base, bases, beginning, beginnings, benefit, benefits, bias, biases, bond, bonds, capital, capitals, care, cares, career, careers, cause, causes, characteristic, characteristics, charge, charges, check, checks, choice, choices, circuit, circuits, circumstance, circumstances, climate, climates, code, codes, color, colors, column, columns, combination, combinations, complex, complexes, connection, connections, constant, constants, constraint, constraints, contact, contacts, content, contents, contract, contracts, context, contexts, contrast, contrasts, crime, crimes, criteria, criterias, cross, crosses, current, currents, curriculum, curriculums, curve, curves, debt, debts, density, densities</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>analysis, analyses, decision, decisions, experience, experiences, assessment, assessments, calculation, calculations, conclusion, conclusions, consequence, consequences, consideration, considerations, evaluation, evaluations, examination, examinations, expectation, expectations, observation, observations, recognition, recognitions, relation, relations, understanding, understandings, hypothesis, hypotheses, ability, abilities, assumption, assumptions, attention, attentions, attitude, attitudes, belief, beliefs, concentration, concentrations, concern, concerns, consciousness, consciousnesses, concept, concepts, fact, facts, idea, ideas, knowledge, knowledges, look, looks, need, needs, reason, reasons, sense, senses, view, views, theory, theories, desire, desires, emotion, emotions, feeling, feelings, judgement, judgements, memory, memories, notion, notions, opinion, opinions, perception, perceptions, perspective, perspectives, possibility, possibilities, probability, probabilities, responsibility, responsibilities, thought, thoughts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tank, tanks, stick, sticks, target, targets, strata, stratas, telephone, telephones, string, strings, telescope, telescopes, sugar, sugars, ticket, tickets, syllabus, syllabuses, tip, tips, salt, salts, tissue, tissues, screen, screens, tooth, teeth, sculpture, sculptures, sphere, spheres, seawater, seawaters, spot, spots, ship, ships, steam, steams, silica, silicas, steel, steels, slide, slides, stem, stems, snow, snows, sodium, mud, muds, solid, solids, mushroom, mushrooms, gift, gifts, muscle, muscles, glacier, glaciers, tube, tubes, gun, guns, nail, nails, handbook, handbooks, newspaper, newspapers, handout, handouts, node, nodes, instrument, instruments, notice, notices, knot, knots, novel, novels, lava, lavas, page, pages, food, foods, transcript, transcripts, leg, legs, eye, eyes, lemon, lemons, brain, brains, magazine, magazines, device, devices, magnet, magnets, oak, oaks, manual, manuals, package, packages, marker, markers, peak, peaks, match, matches, pen, pens, metal, metals, pencil, pencils, block, blocks, pie, pies, board, boards, pipe, pipes, heart, hearts, load, loads, paper, papers, transistor, transistors, modem, modems, book, books, mole, moles, case, cases, motor, motors, computer, computers, mound, mounds, dollar, dollars, mouth, mouths, hand, hands, movie, movies, flower, flowers, object, objects, foot, feet, table, tables, frame, frames, water, waters, vessel, vessels, arm, arms, visa, visas, bar, bars, grain, grains, bed, beds, hair, hairs, body, bodies, head, heads, box, boxes, ice, ices, car, cars, item, items, card, cards, journal, journals, chain, chains, key, keys, chair, chairs, window, windows, vehicle, vehicles, leaf, leaves, copy, copies, machine, machines, document, documents, mail, mails, door, doors, map, maps, dot, dots, phone, phones, drug, drugs, picture, pictures, truck, trucks, piece, pieces, tape, tapes, note, notes, liquid, liquids, wire, wires, equipment, equipments, wood, woods, fiber, fibers, plant, plants, fig, figs, resistor, resistors, film, films, sand, sands, file, files, score, scores, seat, seats, belt, belts, sediment, sediments, boat, boats, seed, seeds, bone, bones, soil, soils, bubble, bubbles, bud, buds, water, waters, bulb, bulbs, portrait, portraits, bulletin, bulletins, step, steps, shell, shells, stone, stones, cake, cakes, tree, trees, camera, cameras, video, videos, face, faces, wall, walls, acid, acids, alcohol, alcohols, cap, caps, aluminium, aluminiums, clay, clays, artifact, artifacts, clock, clocks, rain, rains, clothing, clothings, asteroid, asteroids, club, clubs, automobile, automobiles, comet, comets, award, awards, sheet, sheets, bag, bags, branch, branches, ball, balls, copper, coppers, banana, bananas, counter, counters, band, bands, cover, covers, wheel, wheels, crop, crops, drop, drops, crystal, crystals, basin, basins, cylinder, cylinders, bell, bells, desk, desks, dinner, dinners, pole, poles, button, buttons, pot, pots, disk, disks, pottery, potteries, drain, drains, radio, radios, drink, drinks, reactor, reactors, drawing, drawings, retina, retinas, dust, dusts, ridge, ridges, edge, edges, ring, rings, engine, engines, ripple, ripples, plate, plates, game, games, cent, cents, post, posts, envelope, envelopes, rock, rocks, filter, filters, root, roots, finger, fingers, slope, slopes, fish, fish, space, spaces, fruit, fruits, statue, statues, furniture, furnitures, textbook, textbooks, gap, gaps, tool, tools, gate, gates, train, trains, gel, gels, deposit, deposits, chart, charts, mixture, mixtures</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>family, families, guy, guys, individual, individuals, kid, kids, man, men, manager, managers, member, members, parent, parents, teacher, teachers, child, children, people, peoples, person, people, student, students, woman, women, animal, animals, applicant, applicants, author, authors, baby, babies, boy, boys, client, clients, consumer, consumers, critic, critics, customer, customers, doctor, doctors, employee, employees, employer, employers, father, fathers, female, females, friend, friends, girl, girls, god, gods, historian, historians, husband, husbands, American, Americans, Indian, Indians, instructor, instructors, king, kings, leader, leaders, male, males, mother, mothers, owner, owners, president, presidents, professor, professors, researcher, researchers, scholar, scholars, speaker, speakers, species, species, supplier, suppliers, undergraduate, undergraduates, user, users, wife, wives, worker, workers, writer, writers, accountant, accountants, adult, adults, adviser, advisers, agent, agents, aide, aides, ancestor, ancestors, anthropologist, anthropologists, archaeologist, archaeologists, artist, artists, artiste, artistes, assistant, assistants, associate, associates, attorney, attorneys, audience, audiences, auditor, auditors, bachelor, bachelors, bird, birds, boss, bosses, brother, brothers, buddha, buddhas, buyer, buyers, candidate, candidates, cat, cats, citizen, citizens, colleague, colleagues, collector, collectors, competitor, competitors, counselor, counselors, daughter, daughters, deer, deer, defendant, defendants, designer, designers, developer, developers, director, directors, driver, drivers, economist, economists, engineer, engineers, executive, executives, expert, experts, farmer, farmers, feminist, feminists, freshman, freshmen, eologist, eologists, hero, heroes, host, hosts, hunter, hunters, immigrant, immigrants, infant, infants, investor, investors, jew, jews, judge, judges, lady, ladies, lawyer, lawyers, learner, learners, listener, listeners, maker, makers, manufacturer, manufacturers, miller, millers, minister, ministers, mom, moms, monitor, monitors, monkey, monkeys, neighbor, neighbors, observer, observers, officer, officers, official, officials, participant, participants, partner, partners, patient, patients, personnel, personnels, peer, peers, physician, physicians, plaintiff, plaintiffs, player, players, poet, poets, police, polices, processor, processors, professional, professionals, provider, providers, psychologist, psychologists, resident, residents, respondent, respondents, schizophrenic, schizophrenics, scientist, scientists, secretary, secretaries, server, servers, shareholder, shareholders, sikh, sikhs, sister, sisters, slave, slaves, son, sons, spouse, spouses, supervisor, supervisors, theorist, theorists, tourist, tourists, victim, victims, faculty, faculties, dean, deans, engineer, engineers, reader, readers, couple, couples, graduate, graduates, Pakistani(s), Bangladeshi(s), Srilanakn(s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apartment, apartments, interior, interiors, bathroom, bathrooms, moon, moons, bay, bays, museum, museums, bench, benches, neighborhood, neighborhoods, bookstore, bookstores, opposite, opposites, border, borders, orbit, orbits, cave, caves, orbital, orbitals, continent, continents, outside, outsides, delta, deltas, parallel, parallels, desert, deserts, passage, passages, estuary, estuaries, pool, pools, factory, factories, prison, prisons, farm, farms, restaurant, restaurants, forest, forests, sector, sectors, habitat, habitats, shaft, shafts, hell, hells, shop, shops, hemisphere, hemispheres, southwest, hill, hills, station, stations, hole, holes, territory, territories, horizon, horizons, road, roads, bottom, bottoms, store, stores, boundary, boundaries, stream, streams, building, buildings, top, tops, campus, campuses, valley, valleys, canyon, canyons, village, villages, coast, coasts, city, cities, county, counties, country, countries, court, courts, earth, earths, front, fronts, environment, environments, district, districts, field, fields, floor, floors, market, markets, lake, lakes, office, offices, land, lands, organization, organizations, lecture, lectures, place, places, left, lefts, room, rooms, library, libraries, area, areas, location, locations, class, classes, middle, middles, classroom, classrooms, mountain, mountains, ground, grounds, north, norths, hall, halls, ocean, oceans, park, parks, planet, planets, property, properties, region, regions, residence, residences, river, rivers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cycle, cycles, rate, rates, date, dates, second, seconds, frequency, frequencies, section, sections, future, futures, semester, semesters, half, halves, temperature, temperatures, height, heights, today, todays, number, numbers, amount, amounts, week, weeks, age, ages, day, days, century, centuries, part, parts, energy, energies, lot, lots, heat, heats, term, terms, hour, hours, time, times, month, months, mile, miles, period, periods, moment, moments, morning, mornings, volume, volumes, per, weekend, weekends, percentage, percentages, weight, weights, portion, portions, minute, minutes, quantity, quantities, percent, percents, quarter, quarters, length, lengths, ratio, ratios, measure, measures, summer, summers, meter, meters, volt, volts, voltage, voltages</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not having an additional tag apart from the underscore separated </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cell, cells, unit, units, gene, genes, wave, waves, ion, ions, bacteria, bacterias, electron, electrons, chromosome, chromosomes, element, elements, cloud, clouds, sample, samples, isotope, isotopes, schedule, schedules, neuron, neurons, software, softwares, nuclei, nucleus, solution, solutions, nucleus, nuclei, atom, atoms, ray, rays, margin, margins, virus, viruses, mark, marks, hydrogen, hydrogens, mineral, minerals, internet, internets, molecule, molecules, mineral, minerals, organism, organisms, message, messages, oxygen, oxygens, paragraph, paragraphs, particle, particles, sentence, sentences, play, plays, star, stars, poem, poems, thesis, theses, proton, protons, unit, units, web, webs, layer, layers, center, centers, matter, matters, chapter, chapters, square, squares, data, circle, circles, equation, equations, compound, compounds, exam, exams, letter, letters, bill, bills, page, pages, component, components, statement, statements, diagram, diagrams, word, words, dna, angle, angles, fire, fires, carbon, carbons, formula, formulas, graph, graphs, iron, irons, lead, leads, jury, juries, light, lights, list, lists</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nouns ending at </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tion(s), ment(s), ness, nesses, ity, ities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having a length of greater than 5 characters and not having an additional tag aprt from the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_NN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag.</t>
+    </r>
+  </si>
+  <si>
+    <t>Biber 1988, Nini 2014 adapted by Shakir</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any of the following words tagged as noun and not followed by prepositions </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertion, assertions, conclusion, conclusions, conviction, convictions, discovery, discoveries, doubt, doubts, fact, facts, knowledge, knowledges, observation, observations, principle, principles, realization, realizations, result, results, statement, statements, assumption, assumptions, belief, beliefs, claim, claims, contention, contentions, feeling, feelings, hypothesis, hypotheses, idea, ideas, implication, implications, impression, impressions, notion, notions, opinion, opinions, possibility, possibilities, presumption, presumptions, suggestion, suggestions, grounds, ground, hope, hopes, reason, reasons, view, views, thought, thoughts, comment, comments, news, news, proposal, proposals, proposition, propositions, remark, remarks, report, reports, requirement, requirements, agreement, agreements, decision, decisions, desire, desires, failure, failures, inclination, inclinations, intention, intentions, obligation, obligations, opportunity, opportunities, plan, plans, promise, promises, reluctance, reluctances, responsibility, responsibilities, right, rights, tendency, tendencies, threat, threats, wish, wishes, willingness, willingnesses</t>
+    </r>
+  </si>
+  <si>
+    <t>Biber 2006, adapted by Shakir</t>
+  </si>
+  <si>
+    <t>Biber 2006, additions and adapted by Shakir</t>
   </si>
 </sst>
 </file>
@@ -17743,10 +18192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM136"/>
+  <dimension ref="A1:AMM146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E129" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4"/>
@@ -22045,11 +22494,11 @@
       <c r="E101" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="F101" s="20" t="s">
+      <c r="F101" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G101" s="20" t="s">
-        <v>96</v>
+        <v>543</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="110.4">
@@ -22066,11 +22515,11 @@
       <c r="E102" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="F102" s="20" t="s">
+      <c r="F102" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G102" s="20" t="s">
-        <v>96</v>
+        <v>543</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="110.4">
@@ -22086,11 +22535,11 @@
       <c r="E103" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="F103" s="20" t="s">
+      <c r="F103" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G103" s="20" t="s">
-        <v>96</v>
+        <v>543</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="110.4">
@@ -22106,11 +22555,11 @@
       <c r="E104" s="19" t="s">
         <v>412</v>
       </c>
-      <c r="F104" s="20" t="s">
+      <c r="F104" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G104" s="20" t="s">
-        <v>96</v>
+        <v>543</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="110.4">
@@ -22129,6 +22578,9 @@
       <c r="F105" s="19" t="s">
         <v>17</v>
       </c>
+      <c r="G105" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="106" spans="1:12" ht="110.4">
       <c r="A106" s="19" t="s">
@@ -22146,6 +22598,9 @@
       <c r="F106" s="19" t="s">
         <v>17</v>
       </c>
+      <c r="G106" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="107" spans="1:12" ht="110.4">
       <c r="A107" s="19" t="s">
@@ -22163,6 +22618,9 @@
       <c r="F107" s="19" t="s">
         <v>17</v>
       </c>
+      <c r="G107" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="108" spans="1:12" ht="110.4">
       <c r="A108" s="19" t="s">
@@ -22180,6 +22638,9 @@
       <c r="F108" s="19" t="s">
         <v>17</v>
       </c>
+      <c r="G108" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="109" spans="1:12" ht="110.4">
       <c r="A109" s="19" t="s">
@@ -22197,6 +22658,9 @@
       <c r="F109" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G109" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="110" spans="1:12" ht="409.6">
       <c r="A110" s="19" t="s">
@@ -22214,6 +22678,9 @@
       <c r="F110" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G110" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="111" spans="1:12" ht="138">
       <c r="A111" s="19" t="s">
@@ -22231,6 +22698,9 @@
       <c r="F111" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G111" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="112" spans="1:12" ht="124.2">
       <c r="A112" s="19" t="s">
@@ -22248,8 +22718,11 @@
       <c r="F112" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G112" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="113" spans="1:6" ht="55.2">
+    <row r="113" spans="1:7" ht="55.2">
       <c r="A113" s="19" t="s">
         <v>226</v>
       </c>
@@ -22266,8 +22739,11 @@
       <c r="F113" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G113" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="114" spans="1:6" ht="55.2">
+    <row r="114" spans="1:7" ht="55.2">
       <c r="A114" s="19" t="s">
         <v>226</v>
       </c>
@@ -22284,8 +22760,11 @@
       <c r="F114" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G114" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="115" spans="1:6" ht="55.2">
+    <row r="115" spans="1:7" ht="55.2">
       <c r="A115" s="19" t="s">
         <v>226</v>
       </c>
@@ -22302,8 +22781,11 @@
       <c r="F115" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G115" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="116" spans="1:6" ht="55.2">
+    <row r="116" spans="1:7" ht="55.2">
       <c r="A116" s="19" t="s">
         <v>226</v>
       </c>
@@ -22320,8 +22802,11 @@
       <c r="F116" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G116" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="117" spans="1:6" ht="55.2">
+    <row r="117" spans="1:7" ht="55.2">
       <c r="A117" s="19" t="s">
         <v>226</v>
       </c>
@@ -22338,8 +22823,11 @@
       <c r="F117" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G117" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="118" spans="1:6" ht="110.4">
+    <row r="118" spans="1:7" ht="110.4">
       <c r="A118" s="19" t="s">
         <v>226</v>
       </c>
@@ -22356,8 +22844,11 @@
       <c r="F118" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G118" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="119" spans="1:6" ht="138">
+    <row r="119" spans="1:7" ht="138">
       <c r="A119" s="19" t="s">
         <v>226</v>
       </c>
@@ -22374,8 +22865,11 @@
       <c r="F119" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G119" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="120" spans="1:6" ht="110.4">
+    <row r="120" spans="1:7" ht="110.4">
       <c r="A120" s="19" t="s">
         <v>226</v>
       </c>
@@ -22392,8 +22886,11 @@
       <c r="F120" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G120" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="121" spans="1:6" ht="55.2">
+    <row r="121" spans="1:7" ht="55.2">
       <c r="A121" s="19" t="s">
         <v>226</v>
       </c>
@@ -22410,8 +22907,11 @@
       <c r="F121" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G121" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="122" spans="1:6" ht="69">
+    <row r="122" spans="1:7" ht="69">
       <c r="A122" s="19" t="s">
         <v>226</v>
       </c>
@@ -22428,8 +22928,11 @@
       <c r="F122" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G122" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="123" spans="1:6" ht="96.6">
+    <row r="123" spans="1:7" ht="96.6">
       <c r="A123" s="19" t="s">
         <v>226</v>
       </c>
@@ -22446,8 +22949,11 @@
       <c r="F123" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G123" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="124" spans="1:6" ht="409.6">
+    <row r="124" spans="1:7" ht="409.6">
       <c r="A124" s="19" t="s">
         <v>226</v>
       </c>
@@ -22464,8 +22970,11 @@
       <c r="F124" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G124" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="125" spans="1:6" ht="138">
+    <row r="125" spans="1:7" ht="138">
       <c r="A125" s="19" t="s">
         <v>226</v>
       </c>
@@ -22482,8 +22991,11 @@
       <c r="F125" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G125" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="126" spans="1:6" ht="124.2">
+    <row r="126" spans="1:7" ht="124.2">
       <c r="A126" s="19" t="s">
         <v>226</v>
       </c>
@@ -22500,8 +23012,11 @@
       <c r="F126" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G126" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="127" spans="1:6" ht="69">
+    <row r="127" spans="1:7" ht="69">
       <c r="A127" s="19" t="s">
         <v>226</v>
       </c>
@@ -22517,8 +23032,11 @@
       <c r="F127" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G127" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="128" spans="1:6" ht="179.4">
+    <row r="128" spans="1:7" ht="179.4">
       <c r="A128" s="19" t="s">
         <v>226</v>
       </c>
@@ -22534,8 +23052,11 @@
       <c r="F128" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G128" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="129" spans="1:6" ht="69">
+    <row r="129" spans="1:7" ht="69">
       <c r="A129" s="19" t="s">
         <v>225</v>
       </c>
@@ -22551,8 +23072,11 @@
       <c r="F129" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G129" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="130" spans="1:6" ht="41.4">
+    <row r="130" spans="1:7" ht="55.2">
       <c r="A130" s="19" t="s">
         <v>225</v>
       </c>
@@ -22568,8 +23092,11 @@
       <c r="F130" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G130" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="131" spans="1:6" ht="69">
+    <row r="131" spans="1:7" ht="69">
       <c r="A131" s="19" t="s">
         <v>225</v>
       </c>
@@ -22585,8 +23112,11 @@
       <c r="F131" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G131" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="132" spans="1:6" ht="27.6">
+    <row r="132" spans="1:7" ht="55.2">
       <c r="A132" s="19" t="s">
         <v>225</v>
       </c>
@@ -22602,8 +23132,11 @@
       <c r="F132" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G132" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="133" spans="1:6" ht="55.2">
+    <row r="133" spans="1:7" ht="55.2">
       <c r="A133" s="19" t="s">
         <v>225</v>
       </c>
@@ -22619,8 +23152,11 @@
       <c r="F133" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G133" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="134" spans="1:6" ht="41.4">
+    <row r="134" spans="1:7" ht="55.2">
       <c r="A134" s="19" t="s">
         <v>225</v>
       </c>
@@ -22636,8 +23172,11 @@
       <c r="F134" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G134" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="135" spans="1:6" ht="27.6">
+    <row r="135" spans="1:7" ht="55.2">
       <c r="A135" s="19" t="s">
         <v>225</v>
       </c>
@@ -22653,8 +23192,11 @@
       <c r="F135" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="G135" s="20" t="s">
+        <v>543</v>
+      </c>
     </row>
-    <row r="136" spans="1:6" ht="41.4">
+    <row r="136" spans="1:7" ht="55.2">
       <c r="A136" s="19" t="s">
         <v>225</v>
       </c>
@@ -22669,6 +23211,219 @@
       </c>
       <c r="F136" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="G136" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="409.6">
+      <c r="A137" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G137" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="179.4">
+      <c r="A138" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G138" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="409.6">
+      <c r="A139" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G139" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="96.6">
+      <c r="A140" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G140" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="409.6">
+      <c r="A141" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G141" s="20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="234.6">
+      <c r="A142" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G142" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="138">
+      <c r="A143" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G143" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="193.2">
+      <c r="A144" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G144" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="82.8">
+      <c r="A145" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G145" s="20" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="179.4">
+      <c r="A146" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G146" s="20" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added All and other features, V N normalization
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B2358B-3E45-47FF-BFF8-D714D76805C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20F664-ED2B-4993-B991-8BDDFA8E4F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="646">
   <si>
     <t>Feature</t>
   </si>
@@ -17382,6 +17382,1154 @@
         <scheme val="minor"/>
       </rPr>
       <t>apparently, evidently, perhaps, possibly, predictably, probably, roughly, maybe, in most cases</t>
+    </r>
+  </si>
+  <si>
+    <t>FPPAll</t>
+  </si>
+  <si>
+    <t>MDPOSSCAll</t>
+  </si>
+  <si>
+    <t>MDPREDAll</t>
+  </si>
+  <si>
+    <t>PASSAll</t>
+  </si>
+  <si>
+    <t>RSTNCAll</t>
+  </si>
+  <si>
+    <t>ThJSTNCAll</t>
+  </si>
+  <si>
+    <t>ThNSTNCAll</t>
+  </si>
+  <si>
+    <t>ThSTNCAll</t>
+  </si>
+  <si>
+    <t>ThVSTNCAll</t>
+  </si>
+  <si>
+    <t>ToJSTNCAll</t>
+  </si>
+  <si>
+    <t>ToSTNCAll</t>
+  </si>
+  <si>
+    <t>ToVSTNCAll</t>
+  </si>
+  <si>
+    <t>WhVSTNCAll</t>
+  </si>
+  <si>
+    <t>Prnouns</t>
+  </si>
+  <si>
+    <t>Adjective semantics</t>
+  </si>
+  <si>
+    <t>Noun semantics</t>
+  </si>
+  <si>
+    <t>Adverb semantics</t>
+  </si>
+  <si>
+    <t>All 1st person pronouns</t>
+  </si>
+  <si>
+    <t>Al modals of possibility</t>
+  </si>
+  <si>
+    <t>All modals of prediction</t>
+  </si>
+  <si>
+    <t>All adverbs related to stance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> passives</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses preceded by stance nouns</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses preceded by stance adjectives, nouns, and verbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses preceded by stance verbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> infinitive clauses preceded by stance adjectives</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> infinitive clauses preceded by stance verbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses preceded by stance verbs</t>
+    </r>
+  </si>
+  <si>
+    <t>JJSTNCAllother</t>
+  </si>
+  <si>
+    <t>All adjectives related to stance in other contexts</t>
+  </si>
+  <si>
+    <t>Any word tagged with FPP1P, FPP1S</t>
+  </si>
+  <si>
+    <t>Any word tagged as MDCA, MDCO, MDMM</t>
+  </si>
+  <si>
+    <t>Any word tagged as MDWS, MDWO, GTO</t>
+  </si>
+  <si>
+    <t>Any word tagged as PASS, PGET</t>
+  </si>
+  <si>
+    <t>Any word tagged as RATT, RNONFACT, RFACT, RLIKELY</t>
+  </si>
+  <si>
+    <t>All that complement clauses preceded by stance adjectives, nouns, and verbs</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThJATT, ThJFCT, ThJLIK, ThJEVL</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThNNFCT, ThNATT, ThNFCT, ThNLIK</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK, ThJATT, ThJFCT, ThJLIK, ThJEVL, ThNNFCT, ThNATT, ThNFCT, ThNLIK</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL, ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL, ToNSTNC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> infinitive clauses preceded by stance adjectives, nouns, and verbs</t>
+    </r>
+  </si>
+  <si>
+    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL</t>
+  </si>
+  <si>
+    <t>Any word tagged as WhVATT, WhVFCT, WhVLIK, WhVCOM</t>
+  </si>
+  <si>
+    <t>Composit tags</t>
+  </si>
+  <si>
+    <t>Biber 1988, adapted by Shakir</t>
+  </si>
+  <si>
+    <t>Shakir</t>
+  </si>
+  <si>
+    <t>Biber 1988, Le Foll, adapted by Shakir</t>
+  </si>
+  <si>
+    <t>Le Foll, adapted by Shakir</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All adjectives as mentioned in ThJATT, ThJEVL, ThJFCT, ThJLIK, JJATDother, JJEPSTother and (1) not having a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or _</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag afterwards (2) not having any other tag.</t>
+    </r>
+  </si>
+  <si>
+    <t>VATTother</t>
+  </si>
+  <si>
+    <t>VCOMMother</t>
+  </si>
+  <si>
+    <t>VFCTother</t>
+  </si>
+  <si>
+    <t>VLIKother</t>
+  </si>
+  <si>
+    <t>mental/attitudinal verbs in other contexts</t>
+  </si>
+  <si>
+    <t>communicaton verbs in other contexts</t>
+  </si>
+  <si>
+    <t>factive verbs in other contexts</t>
+  </si>
+  <si>
+    <t>likelihood verbs in other contexts</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word in the following list tagged as verb and (1) not followed by a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2) not having an additional tag apart from the usual underscore separated tag </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assumes, assumed, assuming, assume, believe, believing, believes, believed, doubting, doubted, doubts, doubt, gathers, gathering, gathered, gather, guessed, guess, guessing, guesses, hypothesising, hypothesised, hypothesise, hypothesises, hypothesizing, hypothesized, hypothesize, hypothesizes, imagine, imagining, imagines, imagined, predict, predicted, predicting, predicts, presupposing, presupposes, presuppose, presupposed, presumes, presuming, presumed, presume, reckon, reckoning, reckoned, reckons, seemed, seems, seem, seeming, speculated, speculate, speculating, speculates, suppose, supposes, supposing, supposed, suspected, suspect, suspects, suspecting, think, thinks, thinking, thought</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word in the following list tagged as verb and (1) not followed by a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2) not having an additional tag apart from the usual underscore separated tag </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concluding, conclude, concluded, concludes, demonstrates, demonstrating, demonstrated, demonstrate, determining, determines, determine, determined, discovered, discovers, discover, discovering, finds, finding, found, find, knows, known, knowing, know, knew, learn, learns, learning, learnt, means, meaning, meant, mean, notifies, notices, notice, noticed, notify, notifying, noticing, notified, observed, observes, observing, observe, proven, prove, proving, proved, proves, realized, realizes, realize, realizing, recognizes, recognize, recognized, recognizing, realised, realises, realise, realising, recognises, recognise, recognised, recognising, remembered, remember, remembers, remembering, sees, seen, saw, seeing, see, showing, shows, shown, showed, show, understand, understands, understanding, understood</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word in the following list tagged as verb and (1) not followed by a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2) not having an additional tag apart from the usual underscore separated tag </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>say, says, saying, said, tell, tells, telling, told, call, calls, calling, called, ask, asks, asking, asked, write, writes, writing, wrote, written, talk, talks, talking, talked, speak, speaks, spoke, spoken, speaking, thank, thanks, thanking, thanked, describe, describing, describes, described, claim, claims, claiming, claimed, offer, offers, offering, offered, admit, admits, admitting, admitted, announce, announces, announcing, announced, answer, answers, answering, answered, argue, argues, arguing, argued, deny, denies, denying, denied, discuss, discusses, discussing, discussed, encourage, encourages, encouraging, encouraged, explain, explains, explaining, explained, express, expresses, expressing, expressed, insist, insists, insisting, insisted, mention, mentions, mentioning, mentioned, offer, offers, offering, offered, propose, proposes, proposing, proposed, quote, quotes, quoting, quoted, reply, replies, replying, replied, shout, shouts, shouting, shouted, sign, signs, signing, signed, sing, sings, singing, sang, sung, state, states, stating, stated, teach, teaches, teaching, taught, warn, warns, warning, warned, accuse, accuses, accusing, accused, acknowledge, acknowledges, acknowledging, acknowledged, address, addresses, addressing, addressed, advise, advises, advising, advised, appeal, appeals, appealing, appealed, assure, assures, assuring, assured, challenge, challenges, challenging, challenged, complain, complains, complaining, complained, consult, consults, consulting, consulted, convince, convinces, convincing, convinced, declare, declares, declaring, declared, demand, demands, demanding, demanded, emphasize, emphasizes, emphasizing, emphasized, emphasise, emphasises, emphasising, emphasised, excuse, excuses, excusing, excused, inform, informs, informing, informed, invite, invites, inviting, invited, persuade, persuades, persuading, persuaded, phone, phones, phoning, phoned, pray, prays, praying, prayed, promise, promises, promising, promised, question, questions, questioning, questioned, recommend, recommends, recommending, recommended, remark, remarks, remarking, remarked, respond, responds, responding, responded, specify, specifies, specifying, specified, swear, swears, swearing, swore, sworn, threaten, threatens, threatening, threatened, urge, urges, urging, urged, welcome, welcomes, welcoming, welcomed, whisper, whispers, whispering, whispered, suggest, suggests, suggesting, suggested, plead, pleads, pleaded, pleading, agree, agrees, agreed, agreeing, assert, asserts, asserting, asserted, beg, begs, begging, begged, confide, confides, confiding, confided, command, commands, commanding, commanded, disagree, disagreeing, disagrees, disagreed, object, objects, objected, objects, pledge, pledges, pledging, pledged, report, reports, reported, reporting, testify, testifies, testified, testifying, vow, vows, vowing, vowed, mean, means, meaning, meant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word in the following list tagged as verb and (1) not followed by a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2) not having an additional tag apart from the usual underscore separated tag </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>agreeing, agreed, agree, agrees, anticipates, anticipated, anticipate, anticipating, complain, complained, complaining, complains, conceded, concede, concedes, conceding, ensure, expecting, expect, expects, expected, fears, feared, fear, fearing, feel, feels, feeling, felt, forgetting, forgets, forgotten, forgot, forget, hoped, hope, hopes, hoping, minding, minded, minds, mind, preferred, prefer, preferring, prefers, pretending, pretend, pretended, pretends, requiring, required, requires, require, wishes, wished, wish, wishing, worry, worrying, worries, worried</t>
+    </r>
+  </si>
+  <si>
+    <t>INother</t>
+  </si>
+  <si>
+    <t>JJATother</t>
+  </si>
+  <si>
+    <t>JJPRother</t>
+  </si>
+  <si>
+    <t>NNother</t>
+  </si>
+  <si>
+    <t>RBother</t>
+  </si>
+  <si>
+    <t>THRCother</t>
+  </si>
+  <si>
+    <t>THSCother</t>
+  </si>
+  <si>
+    <t>WHSCother</t>
+  </si>
+  <si>
+    <t>Prepositions having no additional tag</t>
+  </si>
+  <si>
+    <t>Attributive adjectives having no additional tag</t>
+  </si>
+  <si>
+    <t>Predicative adjectives having no additional tag</t>
+  </si>
+  <si>
+    <t>Nouns having no additional tag</t>
+  </si>
+  <si>
+    <t>Adverbs having no additional tag</t>
+  </si>
+  <si>
+    <t>Adverbs</t>
+  </si>
+  <si>
+    <t>Discourse organization</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_JJAT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_JJPR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_NN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_RB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THRC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative clauses not preceded by a stance noun</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses not preceded by a stance adjective or verb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses not preceded by a stance verb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
     </r>
   </si>
 </sst>
@@ -17678,7 +18826,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -17814,6 +18962,14 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -18364,10 +19520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM150"/>
+  <dimension ref="A1:AMM177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4"/>
@@ -22654,7 +23810,7 @@
     </row>
     <row r="101" spans="1:12" ht="110.4">
       <c r="A101" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B101" s="29" t="s">
         <v>402</v>
@@ -22675,7 +23831,7 @@
     </row>
     <row r="102" spans="1:12" ht="110.4">
       <c r="A102" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B102" s="29" t="s">
         <v>408</v>
@@ -22696,7 +23852,7 @@
     </row>
     <row r="103" spans="1:12" ht="110.4">
       <c r="A103" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B103" s="29" t="s">
         <v>409</v>
@@ -22716,7 +23872,7 @@
     </row>
     <row r="104" spans="1:12" ht="110.4">
       <c r="A104" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B104" s="29" t="s">
         <v>410</v>
@@ -22736,7 +23892,7 @@
     </row>
     <row r="105" spans="1:12" ht="110.4">
       <c r="A105" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B105" s="29" t="s">
         <v>422</v>
@@ -22756,7 +23912,7 @@
     </row>
     <row r="106" spans="1:12" ht="110.4">
       <c r="A106" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B106" s="29" t="s">
         <v>423</v>
@@ -22776,7 +23932,7 @@
     </row>
     <row r="107" spans="1:12" ht="110.4">
       <c r="A107" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B107" s="29" t="s">
         <v>424</v>
@@ -22796,7 +23952,7 @@
     </row>
     <row r="108" spans="1:12" ht="110.4">
       <c r="A108" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B108" s="29" t="s">
         <v>425</v>
@@ -22816,7 +23972,7 @@
     </row>
     <row r="109" spans="1:12" ht="110.4">
       <c r="A109" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B109" s="29" t="s">
         <v>429</v>
@@ -22836,7 +23992,7 @@
     </row>
     <row r="110" spans="1:12" ht="409.6">
       <c r="A110" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B110" s="29" t="s">
         <v>430</v>
@@ -22856,7 +24012,7 @@
     </row>
     <row r="111" spans="1:12" ht="138">
       <c r="A111" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B111" s="29" t="s">
         <v>431</v>
@@ -22876,7 +24032,7 @@
     </row>
     <row r="112" spans="1:12" ht="124.2">
       <c r="A112" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B112" s="29" t="s">
         <v>432</v>
@@ -22894,85 +24050,79 @@
         <v>543</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="55.2">
-      <c r="A113" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1" t="s">
-        <v>478</v>
+    <row r="113" spans="1:7" ht="110.4">
+      <c r="A113" s="19"/>
+      <c r="B113" s="41" t="s">
+        <v>612</v>
+      </c>
+      <c r="C113" s="40" t="s">
+        <v>608</v>
+      </c>
+      <c r="E113" s="41" t="s">
+        <v>619</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G113" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="55.2">
+    <row r="114" spans="1:7" ht="409.6">
       <c r="A114" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1" t="s">
-        <v>479</v>
+        <v>93</v>
+      </c>
+      <c r="B114" s="41" t="s">
+        <v>613</v>
+      </c>
+      <c r="C114" s="40" t="s">
+        <v>609</v>
+      </c>
+      <c r="E114" s="41" t="s">
+        <v>618</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G114" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="55.2">
+    <row r="115" spans="1:7" ht="151.80000000000001">
       <c r="A115" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1" t="s">
-        <v>480</v>
+        <v>93</v>
+      </c>
+      <c r="B115" s="41" t="s">
+        <v>614</v>
+      </c>
+      <c r="C115" s="40" t="s">
+        <v>610</v>
+      </c>
+      <c r="E115" s="41" t="s">
+        <v>617</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G115" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="55.2">
+    <row r="116" spans="1:7" ht="138">
       <c r="A116" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>454</v>
+        <v>93</v>
+      </c>
+      <c r="B116" s="41" t="s">
+        <v>615</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>444</v>
-      </c>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1" t="s">
-        <v>481</v>
+        <v>611</v>
+      </c>
+      <c r="E116" s="41" t="s">
+        <v>616</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G116" s="20" t="s">
         <v>543</v>
@@ -22980,17 +24130,17 @@
     </row>
     <row r="117" spans="1:7" ht="55.2">
       <c r="A117" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>8</v>
@@ -22999,64 +24149,64 @@
         <v>543</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="110.4">
+    <row r="118" spans="1:7" ht="55.2">
       <c r="A118" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1" t="s">
-        <v>461</v>
+        <v>479</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G118" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="138">
+    <row r="119" spans="1:7" ht="55.2">
       <c r="A119" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G119" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="110.4">
+    <row r="120" spans="1:7" ht="55.2">
       <c r="A120" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1" t="s">
-        <v>463</v>
+        <v>481</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G120" s="20" t="s">
         <v>543</v>
@@ -23064,38 +24214,38 @@
     </row>
     <row r="121" spans="1:7" ht="55.2">
       <c r="A121" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G121" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="69">
+    <row r="122" spans="1:7" ht="110.4">
       <c r="A122" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>32</v>
@@ -23104,19 +24254,19 @@
         <v>543</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="96.6">
+    <row r="123" spans="1:7" ht="138">
       <c r="A123" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="C123" s="39" t="s">
-        <v>466</v>
+        <v>457</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>448</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>32</v>
@@ -23125,19 +24275,19 @@
         <v>543</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="409.6">
+    <row r="124" spans="1:7" ht="110.4">
       <c r="A124" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="C124" s="39" t="s">
-        <v>467</v>
+        <v>458</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>449</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>32</v>
@@ -23146,19 +24296,19 @@
         <v>543</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="138">
+    <row r="125" spans="1:7" ht="55.2">
       <c r="A125" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="C125" s="39" t="s">
-        <v>468</v>
+        <v>459</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>450</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>32</v>
@@ -23167,19 +24317,19 @@
         <v>543</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="124.2">
+    <row r="126" spans="1:7" ht="69">
       <c r="A126" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C126" s="39" t="s">
-        <v>469</v>
+        <v>460</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>451</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>32</v>
@@ -23188,81 +24338,85 @@
         <v>543</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="69">
+    <row r="127" spans="1:7" ht="96.6">
       <c r="A127" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>446</v>
-      </c>
+        <v>474</v>
+      </c>
+      <c r="C127" s="39" t="s">
+        <v>466</v>
+      </c>
+      <c r="D127" s="1"/>
       <c r="E127" s="1" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G127" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="179.4">
+    <row r="128" spans="1:7" ht="409.6">
       <c r="A128" s="19" t="s">
-        <v>226</v>
+        <v>67</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>485</v>
-      </c>
+        <v>475</v>
+      </c>
+      <c r="C128" s="39" t="s">
+        <v>467</v>
+      </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G128" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="69">
+    <row r="129" spans="1:7" ht="138">
       <c r="A129" s="19" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>488</v>
-      </c>
+        <v>476</v>
+      </c>
+      <c r="C129" s="39" t="s">
+        <v>468</v>
+      </c>
+      <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
-        <v>510</v>
+        <v>472</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G129" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="55.2">
+    <row r="130" spans="1:7" ht="124.2">
       <c r="A130" s="19" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>489</v>
-      </c>
+        <v>477</v>
+      </c>
+      <c r="C130" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="D130" s="1"/>
       <c r="E130" s="1" t="s">
-        <v>506</v>
+        <v>473</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G130" s="20" t="s">
         <v>543</v>
@@ -23270,16 +24424,16 @@
     </row>
     <row r="131" spans="1:7" ht="69">
       <c r="A131" s="19" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>491</v>
+        <v>446</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>511</v>
+        <v>484</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>17</v>
@@ -23288,18 +24442,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="55.2">
+    <row r="132" spans="1:7" ht="179.4">
       <c r="A132" s="19" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>17</v>
@@ -23308,18 +24462,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="55.2">
+    <row r="133" spans="1:7" ht="69">
       <c r="A133" s="19" t="s">
-        <v>225</v>
+        <v>571</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>17</v>
@@ -23330,16 +24484,16 @@
     </row>
     <row r="134" spans="1:7" ht="55.2">
       <c r="A134" s="19" t="s">
-        <v>225</v>
+        <v>571</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>17</v>
@@ -23348,18 +24502,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="55.2">
+    <row r="135" spans="1:7" ht="69">
       <c r="A135" s="19" t="s">
-        <v>225</v>
+        <v>571</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>17</v>
@@ -23370,16 +24524,16 @@
     </row>
     <row r="136" spans="1:7" ht="55.2">
       <c r="A136" s="19" t="s">
-        <v>225</v>
+        <v>571</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>17</v>
@@ -23388,19 +24542,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="409.6">
-      <c r="A137" s="1" t="s">
-        <v>17</v>
+    <row r="137" spans="1:7" ht="55.2">
+      <c r="A137" s="19" t="s">
+        <v>571</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>529</v>
+        <v>501</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="D137" s="1"/>
+        <v>493</v>
+      </c>
       <c r="E137" s="1" t="s">
-        <v>533</v>
+        <v>508</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>17</v>
@@ -23409,19 +24562,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="179.4">
-      <c r="A138" s="1" t="s">
-        <v>17</v>
+    <row r="138" spans="1:7" ht="55.2">
+      <c r="A138" s="19" t="s">
+        <v>571</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="D138" s="1"/>
+        <v>494</v>
+      </c>
       <c r="E138" s="1" t="s">
-        <v>534</v>
+        <v>497</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>17</v>
@@ -23430,19 +24582,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="409.6">
-      <c r="A139" s="1" t="s">
-        <v>17</v>
+    <row r="139" spans="1:7" ht="55.2">
+      <c r="A139" s="19" t="s">
+        <v>571</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="D139" s="1"/>
+        <v>495</v>
+      </c>
       <c r="E139" s="1" t="s">
-        <v>535</v>
+        <v>505</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>17</v>
@@ -23451,19 +24602,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="96.6">
-      <c r="A140" s="1" t="s">
-        <v>17</v>
+    <row r="140" spans="1:7" ht="55.2">
+      <c r="A140" s="19" t="s">
+        <v>571</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>517</v>
-      </c>
-      <c r="D140" s="1"/>
+        <v>496</v>
+      </c>
       <c r="E140" s="1" t="s">
-        <v>532</v>
+        <v>509</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>17</v>
@@ -23474,38 +24624,38 @@
     </row>
     <row r="141" spans="1:7" ht="409.6">
       <c r="A141" s="1" t="s">
-        <v>17</v>
+        <v>572</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G141" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="234.6">
+    <row r="142" spans="1:7" ht="179.4">
       <c r="A142" s="1" t="s">
-        <v>17</v>
+        <v>572</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>17</v>
@@ -23514,19 +24664,19 @@
         <v>543</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="138">
+    <row r="143" spans="1:7" ht="409.6">
       <c r="A143" s="1" t="s">
-        <v>17</v>
+        <v>572</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>17</v>
@@ -23535,19 +24685,19 @@
         <v>543</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="193.2">
+    <row r="144" spans="1:7" ht="96.6">
       <c r="A144" s="1" t="s">
-        <v>17</v>
+        <v>572</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>17</v>
@@ -23556,40 +24706,40 @@
         <v>543</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="82.8">
+    <row r="145" spans="1:7" ht="409.6">
       <c r="A145" s="1" t="s">
-        <v>17</v>
+        <v>572</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G145" s="20" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="179.4">
+    <row r="146" spans="1:7" ht="234.6">
       <c r="A146" s="1" t="s">
-        <v>17</v>
+        <v>572</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>17</v>
@@ -23598,89 +24748,618 @@
         <v>543</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="55.2">
+    <row r="147" spans="1:7" ht="138">
       <c r="A147" s="1" t="s">
-        <v>223</v>
+        <v>572</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C147" s="39" t="s">
-        <v>545</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="D147" s="1"/>
       <c r="E147" s="1" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G147" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="55.2">
+    <row r="148" spans="1:7" ht="193.2">
       <c r="A148" s="1" t="s">
-        <v>223</v>
+        <v>572</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="C148" s="39" t="s">
-        <v>547</v>
-      </c>
+        <v>531</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="D148" s="1"/>
       <c r="E148" s="1" t="s">
-        <v>555</v>
+        <v>539</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G148" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="55.2">
+    <row r="149" spans="1:7" ht="82.8">
       <c r="A149" s="1" t="s">
-        <v>223</v>
+        <v>572</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="C149" s="39" t="s">
-        <v>549</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="D149" s="1"/>
       <c r="E149" s="1" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G149" s="20" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="55.2">
+    <row r="150" spans="1:7" ht="179.4">
       <c r="A150" s="1" t="s">
-        <v>223</v>
+        <v>572</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="C150" s="39" t="s">
-        <v>551</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G150" s="20" t="s">
         <v>543</v>
       </c>
     </row>
+    <row r="151" spans="1:7" ht="55.2">
+      <c r="A151" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C151" s="39" t="s">
+        <v>545</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G151" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="55.2">
+      <c r="A152" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C152" s="39" t="s">
+        <v>547</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G152" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="55.2">
+      <c r="A153" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C153" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G153" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="55.2">
+      <c r="A154" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G154" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="D155" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="55.2">
+      <c r="A156" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="E156" s="38" t="s">
+        <v>587</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G156" s="6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="82.8">
+      <c r="A157" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>585</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G157" s="20" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="69">
+      <c r="A158" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="E158" s="38" t="s">
+        <v>588</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="69">
+      <c r="A159" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G159" s="6" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="41.4">
+      <c r="A160" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G160" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="55.2">
+      <c r="A161" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G161" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="110.4">
+      <c r="A162" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G162" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="82.8">
+      <c r="A163" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G163" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="110.4">
+      <c r="A164" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G164" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="69">
+      <c r="A165" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="E165" s="38" t="s">
+        <v>596</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G165" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="82.8">
+      <c r="A166" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="E166" s="38" t="s">
+        <v>597</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G166" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="110.4">
+      <c r="A167" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G167" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="69">
+      <c r="A168" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="E168" s="38" t="s">
+        <v>600</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G168" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="69">
+      <c r="A169" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C169" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="E169" s="38" t="s">
+        <v>601</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G169" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="55.2">
+      <c r="A170" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="E170" s="38" t="s">
+        <v>635</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G170" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="69">
+      <c r="A171" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="E171" s="38" t="s">
+        <v>636</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G171" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="69">
+      <c r="A172" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="E172" s="38" t="s">
+        <v>637</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G172" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="55.2">
+      <c r="A173" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E173" s="38" t="s">
+        <v>638</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G173" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="55.2">
+      <c r="A174" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E174" s="38" t="s">
+        <v>639</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G174" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="82.8">
+      <c r="A175" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E175" s="38" t="s">
+        <v>640</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G175" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="96.6">
+      <c r="A176" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="E176" s="38" t="s">
+        <v>644</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="82.8">
+      <c r="A177" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="E177" s="38" t="s">
+        <v>645</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G177" s="6" t="s">
+        <v>606</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C129:D142">
-    <sortCondition ref="C129:C142"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C133:D146">
+    <sortCondition ref="C133:C146"/>
   </sortState>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.35" bottom="0.35" header="0" footer="0.3"/>

</xml_diff>

<commit_message>
added PRPother and MDother description
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D3BD9E-384E-4DCA-A15F-E3056341A74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18CD4CE-4A60-4872-B76F-04A3CC0D47AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="648">
   <si>
     <t>Feature</t>
   </si>
@@ -18474,6 +18474,68 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <t>Remaining modal verbs</t>
+  </si>
+  <si>
+    <t>MDother</t>
+  </si>
+  <si>
+    <t>Any word tagged as MD by Stanford tagger and remains as it is after MFTE tagging is completed.</t>
+  </si>
+  <si>
+    <t>PRPother </t>
+  </si>
+  <si>
+    <t>Other personal pronouns</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as PRPS or PRP by Stanford tagger. For example </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (the dialectal fom of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>your</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) is tagged as PRPS.</t>
     </r>
   </si>
 </sst>
@@ -19464,10 +19526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM176"/>
+  <dimension ref="A1:AMM178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157:XFD157"/>
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
@@ -24881,38 +24943,33 @@
         <v>601</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="64.5">
+    <row r="157" spans="1:7" ht="39">
       <c r="A157" s="1" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>575</v>
+        <v>646</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="E157" s="38" t="s">
-        <v>586</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G157" s="6" t="s">
-        <v>602</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="G157" s="6"/>
     </row>
     <row r="158" spans="1:7" ht="64.5">
       <c r="A158" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>559</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>587</v>
+        <v>558</v>
+      </c>
+      <c r="E158" s="38" t="s">
+        <v>586</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>32</v>
@@ -24921,81 +24978,81 @@
         <v>602</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="39">
-      <c r="A159" s="19" t="s">
-        <v>230</v>
+    <row r="159" spans="1:7" ht="64.5">
+      <c r="A159" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G159" s="6" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="39">
+      <c r="A160" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G160" s="6" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="51">
-      <c r="A160" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>561</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="F160" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G160" s="20" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" ht="102.75">
-      <c r="A161" s="1" t="s">
-        <v>67</v>
+    <row r="161" spans="1:7" ht="39">
+      <c r="A161" s="19" t="s">
+        <v>230</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G161" s="20" t="s">
-        <v>543</v>
+      <c r="G161" s="6" t="s">
+        <v>603</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="64.5">
+    <row r="162" spans="1:7" ht="51">
       <c r="A162" s="1" t="s">
-        <v>67</v>
+        <v>573</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G162" s="20" t="s">
         <v>543</v>
@@ -25006,16 +25063,16 @@
         <v>67</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G163" s="20" t="s">
         <v>543</v>
@@ -25026,13 +25083,13 @@
         <v>67</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>565</v>
-      </c>
-      <c r="E164" s="38" t="s">
-        <v>594</v>
+        <v>563</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>592</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>32</v>
@@ -25041,18 +25098,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="77.25">
+    <row r="165" spans="1:7" ht="102.75">
       <c r="A165" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>566</v>
-      </c>
-      <c r="E165" s="38" t="s">
-        <v>595</v>
+        <v>564</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>593</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>8</v>
@@ -25061,201 +25118,201 @@
         <v>543</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="102.75">
+    <row r="166" spans="1:7" ht="64.5">
       <c r="A166" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>597</v>
+        <v>581</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>567</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>596</v>
+        <v>565</v>
+      </c>
+      <c r="E166" s="38" t="s">
+        <v>594</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G166" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="64.5">
+    <row r="167" spans="1:7" ht="77.25">
       <c r="A167" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E167" s="38" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G167" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="64.5">
+    <row r="168" spans="1:7" ht="102.75">
       <c r="A168" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>584</v>
+        <v>597</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>569</v>
-      </c>
-      <c r="E168" s="38" t="s">
-        <v>599</v>
+        <v>567</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>596</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G168" s="20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="51.75">
+    <row r="169" spans="1:7" ht="64.5">
       <c r="A169" s="1" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>624</v>
+        <v>583</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>616</v>
+        <v>568</v>
       </c>
       <c r="E169" s="38" t="s">
-        <v>631</v>
+        <v>598</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G169" s="6" t="s">
-        <v>603</v>
+        <v>32</v>
+      </c>
+      <c r="G169" s="20" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="64.5">
       <c r="A170" s="1" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>625</v>
+        <v>584</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>617</v>
+        <v>569</v>
       </c>
       <c r="E170" s="38" t="s">
-        <v>632</v>
+        <v>599</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G170" s="6" t="s">
-        <v>603</v>
+        <v>32</v>
+      </c>
+      <c r="G170" s="20" t="s">
+        <v>543</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="64.5">
+    <row r="171" spans="1:7" ht="51.75">
       <c r="A171" s="1" t="s">
-        <v>225</v>
+        <v>119</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E171" s="38" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G171" s="6" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="51.75">
+    <row r="172" spans="1:7" ht="64.5">
       <c r="A172" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="E172" s="38" t="s">
+        <v>632</v>
+      </c>
+      <c r="F172" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E172" s="38" t="s">
-        <v>634</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G172" s="6" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="51.75">
+    <row r="173" spans="1:7" ht="64.5">
       <c r="A173" s="1" t="s">
-        <v>629</v>
+        <v>225</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E173" s="38" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G173" s="6" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="64.5">
+    <row r="174" spans="1:7" ht="51.75">
       <c r="A174" s="1" t="s">
-        <v>630</v>
+        <v>17</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E174" s="38" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G174" s="6" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="90">
+    <row r="175" spans="1:7" ht="51.75">
       <c r="A175" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E175" s="38" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="G175" s="6" t="s">
         <v>603</v>
@@ -25266,18 +25323,58 @@
         <v>630</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E176" s="38" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G176" s="6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="90">
+      <c r="A177" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="E177" s="38" t="s">
+        <v>640</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G177" s="6" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="64.5">
+      <c r="A178" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E178" s="38" t="s">
+        <v>641</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G178" s="6" t="s">
         <v>603</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated composite tag descriptions
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F867EBD-376C-D441-9C19-1065B624040E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94A0C16-E850-4799-838B-F8B7780FFA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -17033,39 +17033,9 @@
     </r>
   </si>
   <si>
-    <t>Any word tagged as MDCA, MDCO, MDMM</t>
-  </si>
-  <si>
-    <t>Any word tagged as MDWS, MDWO, GTO</t>
-  </si>
-  <si>
-    <t>Any word tagged as PASS, PGET</t>
-  </si>
-  <si>
-    <t>Any word tagged as RATT, RNONFACT, RFACT, RLIKELY</t>
-  </si>
-  <si>
     <t>All that complement clauses preceded by stance adjectives, nouns, and verbs</t>
   </si>
   <si>
-    <t>Any word tagged as ThJATT, ThJFCT, ThJLIK, ThJEVL</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThNNFCT, ThNATT, ThNFCT, ThNLIK</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK, ThJATT, ThJFCT, ThJLIK, ThJEVL, ThNNFCT, ThNATT, ThNFCT, ThNLIK</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK</t>
-  </si>
-  <si>
-    <t>Any word tagged as ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL</t>
-  </si>
-  <si>
-    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL, ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL, ToNSTNC</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">All </t>
     </r>
@@ -17092,12 +17062,6 @@
     </r>
   </si>
   <si>
-    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL</t>
-  </si>
-  <si>
-    <t>Any word tagged as WhVATT, WhVFCT, WhVLIK, WhVCOM</t>
-  </si>
-  <si>
     <t>Biber 1988, adapted by Shakir</t>
   </si>
   <si>
@@ -17471,6 +17435,1026 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative clauses not preceded by a stance noun</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses not preceded by a stance adjective or verb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clauses not preceded by a stance verb</t>
+    </r>
+  </si>
+  <si>
+    <t>Shakir</t>
+  </si>
+  <si>
+    <t>Composite tags</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>afraid, amazed, (un)aware, concerned, disappointed, encouraged, glad, happy, hopeful, pleased, shocked, surprised, worried</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doubtful, likely, possible, probable, unlikely</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apparent, certain, clear, confident, convinced, correct, evident, false, impossible, inevitable, obvious, positive, right, sure, true, well-known.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>grounds, ground, hope, hopes, reason, reasons, view, views, thought, thoughts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertion, assertions, conclusion, conclusions, conviction, convictions, discovery, discoveries, doubt, doubts, fact, facts, knowledge, knowledges, observation, observations, principle, principles, realization, realizations, result, results, statement, statements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assumption, assumptions, belief, beliefs, claim, claims, contention, contentions, feeling, feelings, hypothesis, hypotheses, idea, ideas, implication, implications, impression, impressions, notion, notions, opinion, opinions, possibility, possibilities, presumption, presumptions, suggestion, suggestions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>comment, comments, news, news, proposal, proposals, proposition, propositions, remark, remarks, report, reports, requirement, requirements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as verb: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>agreeing, agreed, agree, agrees, anticipates, anticipated, anticipate, anticipating, complain, complained, complaining, complains, conceded, concede, concedes, conceding, ensure, expecting, expect, expects, expected, fears, feared, fear, fearing, feel, feels, feeling, felt, forgetting, forgets, forgotten, forgot, forget, hoped, hope, hopes, hoping, minding, minded, minds, mind, preferred, prefer, preferring, prefers, pretending, pretend, pretended, pretends, requiring, required, requires, require, wishes, wished, wish, wishing, worry, worrying, worries, worried</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word in the following list tagged as verb and (1) not followed by a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tag or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2) not having an additional tag apart from the usual underscore separated tag </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_TAG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>concluding, conclude, concluded, concludes, demonstrates, demonstrating, demonstrated, demonstrate, determining, determines, determine, determined, discovered, discovers, discover, discovering, finds, finding, found, find, knows, known, knowing, know, knew, learn, learns, learning, learnt, means, meaning, meant, mean, notifies, notices, notice, noticed, notify, notifying, noticing, notified, observed, observes, observing, observe, proven, prove, proving, proved, proves, realized, realizes, realize, realizing, recognizes, recognize, recognized, recognizing, realised, realises, realise, realising, recognises, recognise, recognised, recognising, remembered, remember, remembers, remembering, sees, seen, saw, seeing, see, showing, shows, shown, showed, show, understand, understands, understanding, understood</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">subordinate clauses (other than relatives) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>preceded by likelihood verbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">subordinate clauses (other than relatives)  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>preceded by factive verbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">that </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">subordinate clauses (other than relatives) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>preceded by attitutidinal verbs</t>
+    </r>
+  </si>
+  <si>
+    <t>All modals of possibility</t>
+  </si>
+  <si>
+    <t>Proper nouns</t>
+  </si>
+  <si>
+    <t>NNP</t>
+  </si>
+  <si>
+    <t>Nouns tagged as NNP and NNPS by Stanford Tagger.</t>
+  </si>
+  <si>
+    <t>Le Foll and Shakir</t>
+  </si>
+  <si>
+    <t>Extended features added in the MFTE python version 1.0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>That</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>afraid, amazed, (un)aware, concerned, disappointed, encouraged, glad, happy, hopeful, pleased, shocked, surprised, worried</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>PP1S</t>
+  </si>
+  <si>
+    <t>PP1P</t>
+  </si>
+  <si>
+    <t>PP2</t>
+  </si>
+  <si>
+    <t>PP3S</t>
+  </si>
+  <si>
+    <t>PP3P</t>
+  </si>
+  <si>
+    <t>PP1</t>
+  </si>
+  <si>
+    <t>PP3</t>
+  </si>
+  <si>
+    <t>All 1st person referents</t>
+  </si>
+  <si>
+    <t>All 3rd person referents</t>
+  </si>
+  <si>
+    <t>Any personal pronoun not included in the other categories</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This tag consists of the remaining personal pronouns not yet tagged as either first (PR1), second (PR2) or third (PR3) person pronouns. In practice, this should only leave </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">one </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and any misspelt, historical or dialectal forms not captured by the other categories.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ppother</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Following Biber (1988), all occurrences of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you, your, yourself, yourselves</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Following Nini (2014: 18), also includes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">thy, thee </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>thyself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. In addition, the forms</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> u, ur, ye, y'all, ya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>thine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the nominal possessive pronoun </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> were also added.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Assigned to all occurrences of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>as long as,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unless,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lest, in that case, otherwise, even when </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>whether.</t>
+    </r>
+  </si>
+  <si>
+    <t>Any word tagged with PP1P, PP1S. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged with PP3P, PP3S. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as MDCA, MDCO, MDMM. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as MDWS, MDWO, GTO. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as PASS, PGET. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as RATT, RNONFACT, RFACT, RLIKELY. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThJATT, ThJFCT, ThJLIK, ThJEVL. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThNNFCT, ThNATT, ThNFCT, ThNLIK. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK, ThJATT, ThJFCT, ThJLIK, ThJEVL, ThNNFCT, ThNATT, ThNFCT, ThNLIK. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL, ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL, ToNSTNC. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <t>Any word tagged as WhVATT, WhVFCT, WhVLIK, WhVCOM. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Any word tagged as </t>
     </r>
     <r>
@@ -17482,6 +18466,32 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>_NN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of nouns. If semantic classes of nouns are included, this feature should be used instead of the original NN.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>_IN</t>
     </r>
     <r>
@@ -17492,7 +18502,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with stance related prepositions. If stance prepositions are included, this feature should be used instead of the original IN.</t>
     </r>
   </si>
   <si>
@@ -17518,7 +18528,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of adjectives. If semantic classes of adjectives (stance related adjectives) are included, this feature should be used instead of the original JJAT.</t>
     </r>
   </si>
   <si>
@@ -17544,7 +18554,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of adjectives. If semantic classes of adjectives (stance related adjectives) are included, this feature should be used instead of the original JJAT.</t>
     </r>
   </si>
   <si>
@@ -17560,17 +18570,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>_NN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with WHSC followed by semantic classes of verbs. If those features are included, this feature should be used instead of the original WHSC.</t>
     </r>
   </si>
   <si>
@@ -17586,6 +18596,58 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>_THRC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with THRC followed by semantic classes of nouns et cetera. If those features are included, this feature should be used instead of the original THRC.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with THSC followed by semantic classes of verbs and adjectives et cetera. If those features are included, this feature should be used instead of the original THSC.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>_RB</t>
     </r>
     <r>
@@ -17596,1069 +18658,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_THRC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>that</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> relative clauses not preceded by a stance noun</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>that</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clauses not preceded by a stance adjective or verb</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clauses not preceded by a stance verb</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_THSC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_WHSC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
-    </r>
-  </si>
-  <si>
-    <t>Shakir</t>
-  </si>
-  <si>
-    <t>Composite tags</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>afraid, amazed, (un)aware, concerned, disappointed, encouraged, glad, happy, hopeful, pleased, shocked, surprised, worried</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>doubtful, likely, possible, probable, unlikely</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>apparent, certain, clear, confident, convinced, correct, evident, false, impossible, inevitable, obvious, positive, right, sure, true, well-known.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>grounds, ground, hope, hopes, reason, reasons, view, views, thought, thoughts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>assertion, assertions, conclusion, conclusions, conviction, convictions, discovery, discoveries, doubt, doubts, fact, facts, knowledge, knowledges, observation, observations, principle, principles, realization, realizations, result, results, statement, statements</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>assumption, assumptions, belief, beliefs, claim, claims, contention, contentions, feeling, feelings, hypothesis, hypotheses, idea, ideas, implication, implications, impression, impressions, notion, notions, opinion, opinions, possibility, possibilities, presumption, presumptions, suggestion, suggestions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> relative clause (THRC) tag preceded by any of the following words tagged as noun: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>comment, comments, news, news, proposal, proposals, proposition, propositions, remark, remarks, report, reports, requirement, requirements.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as verb: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>agreeing, agreed, agree, agrees, anticipates, anticipated, anticipate, anticipating, complain, complained, complaining, complains, conceded, concede, concedes, conceding, ensure, expecting, expect, expects, expected, fears, feared, fear, fearing, feel, feels, feeling, felt, forgetting, forgets, forgotten, forgot, forget, hoped, hope, hopes, hoping, minding, minded, minds, mind, preferred, prefer, preferring, prefers, pretending, pretend, pretended, pretends, requiring, required, requires, require, wishes, wished, wish, wishing, worry, worrying, worries, worried</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word in the following list tagged as verb and (1) not followed by a </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_WHSC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_THSC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tag or </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (2) not having an additional tag apart from the usual underscore separated tag </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_TAG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>concluding, conclude, concluded, concludes, demonstrates, demonstrating, demonstrated, demonstrate, determining, determines, determine, determined, discovered, discovers, discover, discovering, finds, finding, found, find, knows, known, knowing, know, knew, learn, learns, learning, learnt, means, meaning, meant, mean, notifies, notices, notice, noticed, notify, notifying, noticing, notified, observed, observes, observing, observe, proven, prove, proving, proved, proves, realized, realizes, realize, realizing, recognizes, recognize, recognized, recognizing, realised, realises, realise, realising, recognises, recognise, recognised, recognising, remembered, remember, remembers, remembering, sees, seen, saw, seeing, see, showing, shows, shown, showed, show, understand, understands, understanding, understood</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">that </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">subordinate clauses (other than relatives) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>preceded by likelihood verbs</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">that </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">subordinate clauses (other than relatives)  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>preceded by factive verbs</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">that </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">subordinate clauses (other than relatives) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>preceded by attitutidinal verbs</t>
-    </r>
-  </si>
-  <si>
-    <t>All modals of possibility</t>
-  </si>
-  <si>
-    <t>Proper nouns</t>
-  </si>
-  <si>
-    <t>NNP</t>
-  </si>
-  <si>
-    <t>Nouns tagged as NNP and NNPS by Stanford Tagger.</t>
-  </si>
-  <si>
-    <t>Le Foll and Shakir</t>
-  </si>
-  <si>
-    <t>Extended features added in the MFTE python version 1.0</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>That</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> complement clause (THSC) tag preceded by any of the following words tagged as adjective: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>afraid, amazed, (un)aware, concerned, disappointed, encouraged, glad, happy, hopeful, pleased, shocked, surprised, worried</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>PP1S</t>
-  </si>
-  <si>
-    <t>PP1P</t>
-  </si>
-  <si>
-    <t>PP2</t>
-  </si>
-  <si>
-    <t>PP3S</t>
-  </si>
-  <si>
-    <t>PP3P</t>
-  </si>
-  <si>
-    <t>PP1</t>
-  </si>
-  <si>
-    <t>Any word tagged with PP1P, PP1S</t>
-  </si>
-  <si>
-    <t>PP3</t>
-  </si>
-  <si>
-    <t>Any word tagged with PP3P, PP3S</t>
-  </si>
-  <si>
-    <t>All 1st person referents</t>
-  </si>
-  <si>
-    <t>All 3rd person referents</t>
-  </si>
-  <si>
-    <t>Any personal pronoun not included in the other categories</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This tag consists of the remaining personal pronouns not yet tagged as either first (PR1), second (PR2) or third (PR3) person pronouns. In practice, this should only leave </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">one </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and any misspelt, historical or dialectal forms not captured by the other categories.</t>
-    </r>
-  </si>
-  <si>
-    <t>Ppother</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Following Biber (1988), all occurrences of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>you, your, yourself, yourselves</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Following Nini (2014: 18), also includes </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">thy, thee </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>thyself</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. In addition, the forms</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> u, ur, ye, y'all, ya</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>thine</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and the nominal possessive pronoun </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>yours</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> were also added.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Assigned to all occurrences of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>if,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>as long as,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unless,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">lest, in that case, otherwise, even when </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>whether.</t>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of adverbs. If semantic classes of adverbs (stance related adverbs) are included, this feature should be used instead of the original RB.</t>
     </r>
   </si>
 </sst>
@@ -19693,30 +19693,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="B175" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="37" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="70.6640625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" style="4" customWidth="1"/>
-    <col min="13" max="1026" width="14.1640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="16384" width="10.6640625" style="7"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="70.625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="33.625" style="4" customWidth="1"/>
+    <col min="13" max="1026" width="14.125" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="14.625" style="1" customWidth="1"/>
+    <col min="1028" max="16384" width="10.625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="34" customFormat="1" ht="30">
+    <row r="1" spans="1:7" s="34" customFormat="1" ht="25.5">
       <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
@@ -19750,7 +19750,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A3" s="12" t="s">
         <v>284</v>
       </c>
@@ -19773,7 +19773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="38.25">
       <c r="A4" s="12" t="s">
         <v>284</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A5" s="12" t="s">
         <v>284</v>
       </c>
@@ -19819,7 +19819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" ht="45">
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="51">
       <c r="A6" s="12" t="s">
         <v>284</v>
       </c>
@@ -19842,7 +19842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="120">
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="102">
       <c r="A7" s="12" t="s">
         <v>284</v>
       </c>
@@ -19876,7 +19876,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A9" s="18" t="s">
         <v>223</v>
       </c>
@@ -19899,7 +19899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="10" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A10" s="18" t="s">
         <v>223</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="11" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A11" s="18" t="s">
         <v>221</v>
       </c>
@@ -19945,7 +19945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="12" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A12" s="22" t="s">
         <v>221</v>
       </c>
@@ -19968,7 +19968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A13" s="22" t="s">
         <v>221</v>
       </c>
@@ -19991,7 +19991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="14" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A14" s="22" t="s">
         <v>221</v>
       </c>
@@ -20014,7 +20014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A15" s="18" t="s">
         <v>220</v>
       </c>
@@ -20037,7 +20037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="16" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A16" s="18" t="s">
         <v>220</v>
       </c>
@@ -20083,7 +20083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" ht="70.25" customHeight="1">
+    <row r="18" spans="1:7" s="7" customFormat="1" ht="70.349999999999994" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>220</v>
       </c>
@@ -20106,7 +20106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="19" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A19" s="21" t="s">
         <v>220</v>
       </c>
@@ -20129,7 +20129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="20" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A20" s="18" t="s">
         <v>224</v>
       </c>
@@ -20152,7 +20152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="21" spans="1:7" s="7" customFormat="1" ht="114.75">
       <c r="A21" s="18" t="s">
         <v>224</v>
       </c>
@@ -20175,7 +20175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="22" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A22" s="18" t="s">
         <v>224</v>
       </c>
@@ -20198,7 +20198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A23" s="18" t="s">
         <v>224</v>
       </c>
@@ -20221,7 +20221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" ht="30">
+    <row r="24" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A24" s="18" t="s">
         <v>224</v>
       </c>
@@ -20235,7 +20235,7 @@
         <v>239</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>648</v>
+        <v>626</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>32</v>
@@ -20244,7 +20244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="165">
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="140.25">
       <c r="A25" s="18" t="s">
         <v>224</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A26" s="18" t="s">
         <v>224</v>
       </c>
@@ -20290,7 +20290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A27" s="18" t="s">
         <v>224</v>
       </c>
@@ -20313,7 +20313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="28" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A28" s="18" t="s">
         <v>224</v>
       </c>
@@ -20336,7 +20336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="29" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A29" s="18" t="s">
         <v>224</v>
       </c>
@@ -20359,7 +20359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="30" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A30" s="18" t="s">
         <v>224</v>
       </c>
@@ -20382,7 +20382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="31" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A31" s="18" t="s">
         <v>224</v>
       </c>
@@ -20405,7 +20405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="32" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A32" s="18" t="s">
         <v>224</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="33" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A33" s="18" t="s">
         <v>224</v>
       </c>
@@ -20451,7 +20451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="114.75">
       <c r="A34" s="18" t="s">
         <v>224</v>
       </c>
@@ -20474,7 +20474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="35" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A35" s="18" t="s">
         <v>224</v>
       </c>
@@ -20497,7 +20497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="36" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A36" s="18" t="s">
         <v>34</v>
       </c>
@@ -20520,7 +20520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="37" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A37" s="18" t="s">
         <v>34</v>
       </c>
@@ -20543,7 +20543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="38" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A38" s="18" t="s">
         <v>34</v>
       </c>
@@ -20566,7 +20566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="7" customFormat="1">
+    <row r="39" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A39" s="18" t="s">
         <v>34</v>
       </c>
@@ -20589,7 +20589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="40" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A40" s="18" t="s">
         <v>34</v>
       </c>
@@ -20612,7 +20612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="41" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A41" s="18" t="s">
         <v>71</v>
       </c>
@@ -20635,7 +20635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="42" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A42" s="18" t="s">
         <v>117</v>
       </c>
@@ -20658,7 +20658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="43" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A43" s="18" t="s">
         <v>60</v>
       </c>
@@ -20666,7 +20666,7 @@
         <v>244</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>633</v>
+        <v>613</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>242</v>
@@ -20681,7 +20681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="44" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A44" s="18" t="s">
         <v>60</v>
       </c>
@@ -20689,7 +20689,7 @@
         <v>245</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>634</v>
+        <v>614</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>243</v>
@@ -20704,7 +20704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="45" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A45" s="18" t="s">
         <v>60</v>
       </c>
@@ -20712,13 +20712,13 @@
         <v>246</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>635</v>
+        <v>615</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>135</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>647</v>
+        <v>625</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>32</v>
@@ -20727,7 +20727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="46" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A46" s="18" t="s">
         <v>60</v>
       </c>
@@ -20750,21 +20750,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="47" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A47" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>644</v>
+        <v>622</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>646</v>
+        <v>624</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>645</v>
+        <v>623</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>32</v>
@@ -20773,7 +20773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="48" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A48" s="18" t="s">
         <v>60</v>
       </c>
@@ -20781,7 +20781,7 @@
         <v>248</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>636</v>
+        <v>616</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>249</v>
@@ -20796,7 +20796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="49" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A49" s="18" t="s">
         <v>60</v>
       </c>
@@ -20804,7 +20804,7 @@
         <v>247</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>250</v>
@@ -20819,7 +20819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="7" customFormat="1" ht="30">
+    <row r="50" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A50" s="18" t="s">
         <v>60</v>
       </c>
@@ -20842,7 +20842,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="51" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A51" s="18" t="s">
         <v>227</v>
       </c>
@@ -20865,7 +20865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="52" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A52" s="18" t="s">
         <v>227</v>
       </c>
@@ -20888,7 +20888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="53" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A53" s="18" t="s">
         <v>227</v>
       </c>
@@ -20911,7 +20911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="54" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A54" s="18" t="s">
         <v>227</v>
       </c>
@@ -20934,7 +20934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="55" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A55" s="18" t="s">
         <v>227</v>
       </c>
@@ -20957,7 +20957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="56" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A56" s="18" t="s">
         <v>222</v>
       </c>
@@ -20980,7 +20980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="7" customFormat="1" ht="165">
+    <row r="57" spans="1:7" s="7" customFormat="1" ht="153">
       <c r="A57" s="18" t="s">
         <v>222</v>
       </c>
@@ -21003,7 +21003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="58" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A58" s="18" t="s">
         <v>65</v>
       </c>
@@ -21049,7 +21049,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="60" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A60" s="18" t="s">
         <v>228</v>
       </c>
@@ -21072,7 +21072,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="61" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A61" s="18" t="s">
         <v>228</v>
       </c>
@@ -21095,7 +21095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="7" customFormat="1" ht="120">
+    <row r="62" spans="1:7" s="7" customFormat="1" ht="102">
       <c r="A62" s="18" t="s">
         <v>228</v>
       </c>
@@ -21118,7 +21118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="63" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A63" s="18" t="s">
         <v>228</v>
       </c>
@@ -21141,7 +21141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="64" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A64" s="18" t="s">
         <v>228</v>
       </c>
@@ -21164,7 +21164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="65" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A65" s="18" t="s">
         <v>228</v>
       </c>
@@ -21187,7 +21187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="66" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A66" s="18" t="s">
         <v>228</v>
       </c>
@@ -21210,7 +21210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="67" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A67" s="18" t="s">
         <v>228</v>
       </c>
@@ -21233,7 +21233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="7" customFormat="1" ht="165">
+    <row r="68" spans="1:7" s="7" customFormat="1" ht="140.25">
       <c r="A68" s="18" t="s">
         <v>228</v>
       </c>
@@ -21256,7 +21256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="69" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A69" s="18" t="s">
         <v>228</v>
       </c>
@@ -21279,7 +21279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="7" customFormat="1" ht="120">
+    <row r="70" spans="1:7" s="7" customFormat="1" ht="102">
       <c r="A70" s="18" t="s">
         <v>228</v>
       </c>
@@ -21302,7 +21302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="71" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A71" s="18" t="s">
         <v>228</v>
       </c>
@@ -21325,7 +21325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="72" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A72" s="18" t="s">
         <v>228</v>
       </c>
@@ -21348,7 +21348,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="73" spans="1:7" s="7" customFormat="1" ht="114.75">
       <c r="A73" s="18" t="s">
         <v>91</v>
       </c>
@@ -21371,7 +21371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="74" spans="1:7" s="7" customFormat="1" ht="127.5">
       <c r="A74" s="18" t="s">
         <v>91</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="7" customFormat="1" ht="30">
+    <row r="75" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A75" s="18" t="s">
         <v>91</v>
       </c>
@@ -21417,7 +21417,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="76" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A76" s="18" t="s">
         <v>91</v>
       </c>
@@ -21440,7 +21440,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="7" customFormat="1" ht="150">
+    <row r="77" spans="1:7" s="7" customFormat="1" ht="127.5">
       <c r="A77" s="18" t="s">
         <v>91</v>
       </c>
@@ -21463,7 +21463,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="78" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A78" s="18" t="s">
         <v>91</v>
       </c>
@@ -21486,7 +21486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="7" customFormat="1" ht="180">
+    <row r="79" spans="1:7" s="7" customFormat="1" ht="153">
       <c r="A79" s="18" t="s">
         <v>91</v>
       </c>
@@ -21509,7 +21509,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="80" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A80" s="18" t="s">
         <v>91</v>
       </c>
@@ -21532,7 +21532,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:1022" s="7" customFormat="1" ht="75">
+    <row r="81" spans="1:1022" s="7" customFormat="1" ht="63.75">
       <c r="A81" s="18" t="s">
         <v>91</v>
       </c>
@@ -21555,7 +21555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:1022" s="7" customFormat="1" ht="30">
+    <row r="82" spans="1:1022" s="7" customFormat="1" ht="25.5">
       <c r="A82" s="18" t="s">
         <v>91</v>
       </c>
@@ -21578,7 +21578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:1022" s="7" customFormat="1" ht="60">
+    <row r="83" spans="1:1022" s="7" customFormat="1" ht="51">
       <c r="A83" s="18" t="s">
         <v>91</v>
       </c>
@@ -21601,7 +21601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:1022" s="7" customFormat="1" ht="30">
+    <row r="84" spans="1:1022" s="7" customFormat="1" ht="25.5">
       <c r="A84" s="18" t="s">
         <v>91</v>
       </c>
@@ -21624,7 +21624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:1022" s="7" customFormat="1" ht="30">
+    <row r="85" spans="1:1022" s="7" customFormat="1" ht="25.5">
       <c r="A85" s="18" t="s">
         <v>91</v>
       </c>
@@ -21647,7 +21647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:1022" s="7" customFormat="1" ht="60">
+    <row r="86" spans="1:1022" s="7" customFormat="1" ht="51">
       <c r="A86" s="18" t="s">
         <v>91</v>
       </c>
@@ -21670,7 +21670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:1022" s="7" customFormat="1" ht="45">
+    <row r="87" spans="1:1022" s="7" customFormat="1" ht="38.25">
       <c r="A87" s="18" t="s">
         <v>91</v>
       </c>
@@ -21704,7 +21704,7 @@
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
     </row>
-    <row r="89" spans="1:1022" s="8" customFormat="1" ht="60">
+    <row r="89" spans="1:1022" s="8" customFormat="1" ht="51">
       <c r="A89" s="12" t="s">
         <v>34</v>
       </c>
@@ -22742,7 +22742,7 @@
       <c r="AMG89" s="5"/>
       <c r="AMH89" s="5"/>
     </row>
-    <row r="90" spans="1:1022" s="8" customFormat="1" ht="45">
+    <row r="90" spans="1:1022" s="8" customFormat="1" ht="51">
       <c r="A90" s="12" t="s">
         <v>34</v>
       </c>
@@ -23780,7 +23780,7 @@
       <c r="AMG90" s="5"/>
       <c r="AMH90" s="5"/>
     </row>
-    <row r="91" spans="1:1022" s="8" customFormat="1" ht="75">
+    <row r="91" spans="1:1022" s="8" customFormat="1" ht="63.75">
       <c r="A91" s="12" t="s">
         <v>228</v>
       </c>
@@ -23803,7 +23803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:1022" s="7" customFormat="1" ht="75">
+    <row r="92" spans="1:1022" s="7" customFormat="1" ht="63.75">
       <c r="A92" s="12" t="s">
         <v>228</v>
       </c>
@@ -23826,7 +23826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:1022" s="8" customFormat="1" ht="105">
+    <row r="93" spans="1:1022" s="8" customFormat="1" ht="89.25">
       <c r="A93" s="12" t="s">
         <v>91</v>
       </c>
@@ -23849,7 +23849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:1022" s="8" customFormat="1" ht="90">
+    <row r="94" spans="1:1022" s="8" customFormat="1" ht="76.5">
       <c r="A94" s="12" t="s">
         <v>91</v>
       </c>
@@ -23872,7 +23872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:1022" s="8" customFormat="1" ht="75">
+    <row r="95" spans="1:1022" s="8" customFormat="1" ht="63.75">
       <c r="A95" s="12" t="s">
         <v>91</v>
       </c>
@@ -23895,7 +23895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:1022" s="8" customFormat="1" ht="37.25" customHeight="1">
+    <row r="96" spans="1:1022" s="8" customFormat="1" ht="37.35" customHeight="1">
       <c r="A96" s="15"/>
       <c r="B96" s="30"/>
       <c r="C96" s="16"/>
@@ -23906,7 +23906,7 @@
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
     </row>
-    <row r="97" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="97" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A97" s="12" t="s">
         <v>91</v>
       </c>
@@ -23929,7 +23929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="8" customFormat="1" ht="45">
+    <row r="98" spans="1:7" s="8" customFormat="1" ht="38.25">
       <c r="A98" s="12" t="s">
         <v>228</v>
       </c>
@@ -23952,7 +23952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="99" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A99" s="12" t="s">
         <v>224</v>
       </c>
@@ -23975,18 +23975,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="8" customFormat="1" ht="37.25" customHeight="1">
+    <row r="100" spans="1:7" s="8" customFormat="1" ht="37.35" customHeight="1">
       <c r="A100" s="41"/>
       <c r="B100" s="42"/>
       <c r="C100" s="43"/>
       <c r="D100" s="44"/>
       <c r="E100" s="45" t="s">
-        <v>631</v>
+        <v>611</v>
       </c>
       <c r="F100" s="41"/>
       <c r="G100" s="41"/>
     </row>
-    <row r="101" spans="1:7" ht="120">
+    <row r="101" spans="1:7" ht="102">
       <c r="A101" s="18" t="s">
         <v>65</v>
       </c>
@@ -23998,7 +23998,7 @@
       </c>
       <c r="D101" s="19"/>
       <c r="E101" s="19" t="s">
-        <v>632</v>
+        <v>612</v>
       </c>
       <c r="F101" s="18" t="s">
         <v>32</v>
@@ -24007,7 +24007,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="120">
+    <row r="102" spans="1:7" ht="102">
       <c r="A102" s="18" t="s">
         <v>65</v>
       </c>
@@ -24019,7 +24019,7 @@
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="18" t="s">
-        <v>616</v>
+        <v>596</v>
       </c>
       <c r="F102" s="18" t="s">
         <v>32</v>
@@ -24028,7 +24028,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="120">
+    <row r="103" spans="1:7" ht="102">
       <c r="A103" s="18" t="s">
         <v>65</v>
       </c>
@@ -24039,7 +24039,7 @@
         <v>395</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="F103" s="18" t="s">
         <v>32</v>
@@ -24048,7 +24048,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="120">
+    <row r="104" spans="1:7" ht="102">
       <c r="A104" s="18" t="s">
         <v>65</v>
       </c>
@@ -24059,7 +24059,7 @@
         <v>396</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>615</v>
+        <v>595</v>
       </c>
       <c r="F104" s="18" t="s">
         <v>32</v>
@@ -24068,7 +24068,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="120">
+    <row r="105" spans="1:7" ht="102">
       <c r="A105" s="18" t="s">
         <v>65</v>
       </c>
@@ -24079,7 +24079,7 @@
         <v>400</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>617</v>
+        <v>597</v>
       </c>
       <c r="F105" s="18" t="s">
         <v>17</v>
@@ -24088,7 +24088,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="105">
+    <row r="106" spans="1:7" ht="102">
       <c r="A106" s="18" t="s">
         <v>65</v>
       </c>
@@ -24099,7 +24099,7 @@
         <v>401</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>618</v>
+        <v>598</v>
       </c>
       <c r="F106" s="18" t="s">
         <v>17</v>
@@ -24108,7 +24108,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="120">
+    <row r="107" spans="1:7" ht="102">
       <c r="A107" s="18" t="s">
         <v>65</v>
       </c>
@@ -24119,7 +24119,7 @@
         <v>402</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>619</v>
+        <v>599</v>
       </c>
       <c r="F107" s="18" t="s">
         <v>17</v>
@@ -24128,7 +24128,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="120">
+    <row r="108" spans="1:7" ht="102">
       <c r="A108" s="18" t="s">
         <v>65</v>
       </c>
@@ -24139,7 +24139,7 @@
         <v>403</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="F108" s="18" t="s">
         <v>17</v>
@@ -24148,18 +24148,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="120">
+    <row r="109" spans="1:7" ht="102">
       <c r="A109" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="C109" s="19" t="s">
         <v>413</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>621</v>
+        <v>601</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>32</v>
@@ -24168,7 +24168,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="409.6">
+    <row r="110" spans="1:7" ht="382.5">
       <c r="A110" s="18" t="s">
         <v>65</v>
       </c>
@@ -24188,12 +24188,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="135">
+    <row r="111" spans="1:7" ht="127.5">
       <c r="A111" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>624</v>
+        <v>604</v>
       </c>
       <c r="C111" s="19" t="s">
         <v>415</v>
@@ -24208,12 +24208,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="120">
+    <row r="112" spans="1:7" ht="114.75">
       <c r="A112" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="C112" s="19" t="s">
         <v>416</v>
@@ -24228,16 +24228,16 @@
         <v>522</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="120">
+    <row r="113" spans="1:7" ht="102">
       <c r="A113" s="18"/>
       <c r="B113" s="40" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="E113" s="40" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>32</v>
@@ -24246,18 +24246,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="409.6">
+    <row r="114" spans="1:7" ht="395.25">
       <c r="A114" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="C114" s="39" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="E114" s="40" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>32</v>
@@ -24266,18 +24266,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="150">
+    <row r="115" spans="1:7" ht="127.5">
       <c r="A115" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="C115" s="39" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="E115" s="40" t="s">
-        <v>622</v>
+        <v>602</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>32</v>
@@ -24286,18 +24286,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="135">
+    <row r="116" spans="1:7" ht="127.5">
       <c r="A116" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B116" s="40" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="E116" s="40" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>32</v>
@@ -24306,7 +24306,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="75">
+    <row r="117" spans="1:7" ht="51.75">
       <c r="A117" s="18" t="s">
         <v>65</v>
       </c>
@@ -24327,7 +24327,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="75">
+    <row r="118" spans="1:7" ht="51.75">
       <c r="A118" s="18" t="s">
         <v>65</v>
       </c>
@@ -24348,7 +24348,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="75">
+    <row r="119" spans="1:7" ht="51.75">
       <c r="A119" s="18" t="s">
         <v>65</v>
       </c>
@@ -24369,7 +24369,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="75">
+    <row r="120" spans="1:7" ht="51.75">
       <c r="A120" s="18" t="s">
         <v>65</v>
       </c>
@@ -24390,7 +24390,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="75">
+    <row r="121" spans="1:7" ht="51.75">
       <c r="A121" s="18" t="s">
         <v>65</v>
       </c>
@@ -24411,7 +24411,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="105">
+    <row r="122" spans="1:7" ht="90">
       <c r="A122" s="18" t="s">
         <v>65</v>
       </c>
@@ -24432,7 +24432,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="135">
+    <row r="123" spans="1:7" ht="115.5">
       <c r="A123" s="18" t="s">
         <v>65</v>
       </c>
@@ -24453,7 +24453,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="105">
+    <row r="124" spans="1:7" ht="90">
       <c r="A124" s="18" t="s">
         <v>65</v>
       </c>
@@ -24474,7 +24474,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="75">
+    <row r="125" spans="1:7" ht="51.75">
       <c r="A125" s="18" t="s">
         <v>65</v>
       </c>
@@ -24495,7 +24495,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="75">
+    <row r="126" spans="1:7" ht="64.5">
       <c r="A126" s="18" t="s">
         <v>65</v>
       </c>
@@ -24516,7 +24516,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="105">
+    <row r="127" spans="1:7" ht="90">
       <c r="A127" s="18" t="s">
         <v>65</v>
       </c>
@@ -24537,7 +24537,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="409.6">
+    <row r="128" spans="1:7" ht="383.25">
       <c r="A128" s="18" t="s">
         <v>65</v>
       </c>
@@ -24558,7 +24558,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="135">
+    <row r="129" spans="1:7" ht="115.5">
       <c r="A129" s="18" t="s">
         <v>65</v>
       </c>
@@ -24579,7 +24579,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="120">
+    <row r="130" spans="1:7" ht="102.75">
       <c r="A130" s="18" t="s">
         <v>65</v>
       </c>
@@ -24600,7 +24600,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="75">
+    <row r="131" spans="1:7" ht="64.5">
       <c r="A131" s="18" t="s">
         <v>65</v>
       </c>
@@ -24620,7 +24620,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="180">
+    <row r="132" spans="1:7" ht="166.5">
       <c r="A132" s="18" t="s">
         <v>65</v>
       </c>
@@ -24640,7 +24640,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="75">
+    <row r="133" spans="1:7" ht="64.5">
       <c r="A133" s="18" t="s">
         <v>548</v>
       </c>
@@ -24660,7 +24660,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="75">
+    <row r="134" spans="1:7" ht="51">
       <c r="A134" s="18" t="s">
         <v>548</v>
       </c>
@@ -24680,7 +24680,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="75">
+    <row r="135" spans="1:7" ht="64.5">
       <c r="A135" s="18" t="s">
         <v>548</v>
       </c>
@@ -24700,7 +24700,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="75">
+    <row r="136" spans="1:7" ht="51">
       <c r="A136" s="18" t="s">
         <v>548</v>
       </c>
@@ -24720,7 +24720,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="75">
+    <row r="137" spans="1:7" ht="51.75">
       <c r="A137" s="18" t="s">
         <v>548</v>
       </c>
@@ -24740,7 +24740,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="75">
+    <row r="138" spans="1:7" ht="51">
       <c r="A138" s="18" t="s">
         <v>548</v>
       </c>
@@ -24760,7 +24760,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="75">
+    <row r="139" spans="1:7" ht="51">
       <c r="A139" s="18" t="s">
         <v>548</v>
       </c>
@@ -24780,7 +24780,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="75">
+    <row r="140" spans="1:7" ht="51">
       <c r="A140" s="18" t="s">
         <v>548</v>
       </c>
@@ -24821,7 +24821,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="180">
+    <row r="142" spans="1:7" ht="153.75">
       <c r="A142" s="1" t="s">
         <v>549</v>
       </c>
@@ -24863,7 +24863,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="90">
+    <row r="144" spans="1:7" ht="77.25">
       <c r="A144" s="1" t="s">
         <v>549</v>
       </c>
@@ -24884,7 +24884,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="145" spans="1:1027" ht="409.6">
+    <row r="145" spans="1:1027" ht="383.25">
       <c r="A145" s="1" t="s">
         <v>549</v>
       </c>
@@ -24905,7 +24905,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="1:1027" ht="240">
+    <row r="146" spans="1:1027" ht="204.75">
       <c r="A146" s="1" t="s">
         <v>549</v>
       </c>
@@ -24926,7 +24926,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:1027" ht="135">
+    <row r="147" spans="1:1027" ht="115.5">
       <c r="A147" s="1" t="s">
         <v>549</v>
       </c>
@@ -24947,7 +24947,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="148" spans="1:1027" ht="195">
+    <row r="148" spans="1:1027" ht="166.5">
       <c r="A148" s="1" t="s">
         <v>549</v>
       </c>
@@ -24968,7 +24968,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="149" spans="1:1027" ht="105">
+    <row r="149" spans="1:1027" ht="76.5">
       <c r="A149" s="1" t="s">
         <v>549</v>
       </c>
@@ -24989,28 +24989,28 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:1027" ht="45">
+    <row r="150" spans="1:1027" ht="38.25">
       <c r="A150" s="1" t="s">
         <v>549</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>627</v>
+        <v>607</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>628</v>
+        <v>608</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G150" s="19" t="s">
-        <v>630</v>
+        <v>610</v>
       </c>
     </row>
-    <row r="151" spans="1:1027" ht="180">
+    <row r="151" spans="1:1027" ht="166.5">
       <c r="A151" s="1" t="s">
         <v>549</v>
       </c>
@@ -25031,7 +25031,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="152" spans="1:1027" ht="75">
+    <row r="152" spans="1:1027" ht="51">
       <c r="A152" s="1" t="s">
         <v>550</v>
       </c>
@@ -25051,7 +25051,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="153" spans="1:1027" ht="75">
+    <row r="153" spans="1:1027" ht="51">
       <c r="A153" s="1" t="s">
         <v>550</v>
       </c>
@@ -25071,7 +25071,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="154" spans="1:1027" ht="75">
+    <row r="154" spans="1:1027" ht="51">
       <c r="A154" s="1" t="s">
         <v>550</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="155" spans="1:1027" ht="75">
+    <row r="155" spans="1:1027" ht="51">
       <c r="A155" s="1" t="s">
         <v>550</v>
       </c>
@@ -25116,7 +25116,7 @@
       <c r="B156" s="47"/>
       <c r="C156" s="46"/>
       <c r="D156" s="48" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
       <c r="E156" s="47"/>
       <c r="F156" s="46"/>
@@ -26142,67 +26142,67 @@
       <c r="AML156" s="46"/>
       <c r="AMM156" s="46"/>
     </row>
-    <row r="157" spans="1:1027" ht="75">
+    <row r="157" spans="1:1027" ht="51.75">
       <c r="A157" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>642</v>
+        <v>620</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>638</v>
-      </c>
-      <c r="E157" s="37" t="s">
-        <v>639</v>
+        <v>618</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>627</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G157" s="6" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
-    <row r="158" spans="1:1027" ht="75">
+    <row r="158" spans="1:1027" ht="51.75">
       <c r="A158" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>643</v>
+        <v>621</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>640</v>
-      </c>
-      <c r="E158" s="37" t="s">
-        <v>641</v>
+        <v>619</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>628</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G158" s="6" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
-    <row r="159" spans="1:1027" ht="30">
+    <row r="159" spans="1:1027" ht="51.75">
       <c r="A159" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>626</v>
+        <v>606</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="E159" s="37" t="s">
-        <v>560</v>
+      <c r="E159" s="1" t="s">
+        <v>629</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G159" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="160" spans="1:1027" ht="30">
+    <row r="160" spans="1:1027" ht="51.75">
       <c r="A160" s="1" t="s">
         <v>91</v>
       </c>
@@ -26213,16 +26213,16 @@
         <v>537</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>561</v>
+        <v>630</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G160" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="30">
+    <row r="161" spans="1:7" ht="39">
       <c r="A161" s="18" t="s">
         <v>228</v>
       </c>
@@ -26233,16 +26233,16 @@
         <v>538</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>562</v>
+        <v>631</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G161" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="75">
+    <row r="162" spans="1:7" ht="51.75">
       <c r="A162" s="1" t="s">
         <v>550</v>
       </c>
@@ -26253,7 +26253,7 @@
         <v>539</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>563</v>
+        <v>632</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>8</v>
@@ -26262,18 +26262,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="120">
+    <row r="163" spans="1:7" ht="102.75">
       <c r="A163" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>540</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>565</v>
+        <v>633</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>32</v>
@@ -26282,7 +26282,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="75">
+    <row r="164" spans="1:7" ht="64.5">
       <c r="A164" s="1" t="s">
         <v>65</v>
       </c>
@@ -26293,7 +26293,7 @@
         <v>541</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>566</v>
+        <v>634</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>32</v>
@@ -26302,7 +26302,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="120">
+    <row r="165" spans="1:7" ht="102.75">
       <c r="A165" s="1" t="s">
         <v>65</v>
       </c>
@@ -26313,7 +26313,7 @@
         <v>542</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>567</v>
+        <v>635</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>8</v>
@@ -26322,7 +26322,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="75">
+    <row r="166" spans="1:7" ht="64.5">
       <c r="A166" s="1" t="s">
         <v>65</v>
       </c>
@@ -26332,8 +26332,8 @@
       <c r="C166" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="E166" s="37" t="s">
-        <v>568</v>
+      <c r="E166" s="1" t="s">
+        <v>636</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>32</v>
@@ -26342,7 +26342,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="90">
+    <row r="167" spans="1:7" ht="77.25">
       <c r="A167" s="1" t="s">
         <v>65</v>
       </c>
@@ -26352,8 +26352,8 @@
       <c r="C167" s="6" t="s">
         <v>544</v>
       </c>
-      <c r="E167" s="37" t="s">
-        <v>569</v>
+      <c r="E167" s="1" t="s">
+        <v>637</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>8</v>
@@ -26362,18 +26362,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="120">
+    <row r="168" spans="1:7" ht="102.75">
       <c r="A168" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>545</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>570</v>
+        <v>638</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>8</v>
@@ -26382,7 +26382,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="75">
+    <row r="169" spans="1:7" ht="64.5">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
@@ -26392,8 +26392,8 @@
       <c r="C169" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="E169" s="37" t="s">
-        <v>572</v>
+      <c r="E169" s="1" t="s">
+        <v>639</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>32</v>
@@ -26402,7 +26402,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="75">
+    <row r="170" spans="1:7" ht="64.5">
       <c r="A170" s="1" t="s">
         <v>65</v>
       </c>
@@ -26412,8 +26412,8 @@
       <c r="C170" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="E170" s="37" t="s">
-        <v>573</v>
+      <c r="E170" s="1" t="s">
+        <v>640</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>32</v>
@@ -26422,164 +26422,164 @@
         <v>522</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="60">
+    <row r="171" spans="1:7" ht="51.75">
       <c r="A171" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>586</v>
-      </c>
-      <c r="E171" s="37" t="s">
-        <v>601</v>
+        <v>574</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>642</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G171" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="75">
+    <row r="172" spans="1:7" ht="64.5">
       <c r="A172" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>587</v>
-      </c>
-      <c r="E172" s="37" t="s">
-        <v>602</v>
+        <v>575</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>643</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G172" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="75">
+    <row r="173" spans="1:7" ht="64.5">
       <c r="A173" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>588</v>
-      </c>
-      <c r="E173" s="37" t="s">
-        <v>603</v>
+        <v>576</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>644</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G173" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="60">
+    <row r="174" spans="1:7" ht="51.75">
       <c r="A174" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>597</v>
+        <v>585</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>589</v>
-      </c>
-      <c r="E174" s="37" t="s">
-        <v>604</v>
+        <v>577</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>641</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G174" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="60">
+    <row r="175" spans="1:7" ht="51.75">
       <c r="A175" s="1" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>590</v>
-      </c>
-      <c r="E175" s="37" t="s">
-        <v>605</v>
+        <v>578</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>648</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="75">
+    <row r="176" spans="1:7" ht="64.5">
       <c r="A176" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>591</v>
-      </c>
-      <c r="E176" s="37" t="s">
-        <v>606</v>
+        <v>579</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>646</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G176" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="105">
+    <row r="177" spans="1:7" ht="90">
       <c r="A177" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>592</v>
-      </c>
-      <c r="E177" s="37" t="s">
-        <v>610</v>
+        <v>580</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>647</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G177" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="75">
+    <row r="178" spans="1:7" ht="64.5">
       <c r="A178" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>609</v>
+        <v>591</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>593</v>
-      </c>
-      <c r="E178" s="37" t="s">
-        <v>611</v>
+        <v>581</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>645</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G178" s="6" t="s">
-        <v>612</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of minor fixes
Including improvements to QU-tags and other minor fixes.
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94A0C16-E850-4799-838B-F8B7780FFA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D570F4B-190B-EC4C-8E26-CD2C1471299B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -17033,9 +17033,39 @@
     </r>
   </si>
   <si>
+    <t>Any word tagged as MDCA, MDCO, MDMM</t>
+  </si>
+  <si>
+    <t>Any word tagged as MDWS, MDWO, GTO</t>
+  </si>
+  <si>
+    <t>Any word tagged as PASS, PGET</t>
+  </si>
+  <si>
+    <t>Any word tagged as RATT, RNONFACT, RFACT, RLIKELY</t>
+  </si>
+  <si>
     <t>All that complement clauses preceded by stance adjectives, nouns, and verbs</t>
   </si>
   <si>
+    <t>Any word tagged as ThJATT, ThJFCT, ThJLIK, ThJEVL</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThNNFCT, ThNATT, ThNFCT, ThNLIK</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK, ThJATT, ThJFCT, ThJLIK, ThJEVL, ThNNFCT, ThNATT, ThNFCT, ThNLIK</t>
+  </si>
+  <si>
+    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL</t>
+  </si>
+  <si>
+    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL, ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL, ToNSTNC</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">All </t>
     </r>
@@ -17062,6 +17092,12 @@
     </r>
   </si>
   <si>
+    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL</t>
+  </si>
+  <si>
+    <t>Any word tagged as WhVATT, WhVFCT, WhVLIK, WhVCOM</t>
+  </si>
+  <si>
     <t>Biber 1988, adapted by Shakir</t>
   </si>
   <si>
@@ -17435,6 +17471,162 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_IN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_JJAT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_JJPR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_NN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_RB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THRC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <i/>
         <sz val="10"/>
@@ -17503,6 +17695,58 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_THSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Any word tagged as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_WHSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and having no additional semantic tag separated by a space.</t>
+    </r>
+  </si>
+  <si>
     <t>Shakir</t>
   </si>
   <si>
@@ -18140,9 +18384,15 @@
     <t>PP1</t>
   </si>
   <si>
+    <t>Any word tagged with PP1P, PP1S</t>
+  </si>
+  <si>
     <t>PP3</t>
   </si>
   <si>
+    <t>Any word tagged with PP3P, PP3S</t>
+  </si>
+  <si>
     <t>All 1st person referents</t>
   </si>
   <si>
@@ -18409,256 +18659,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>whether.</t>
-    </r>
-  </si>
-  <si>
-    <t>Any word tagged with PP1P, PP1S. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged with PP3P, PP3S. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as MDCA, MDCO, MDMM. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as MDWS, MDWO, GTO. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as PASS, PGET. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as RATT, RNONFACT, RFACT, RLIKELY. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThJATT, ThJFCT, ThJLIK, ThJEVL. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThNNFCT, ThNATT, ThNFCT, ThNLIK. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK, ThJATT, ThJFCT, ThJLIK, ThJEVL, ThNNFCT, ThNATT, ThNFCT, ThNLIK. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ThVCOMM, ThVATT, ThVFCT, ThVLIK. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL, ToJCRTN, ToJABL, ToJEFCT, ToJEASE, ToJEVAL, ToNSTNC. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as ToVDSR, ToVEFRT, ToVPROB, ToVSPCH, ToVMNTL. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <t>Any word tagged as WhVATT, WhVFCT, WhVLIK, WhVCOM. This is an aggregate of the mentioned individual features. If this feature is included in the data table, the corresponding individual features should be excluded to avoid double counting and false correlation between the individual features and the general feature.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_NN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of nouns. If semantic classes of nouns are included, this feature should be used instead of the original NN.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_IN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with stance related prepositions. If stance prepositions are included, this feature should be used instead of the original IN.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_JJAT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of adjectives. If semantic classes of adjectives (stance related adjectives) are included, this feature should be used instead of the original JJAT.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_JJPR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of adjectives. If semantic classes of adjectives (stance related adjectives) are included, this feature should be used instead of the original JJAT.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_WHSC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with WHSC followed by semantic classes of verbs. If those features are included, this feature should be used instead of the original WHSC.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_THRC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with THRC followed by semantic classes of nouns et cetera. If those features are included, this feature should be used instead of the original THRC.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_THSC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with THSC followed by semantic classes of verbs and adjectives et cetera. If those features are included, this feature should be used instead of the original THSC.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Any word tagged as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_RB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and having no additional semantic tag separated by a space. This is an additional feature to circumvent double counting problem with semantic classes of adverbs. If semantic classes of adverbs (stance related adverbs) are included, this feature should be used instead of the original RB.</t>
     </r>
   </si>
 </sst>
@@ -19693,30 +19693,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B175" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E178" sqref="E178"/>
+    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="37" customWidth="1"/>
-    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="70.625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.625" style="4" customWidth="1"/>
-    <col min="13" max="1026" width="14.125" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="14.625" style="1" customWidth="1"/>
-    <col min="1028" max="16384" width="10.625" style="7"/>
+    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="70.6640625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="33.6640625" style="4" customWidth="1"/>
+    <col min="13" max="1026" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1028" max="16384" width="10.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="34" customFormat="1" ht="25.5">
+    <row r="1" spans="1:7" s="34" customFormat="1" ht="30">
       <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
@@ -19750,7 +19750,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="51">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="60">
       <c r="A3" s="12" t="s">
         <v>284</v>
       </c>
@@ -19773,7 +19773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="38.25">
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="45">
       <c r="A4" s="12" t="s">
         <v>284</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="51">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="60">
       <c r="A5" s="12" t="s">
         <v>284</v>
       </c>
@@ -19819,7 +19819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" ht="51">
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="45">
       <c r="A6" s="12" t="s">
         <v>284</v>
       </c>
@@ -19842,7 +19842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="102">
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="120">
       <c r="A7" s="12" t="s">
         <v>284</v>
       </c>
@@ -19876,7 +19876,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A9" s="18" t="s">
         <v>223</v>
       </c>
@@ -19899,7 +19899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="10" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A10" s="18" t="s">
         <v>223</v>
       </c>
@@ -19922,7 +19922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="11" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A11" s="18" t="s">
         <v>221</v>
       </c>
@@ -19945,7 +19945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="12" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A12" s="22" t="s">
         <v>221</v>
       </c>
@@ -19968,7 +19968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A13" s="22" t="s">
         <v>221</v>
       </c>
@@ -19991,7 +19991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="14" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A14" s="22" t="s">
         <v>221</v>
       </c>
@@ -20014,7 +20014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A15" s="18" t="s">
         <v>220</v>
       </c>
@@ -20037,7 +20037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="16" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A16" s="18" t="s">
         <v>220</v>
       </c>
@@ -20083,7 +20083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" ht="70.349999999999994" customHeight="1">
+    <row r="18" spans="1:7" s="7" customFormat="1" ht="70.25" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>220</v>
       </c>
@@ -20106,7 +20106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="19" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A19" s="21" t="s">
         <v>220</v>
       </c>
@@ -20129,7 +20129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="20" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A20" s="18" t="s">
         <v>224</v>
       </c>
@@ -20152,7 +20152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" ht="114.75">
+    <row r="21" spans="1:7" s="7" customFormat="1" ht="135">
       <c r="A21" s="18" t="s">
         <v>224</v>
       </c>
@@ -20175,7 +20175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="22" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A22" s="18" t="s">
         <v>224</v>
       </c>
@@ -20198,7 +20198,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A23" s="18" t="s">
         <v>224</v>
       </c>
@@ -20221,7 +20221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" ht="25.5">
+    <row r="24" spans="1:7" s="7" customFormat="1" ht="30">
       <c r="A24" s="18" t="s">
         <v>224</v>
       </c>
@@ -20235,7 +20235,7 @@
         <v>239</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>626</v>
+        <v>648</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>32</v>
@@ -20244,7 +20244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="140.25">
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="165">
       <c r="A25" s="18" t="s">
         <v>224</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A26" s="18" t="s">
         <v>224</v>
       </c>
@@ -20290,7 +20290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A27" s="18" t="s">
         <v>224</v>
       </c>
@@ -20313,7 +20313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="28" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A28" s="18" t="s">
         <v>224</v>
       </c>
@@ -20336,7 +20336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="29" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A29" s="18" t="s">
         <v>224</v>
       </c>
@@ -20359,7 +20359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="30" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A30" s="18" t="s">
         <v>224</v>
       </c>
@@ -20382,7 +20382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="31" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A31" s="18" t="s">
         <v>224</v>
       </c>
@@ -20405,7 +20405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="32" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A32" s="18" t="s">
         <v>224</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="33" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A33" s="18" t="s">
         <v>224</v>
       </c>
@@ -20451,7 +20451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="7" customFormat="1" ht="114.75">
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="135">
       <c r="A34" s="18" t="s">
         <v>224</v>
       </c>
@@ -20474,7 +20474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="35" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A35" s="18" t="s">
         <v>224</v>
       </c>
@@ -20497,7 +20497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="36" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A36" s="18" t="s">
         <v>34</v>
       </c>
@@ -20520,7 +20520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="37" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A37" s="18" t="s">
         <v>34</v>
       </c>
@@ -20543,7 +20543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="38" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A38" s="18" t="s">
         <v>34</v>
       </c>
@@ -20566,7 +20566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="7" customFormat="1" ht="25.5">
+    <row r="39" spans="1:7" s="7" customFormat="1">
       <c r="A39" s="18" t="s">
         <v>34</v>
       </c>
@@ -20589,7 +20589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="40" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A40" s="18" t="s">
         <v>34</v>
       </c>
@@ -20612,7 +20612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="41" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A41" s="18" t="s">
         <v>71</v>
       </c>
@@ -20635,7 +20635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="42" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A42" s="18" t="s">
         <v>117</v>
       </c>
@@ -20658,7 +20658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="43" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A43" s="18" t="s">
         <v>60</v>
       </c>
@@ -20666,7 +20666,7 @@
         <v>244</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>613</v>
+        <v>633</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>242</v>
@@ -20681,7 +20681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="44" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A44" s="18" t="s">
         <v>60</v>
       </c>
@@ -20689,7 +20689,7 @@
         <v>245</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>614</v>
+        <v>634</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>243</v>
@@ -20704,7 +20704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="45" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A45" s="18" t="s">
         <v>60</v>
       </c>
@@ -20712,13 +20712,13 @@
         <v>246</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>615</v>
+        <v>635</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>135</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>625</v>
+        <v>647</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>32</v>
@@ -20727,7 +20727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="46" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A46" s="18" t="s">
         <v>60</v>
       </c>
@@ -20750,21 +20750,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="47" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A47" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>622</v>
+        <v>644</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>624</v>
+        <v>646</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>623</v>
+        <v>645</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>32</v>
@@ -20773,7 +20773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="48" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A48" s="18" t="s">
         <v>60</v>
       </c>
@@ -20781,7 +20781,7 @@
         <v>248</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>249</v>
@@ -20796,7 +20796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="49" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A49" s="18" t="s">
         <v>60</v>
       </c>
@@ -20804,7 +20804,7 @@
         <v>247</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>617</v>
+        <v>637</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>250</v>
@@ -20819,7 +20819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="7" customFormat="1" ht="25.5">
+    <row r="50" spans="1:7" s="7" customFormat="1" ht="30">
       <c r="A50" s="18" t="s">
         <v>60</v>
       </c>
@@ -20842,7 +20842,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="51" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A51" s="18" t="s">
         <v>227</v>
       </c>
@@ -20865,7 +20865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="52" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A52" s="18" t="s">
         <v>227</v>
       </c>
@@ -20888,7 +20888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="53" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A53" s="18" t="s">
         <v>227</v>
       </c>
@@ -20911,7 +20911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="54" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A54" s="18" t="s">
         <v>227</v>
       </c>
@@ -20934,7 +20934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="7" customFormat="1" ht="89.25">
+    <row r="55" spans="1:7" s="7" customFormat="1" ht="105">
       <c r="A55" s="18" t="s">
         <v>227</v>
       </c>
@@ -20957,7 +20957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="56" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A56" s="18" t="s">
         <v>222</v>
       </c>
@@ -20980,7 +20980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="7" customFormat="1" ht="153">
+    <row r="57" spans="1:7" s="7" customFormat="1" ht="165">
       <c r="A57" s="18" t="s">
         <v>222</v>
       </c>
@@ -21003,7 +21003,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="58" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A58" s="18" t="s">
         <v>65</v>
       </c>
@@ -21049,7 +21049,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="60" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A60" s="18" t="s">
         <v>228</v>
       </c>
@@ -21072,7 +21072,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="61" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A61" s="18" t="s">
         <v>228</v>
       </c>
@@ -21095,7 +21095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="7" customFormat="1" ht="102">
+    <row r="62" spans="1:7" s="7" customFormat="1" ht="120">
       <c r="A62" s="18" t="s">
         <v>228</v>
       </c>
@@ -21118,7 +21118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="63" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A63" s="18" t="s">
         <v>228</v>
       </c>
@@ -21141,7 +21141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="64" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A64" s="18" t="s">
         <v>228</v>
       </c>
@@ -21164,7 +21164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="65" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A65" s="18" t="s">
         <v>228</v>
       </c>
@@ -21187,7 +21187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="66" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A66" s="18" t="s">
         <v>228</v>
       </c>
@@ -21210,7 +21210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="67" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A67" s="18" t="s">
         <v>228</v>
       </c>
@@ -21233,7 +21233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="7" customFormat="1" ht="140.25">
+    <row r="68" spans="1:7" s="7" customFormat="1" ht="165">
       <c r="A68" s="18" t="s">
         <v>228</v>
       </c>
@@ -21256,7 +21256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="69" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A69" s="18" t="s">
         <v>228</v>
       </c>
@@ -21279,7 +21279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="7" customFormat="1" ht="102">
+    <row r="70" spans="1:7" s="7" customFormat="1" ht="120">
       <c r="A70" s="18" t="s">
         <v>228</v>
       </c>
@@ -21302,7 +21302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="71" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A71" s="18" t="s">
         <v>228</v>
       </c>
@@ -21325,7 +21325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="7" customFormat="1" ht="63.75">
+    <row r="72" spans="1:7" s="7" customFormat="1" ht="75">
       <c r="A72" s="18" t="s">
         <v>228</v>
       </c>
@@ -21348,7 +21348,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="7" customFormat="1" ht="114.75">
+    <row r="73" spans="1:7" s="7" customFormat="1" ht="135">
       <c r="A73" s="18" t="s">
         <v>91</v>
       </c>
@@ -21371,7 +21371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="7" customFormat="1" ht="127.5">
+    <row r="74" spans="1:7" s="7" customFormat="1" ht="135">
       <c r="A74" s="18" t="s">
         <v>91</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="7" customFormat="1" ht="25.5">
+    <row r="75" spans="1:7" s="7" customFormat="1" ht="30">
       <c r="A75" s="18" t="s">
         <v>91</v>
       </c>
@@ -21417,7 +21417,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="7" customFormat="1" ht="51">
+    <row r="76" spans="1:7" s="7" customFormat="1" ht="60">
       <c r="A76" s="18" t="s">
         <v>91</v>
       </c>
@@ -21440,7 +21440,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="7" customFormat="1" ht="127.5">
+    <row r="77" spans="1:7" s="7" customFormat="1" ht="150">
       <c r="A77" s="18" t="s">
         <v>91</v>
       </c>
@@ -21463,7 +21463,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="7" customFormat="1" ht="76.5">
+    <row r="78" spans="1:7" s="7" customFormat="1" ht="90">
       <c r="A78" s="18" t="s">
         <v>91</v>
       </c>
@@ -21486,7 +21486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="7" customFormat="1" ht="153">
+    <row r="79" spans="1:7" s="7" customFormat="1" ht="180">
       <c r="A79" s="18" t="s">
         <v>91</v>
       </c>
@@ -21509,7 +21509,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="80" spans="1:7" s="7" customFormat="1" ht="45">
       <c r="A80" s="18" t="s">
         <v>91</v>
       </c>
@@ -21532,7 +21532,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:1022" s="7" customFormat="1" ht="63.75">
+    <row r="81" spans="1:1022" s="7" customFormat="1" ht="75">
       <c r="A81" s="18" t="s">
         <v>91</v>
       </c>
@@ -21555,7 +21555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:1022" s="7" customFormat="1" ht="25.5">
+    <row r="82" spans="1:1022" s="7" customFormat="1" ht="30">
       <c r="A82" s="18" t="s">
         <v>91</v>
       </c>
@@ -21578,7 +21578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:1022" s="7" customFormat="1" ht="51">
+    <row r="83" spans="1:1022" s="7" customFormat="1" ht="60">
       <c r="A83" s="18" t="s">
         <v>91</v>
       </c>
@@ -21601,7 +21601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:1022" s="7" customFormat="1" ht="25.5">
+    <row r="84" spans="1:1022" s="7" customFormat="1" ht="30">
       <c r="A84" s="18" t="s">
         <v>91</v>
       </c>
@@ -21624,7 +21624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:1022" s="7" customFormat="1" ht="25.5">
+    <row r="85" spans="1:1022" s="7" customFormat="1" ht="30">
       <c r="A85" s="18" t="s">
         <v>91</v>
       </c>
@@ -21647,7 +21647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:1022" s="7" customFormat="1" ht="51">
+    <row r="86" spans="1:1022" s="7" customFormat="1" ht="60">
       <c r="A86" s="18" t="s">
         <v>91</v>
       </c>
@@ -21670,7 +21670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:1022" s="7" customFormat="1" ht="38.25">
+    <row r="87" spans="1:1022" s="7" customFormat="1" ht="45">
       <c r="A87" s="18" t="s">
         <v>91</v>
       </c>
@@ -21704,7 +21704,7 @@
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
     </row>
-    <row r="89" spans="1:1022" s="8" customFormat="1" ht="51">
+    <row r="89" spans="1:1022" s="8" customFormat="1" ht="60">
       <c r="A89" s="12" t="s">
         <v>34</v>
       </c>
@@ -22742,7 +22742,7 @@
       <c r="AMG89" s="5"/>
       <c r="AMH89" s="5"/>
     </row>
-    <row r="90" spans="1:1022" s="8" customFormat="1" ht="51">
+    <row r="90" spans="1:1022" s="8" customFormat="1" ht="45">
       <c r="A90" s="12" t="s">
         <v>34</v>
       </c>
@@ -23780,7 +23780,7 @@
       <c r="AMG90" s="5"/>
       <c r="AMH90" s="5"/>
     </row>
-    <row r="91" spans="1:1022" s="8" customFormat="1" ht="63.75">
+    <row r="91" spans="1:1022" s="8" customFormat="1" ht="75">
       <c r="A91" s="12" t="s">
         <v>228</v>
       </c>
@@ -23803,7 +23803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:1022" s="7" customFormat="1" ht="63.75">
+    <row r="92" spans="1:1022" s="7" customFormat="1" ht="75">
       <c r="A92" s="12" t="s">
         <v>228</v>
       </c>
@@ -23826,7 +23826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:1022" s="8" customFormat="1" ht="89.25">
+    <row r="93" spans="1:1022" s="8" customFormat="1" ht="105">
       <c r="A93" s="12" t="s">
         <v>91</v>
       </c>
@@ -23849,7 +23849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:1022" s="8" customFormat="1" ht="76.5">
+    <row r="94" spans="1:1022" s="8" customFormat="1" ht="90">
       <c r="A94" s="12" t="s">
         <v>91</v>
       </c>
@@ -23872,7 +23872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:1022" s="8" customFormat="1" ht="63.75">
+    <row r="95" spans="1:1022" s="8" customFormat="1" ht="75">
       <c r="A95" s="12" t="s">
         <v>91</v>
       </c>
@@ -23895,7 +23895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:1022" s="8" customFormat="1" ht="37.35" customHeight="1">
+    <row r="96" spans="1:1022" s="8" customFormat="1" ht="37.25" customHeight="1">
       <c r="A96" s="15"/>
       <c r="B96" s="30"/>
       <c r="C96" s="16"/>
@@ -23906,7 +23906,7 @@
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
     </row>
-    <row r="97" spans="1:7" s="8" customFormat="1" ht="51">
+    <row r="97" spans="1:7" s="8" customFormat="1" ht="60">
       <c r="A97" s="12" t="s">
         <v>91</v>
       </c>
@@ -23929,7 +23929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="8" customFormat="1" ht="38.25">
+    <row r="98" spans="1:7" s="8" customFormat="1" ht="45">
       <c r="A98" s="12" t="s">
         <v>228</v>
       </c>
@@ -23952,7 +23952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="8" customFormat="1" ht="51">
+    <row r="99" spans="1:7" s="8" customFormat="1" ht="60">
       <c r="A99" s="12" t="s">
         <v>224</v>
       </c>
@@ -23975,18 +23975,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="8" customFormat="1" ht="37.35" customHeight="1">
+    <row r="100" spans="1:7" s="8" customFormat="1" ht="37.25" customHeight="1">
       <c r="A100" s="41"/>
       <c r="B100" s="42"/>
       <c r="C100" s="43"/>
       <c r="D100" s="44"/>
       <c r="E100" s="45" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="F100" s="41"/>
       <c r="G100" s="41"/>
     </row>
-    <row r="101" spans="1:7" ht="102">
+    <row r="101" spans="1:7" ht="120">
       <c r="A101" s="18" t="s">
         <v>65</v>
       </c>
@@ -23998,7 +23998,7 @@
       </c>
       <c r="D101" s="19"/>
       <c r="E101" s="19" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="F101" s="18" t="s">
         <v>32</v>
@@ -24007,7 +24007,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="102">
+    <row r="102" spans="1:7" ht="120">
       <c r="A102" s="18" t="s">
         <v>65</v>
       </c>
@@ -24019,7 +24019,7 @@
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="18" t="s">
-        <v>596</v>
+        <v>616</v>
       </c>
       <c r="F102" s="18" t="s">
         <v>32</v>
@@ -24028,7 +24028,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="102">
+    <row r="103" spans="1:7" ht="120">
       <c r="A103" s="18" t="s">
         <v>65</v>
       </c>
@@ -24039,7 +24039,7 @@
         <v>395</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>594</v>
+        <v>614</v>
       </c>
       <c r="F103" s="18" t="s">
         <v>32</v>
@@ -24048,7 +24048,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="102">
+    <row r="104" spans="1:7" ht="120">
       <c r="A104" s="18" t="s">
         <v>65</v>
       </c>
@@ -24059,7 +24059,7 @@
         <v>396</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>595</v>
+        <v>615</v>
       </c>
       <c r="F104" s="18" t="s">
         <v>32</v>
@@ -24068,7 +24068,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="102">
+    <row r="105" spans="1:7" ht="120">
       <c r="A105" s="18" t="s">
         <v>65</v>
       </c>
@@ -24079,7 +24079,7 @@
         <v>400</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>597</v>
+        <v>617</v>
       </c>
       <c r="F105" s="18" t="s">
         <v>17</v>
@@ -24088,7 +24088,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="102">
+    <row r="106" spans="1:7" ht="105">
       <c r="A106" s="18" t="s">
         <v>65</v>
       </c>
@@ -24099,7 +24099,7 @@
         <v>401</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="F106" s="18" t="s">
         <v>17</v>
@@ -24108,7 +24108,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="102">
+    <row r="107" spans="1:7" ht="120">
       <c r="A107" s="18" t="s">
         <v>65</v>
       </c>
@@ -24119,7 +24119,7 @@
         <v>402</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>599</v>
+        <v>619</v>
       </c>
       <c r="F107" s="18" t="s">
         <v>17</v>
@@ -24128,7 +24128,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="102">
+    <row r="108" spans="1:7" ht="120">
       <c r="A108" s="18" t="s">
         <v>65</v>
       </c>
@@ -24139,7 +24139,7 @@
         <v>403</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="F108" s="18" t="s">
         <v>17</v>
@@ -24148,18 +24148,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="102">
+    <row r="109" spans="1:7" ht="120">
       <c r="A109" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>605</v>
+        <v>625</v>
       </c>
       <c r="C109" s="19" t="s">
         <v>413</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>601</v>
+        <v>621</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>32</v>
@@ -24168,7 +24168,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="382.5">
+    <row r="110" spans="1:7" ht="409.6">
       <c r="A110" s="18" t="s">
         <v>65</v>
       </c>
@@ -24188,12 +24188,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="127.5">
+    <row r="111" spans="1:7" ht="135">
       <c r="A111" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>604</v>
+        <v>624</v>
       </c>
       <c r="C111" s="19" t="s">
         <v>415</v>
@@ -24208,12 +24208,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="114.75">
+    <row r="112" spans="1:7" ht="120">
       <c r="A112" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>603</v>
+        <v>623</v>
       </c>
       <c r="C112" s="19" t="s">
         <v>416</v>
@@ -24228,16 +24228,16 @@
         <v>522</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="102">
+    <row r="113" spans="1:7" ht="120">
       <c r="A113" s="18"/>
       <c r="B113" s="40" t="s">
-        <v>567</v>
+        <v>579</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="E113" s="40" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>32</v>
@@ -24246,18 +24246,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="395.25">
+    <row r="114" spans="1:7" ht="409.6">
       <c r="A114" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>568</v>
+        <v>580</v>
       </c>
       <c r="C114" s="39" t="s">
-        <v>564</v>
+        <v>576</v>
       </c>
       <c r="E114" s="40" t="s">
-        <v>572</v>
+        <v>584</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>32</v>
@@ -24266,18 +24266,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="127.5">
+    <row r="115" spans="1:7" ht="150">
       <c r="A115" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>569</v>
+        <v>581</v>
       </c>
       <c r="C115" s="39" t="s">
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="E115" s="40" t="s">
-        <v>602</v>
+        <v>622</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>32</v>
@@ -24286,18 +24286,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="127.5">
+    <row r="116" spans="1:7" ht="135">
       <c r="A116" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B116" s="40" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="E116" s="40" t="s">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>32</v>
@@ -24306,7 +24306,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="51.75">
+    <row r="117" spans="1:7" ht="75">
       <c r="A117" s="18" t="s">
         <v>65</v>
       </c>
@@ -24327,7 +24327,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="51.75">
+    <row r="118" spans="1:7" ht="75">
       <c r="A118" s="18" t="s">
         <v>65</v>
       </c>
@@ -24348,7 +24348,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="51.75">
+    <row r="119" spans="1:7" ht="75">
       <c r="A119" s="18" t="s">
         <v>65</v>
       </c>
@@ -24369,7 +24369,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="51.75">
+    <row r="120" spans="1:7" ht="75">
       <c r="A120" s="18" t="s">
         <v>65</v>
       </c>
@@ -24390,7 +24390,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="51.75">
+    <row r="121" spans="1:7" ht="75">
       <c r="A121" s="18" t="s">
         <v>65</v>
       </c>
@@ -24411,7 +24411,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="90">
+    <row r="122" spans="1:7" ht="105">
       <c r="A122" s="18" t="s">
         <v>65</v>
       </c>
@@ -24432,7 +24432,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="115.5">
+    <row r="123" spans="1:7" ht="135">
       <c r="A123" s="18" t="s">
         <v>65</v>
       </c>
@@ -24453,7 +24453,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="90">
+    <row r="124" spans="1:7" ht="105">
       <c r="A124" s="18" t="s">
         <v>65</v>
       </c>
@@ -24474,7 +24474,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="51.75">
+    <row r="125" spans="1:7" ht="75">
       <c r="A125" s="18" t="s">
         <v>65</v>
       </c>
@@ -24495,7 +24495,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="64.5">
+    <row r="126" spans="1:7" ht="75">
       <c r="A126" s="18" t="s">
         <v>65</v>
       </c>
@@ -24516,7 +24516,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="90">
+    <row r="127" spans="1:7" ht="105">
       <c r="A127" s="18" t="s">
         <v>65</v>
       </c>
@@ -24537,7 +24537,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="383.25">
+    <row r="128" spans="1:7" ht="409.6">
       <c r="A128" s="18" t="s">
         <v>65</v>
       </c>
@@ -24558,7 +24558,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="115.5">
+    <row r="129" spans="1:7" ht="135">
       <c r="A129" s="18" t="s">
         <v>65</v>
       </c>
@@ -24579,7 +24579,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="102.75">
+    <row r="130" spans="1:7" ht="120">
       <c r="A130" s="18" t="s">
         <v>65</v>
       </c>
@@ -24600,7 +24600,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="64.5">
+    <row r="131" spans="1:7" ht="75">
       <c r="A131" s="18" t="s">
         <v>65</v>
       </c>
@@ -24620,7 +24620,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="166.5">
+    <row r="132" spans="1:7" ht="180">
       <c r="A132" s="18" t="s">
         <v>65</v>
       </c>
@@ -24640,7 +24640,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="64.5">
+    <row r="133" spans="1:7" ht="75">
       <c r="A133" s="18" t="s">
         <v>548</v>
       </c>
@@ -24660,7 +24660,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="51">
+    <row r="134" spans="1:7" ht="75">
       <c r="A134" s="18" t="s">
         <v>548</v>
       </c>
@@ -24680,7 +24680,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="64.5">
+    <row r="135" spans="1:7" ht="75">
       <c r="A135" s="18" t="s">
         <v>548</v>
       </c>
@@ -24700,7 +24700,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="51">
+    <row r="136" spans="1:7" ht="75">
       <c r="A136" s="18" t="s">
         <v>548</v>
       </c>
@@ -24720,7 +24720,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="51.75">
+    <row r="137" spans="1:7" ht="75">
       <c r="A137" s="18" t="s">
         <v>548</v>
       </c>
@@ -24740,7 +24740,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="51">
+    <row r="138" spans="1:7" ht="75">
       <c r="A138" s="18" t="s">
         <v>548</v>
       </c>
@@ -24760,7 +24760,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="51">
+    <row r="139" spans="1:7" ht="75">
       <c r="A139" s="18" t="s">
         <v>548</v>
       </c>
@@ -24780,7 +24780,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="51">
+    <row r="140" spans="1:7" ht="75">
       <c r="A140" s="18" t="s">
         <v>548</v>
       </c>
@@ -24821,7 +24821,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="153.75">
+    <row r="142" spans="1:7" ht="180">
       <c r="A142" s="1" t="s">
         <v>549</v>
       </c>
@@ -24863,7 +24863,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="77.25">
+    <row r="144" spans="1:7" ht="90">
       <c r="A144" s="1" t="s">
         <v>549</v>
       </c>
@@ -24884,7 +24884,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="145" spans="1:1027" ht="383.25">
+    <row r="145" spans="1:1027" ht="409.6">
       <c r="A145" s="1" t="s">
         <v>549</v>
       </c>
@@ -24905,7 +24905,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="1:1027" ht="204.75">
+    <row r="146" spans="1:1027" ht="240">
       <c r="A146" s="1" t="s">
         <v>549</v>
       </c>
@@ -24926,7 +24926,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:1027" ht="115.5">
+    <row r="147" spans="1:1027" ht="135">
       <c r="A147" s="1" t="s">
         <v>549</v>
       </c>
@@ -24947,7 +24947,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="148" spans="1:1027" ht="166.5">
+    <row r="148" spans="1:1027" ht="195">
       <c r="A148" s="1" t="s">
         <v>549</v>
       </c>
@@ -24968,7 +24968,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="149" spans="1:1027" ht="76.5">
+    <row r="149" spans="1:1027" ht="105">
       <c r="A149" s="1" t="s">
         <v>549</v>
       </c>
@@ -24989,28 +24989,28 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:1027" ht="38.25">
+    <row r="150" spans="1:1027" ht="45">
       <c r="A150" s="1" t="s">
         <v>549</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>607</v>
+        <v>627</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G150" s="19" t="s">
-        <v>610</v>
+        <v>630</v>
       </c>
     </row>
-    <row r="151" spans="1:1027" ht="166.5">
+    <row r="151" spans="1:1027" ht="180">
       <c r="A151" s="1" t="s">
         <v>549</v>
       </c>
@@ -25031,7 +25031,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="152" spans="1:1027" ht="51">
+    <row r="152" spans="1:1027" ht="75">
       <c r="A152" s="1" t="s">
         <v>550</v>
       </c>
@@ -25051,7 +25051,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="153" spans="1:1027" ht="51">
+    <row r="153" spans="1:1027" ht="75">
       <c r="A153" s="1" t="s">
         <v>550</v>
       </c>
@@ -25071,7 +25071,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="154" spans="1:1027" ht="51">
+    <row r="154" spans="1:1027" ht="75">
       <c r="A154" s="1" t="s">
         <v>550</v>
       </c>
@@ -25091,7 +25091,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="155" spans="1:1027" ht="51">
+    <row r="155" spans="1:1027" ht="75">
       <c r="A155" s="1" t="s">
         <v>550</v>
       </c>
@@ -25116,7 +25116,7 @@
       <c r="B156" s="47"/>
       <c r="C156" s="46"/>
       <c r="D156" s="48" t="s">
-        <v>593</v>
+        <v>613</v>
       </c>
       <c r="E156" s="47"/>
       <c r="F156" s="46"/>
@@ -26142,67 +26142,67 @@
       <c r="AML156" s="46"/>
       <c r="AMM156" s="46"/>
     </row>
-    <row r="157" spans="1:1027" ht="51.75">
+    <row r="157" spans="1:1027" ht="75">
       <c r="A157" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>620</v>
+        <v>642</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>618</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>627</v>
+        <v>638</v>
+      </c>
+      <c r="E157" s="37" t="s">
+        <v>639</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G157" s="6" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
     </row>
-    <row r="158" spans="1:1027" ht="51.75">
+    <row r="158" spans="1:1027" ht="75">
       <c r="A158" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>621</v>
+        <v>643</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>628</v>
+        <v>640</v>
+      </c>
+      <c r="E158" s="37" t="s">
+        <v>641</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G158" s="6" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
     </row>
-    <row r="159" spans="1:1027" ht="51.75">
+    <row r="159" spans="1:1027" ht="30">
       <c r="A159" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>606</v>
+        <v>626</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="E159" s="1" t="s">
-        <v>629</v>
+      <c r="E159" s="37" t="s">
+        <v>560</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G159" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="160" spans="1:1027" ht="51.75">
+    <row r="160" spans="1:1027" ht="30">
       <c r="A160" s="1" t="s">
         <v>91</v>
       </c>
@@ -26213,16 +26213,16 @@
         <v>537</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>630</v>
+        <v>561</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G160" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="39">
+    <row r="161" spans="1:7" ht="30">
       <c r="A161" s="18" t="s">
         <v>228</v>
       </c>
@@ -26233,16 +26233,16 @@
         <v>538</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>631</v>
+        <v>562</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G161" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="51.75">
+    <row r="162" spans="1:7" ht="75">
       <c r="A162" s="1" t="s">
         <v>550</v>
       </c>
@@ -26253,7 +26253,7 @@
         <v>539</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>632</v>
+        <v>563</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>8</v>
@@ -26262,18 +26262,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="102.75">
+    <row r="163" spans="1:7" ht="120">
       <c r="A163" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>540</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>633</v>
+        <v>565</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>32</v>
@@ -26282,7 +26282,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="64.5">
+    <row r="164" spans="1:7" ht="75">
       <c r="A164" s="1" t="s">
         <v>65</v>
       </c>
@@ -26293,7 +26293,7 @@
         <v>541</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>634</v>
+        <v>566</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>32</v>
@@ -26302,7 +26302,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="102.75">
+    <row r="165" spans="1:7" ht="120">
       <c r="A165" s="1" t="s">
         <v>65</v>
       </c>
@@ -26313,7 +26313,7 @@
         <v>542</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>635</v>
+        <v>567</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>8</v>
@@ -26322,7 +26322,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="64.5">
+    <row r="166" spans="1:7" ht="75">
       <c r="A166" s="1" t="s">
         <v>65</v>
       </c>
@@ -26332,8 +26332,8 @@
       <c r="C166" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="E166" s="1" t="s">
-        <v>636</v>
+      <c r="E166" s="37" t="s">
+        <v>568</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>32</v>
@@ -26342,7 +26342,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="77.25">
+    <row r="167" spans="1:7" ht="90">
       <c r="A167" s="1" t="s">
         <v>65</v>
       </c>
@@ -26352,8 +26352,8 @@
       <c r="C167" s="6" t="s">
         <v>544</v>
       </c>
-      <c r="E167" s="1" t="s">
-        <v>637</v>
+      <c r="E167" s="37" t="s">
+        <v>569</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>8</v>
@@ -26362,18 +26362,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="102.75">
+    <row r="168" spans="1:7" ht="120">
       <c r="A168" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>561</v>
+        <v>571</v>
       </c>
       <c r="C168" s="6" t="s">
         <v>545</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>638</v>
+        <v>570</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>8</v>
@@ -26382,7 +26382,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="64.5">
+    <row r="169" spans="1:7" ht="75">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
@@ -26392,8 +26392,8 @@
       <c r="C169" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="E169" s="1" t="s">
-        <v>639</v>
+      <c r="E169" s="37" t="s">
+        <v>572</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>32</v>
@@ -26402,7 +26402,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="64.5">
+    <row r="170" spans="1:7" ht="75">
       <c r="A170" s="1" t="s">
         <v>65</v>
       </c>
@@ -26412,8 +26412,8 @@
       <c r="C170" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="E170" s="1" t="s">
-        <v>640</v>
+      <c r="E170" s="37" t="s">
+        <v>573</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>32</v>
@@ -26422,164 +26422,164 @@
         <v>522</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="51.75">
+    <row r="171" spans="1:7" ht="60">
       <c r="A171" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>574</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>642</v>
+        <v>586</v>
+      </c>
+      <c r="E171" s="37" t="s">
+        <v>601</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G171" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="64.5">
+    <row r="172" spans="1:7" ht="75">
       <c r="A172" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>575</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>643</v>
+        <v>587</v>
+      </c>
+      <c r="E172" s="37" t="s">
+        <v>602</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G172" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="64.5">
+    <row r="173" spans="1:7" ht="75">
       <c r="A173" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>576</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>644</v>
+        <v>588</v>
+      </c>
+      <c r="E173" s="37" t="s">
+        <v>603</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G173" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="51.75">
+    <row r="174" spans="1:7" ht="60">
       <c r="A174" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>641</v>
+        <v>589</v>
+      </c>
+      <c r="E174" s="37" t="s">
+        <v>604</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G174" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="51.75">
+    <row r="175" spans="1:7" ht="60">
       <c r="A175" s="1" t="s">
-        <v>587</v>
+        <v>599</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>586</v>
+        <v>598</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>578</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>648</v>
+        <v>590</v>
+      </c>
+      <c r="E175" s="37" t="s">
+        <v>605</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="64.5">
+    <row r="176" spans="1:7" ht="75">
       <c r="A176" s="1" t="s">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>589</v>
+        <v>607</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>646</v>
+        <v>591</v>
+      </c>
+      <c r="E176" s="37" t="s">
+        <v>606</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G176" s="6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="105">
+      <c r="A177" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C177" s="6" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" ht="90">
-      <c r="A177" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>580</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>647</v>
+      <c r="E177" s="37" t="s">
+        <v>610</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G177" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="64.5">
+    <row r="178" spans="1:7" ht="75">
       <c r="A178" s="1" t="s">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>591</v>
+        <v>609</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>581</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>645</v>
+        <v>593</v>
+      </c>
+      <c r="E178" s="37" t="s">
+        <v>611</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G178" s="6" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a warning in fron of composite tags
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D570F4B-190B-EC4C-8E26-CD2C1471299B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27393D6-4C32-4731-872B-B0F270C9DC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="650">
   <si>
     <t>Feature</t>
   </si>
@@ -16779,42 +16779,6 @@
     </r>
   </si>
   <si>
-    <t>MDPOSSCAll</t>
-  </si>
-  <si>
-    <t>MDPREDAll</t>
-  </si>
-  <si>
-    <t>PASSAll</t>
-  </si>
-  <si>
-    <t>RSTNCAll</t>
-  </si>
-  <si>
-    <t>ThJSTNCAll</t>
-  </si>
-  <si>
-    <t>ThNSTNCAll</t>
-  </si>
-  <si>
-    <t>ThSTNCAll</t>
-  </si>
-  <si>
-    <t>ThVSTNCAll</t>
-  </si>
-  <si>
-    <t>ToJSTNCAll</t>
-  </si>
-  <si>
-    <t>ToSTNCAll</t>
-  </si>
-  <si>
-    <t>ToVSTNCAll</t>
-  </si>
-  <si>
-    <t>WhVSTNCAll</t>
-  </si>
-  <si>
     <t>Adjective semantics</t>
   </si>
   <si>
@@ -18660,6 +18624,45 @@
       </rPr>
       <t>whether.</t>
     </r>
+  </si>
+  <si>
+    <t>PASSall</t>
+  </si>
+  <si>
+    <t>RSTNCall</t>
+  </si>
+  <si>
+    <t>ThJSTNCall</t>
+  </si>
+  <si>
+    <t>ThNSTNCall</t>
+  </si>
+  <si>
+    <t>ThSTNCall</t>
+  </si>
+  <si>
+    <t>ThVSTNCall</t>
+  </si>
+  <si>
+    <t>ToJSTNCall</t>
+  </si>
+  <si>
+    <t>ToSTNCall</t>
+  </si>
+  <si>
+    <t>ToVSTNCall</t>
+  </si>
+  <si>
+    <t>WhVSTNCall</t>
+  </si>
+  <si>
+    <t>MDPOSSCall</t>
+  </si>
+  <si>
+    <t>MDPREDall</t>
+  </si>
+  <si>
+    <t>The tags consist of aggregates of individual tags. To avoid false correlation, skew etc. in the data, they should not be used in combination with the tags they are made of.</t>
   </si>
 </sst>
 </file>
@@ -19693,30 +19696,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="37" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="70.6640625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" style="4" customWidth="1"/>
-    <col min="13" max="1026" width="14.1640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="16384" width="10.6640625" style="7"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="70.625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="33.625" style="4" customWidth="1"/>
+    <col min="13" max="1026" width="14.125" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="14.625" style="1" customWidth="1"/>
+    <col min="1028" max="16384" width="10.625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="34" customFormat="1" ht="30">
+    <row r="1" spans="1:7" s="34" customFormat="1" ht="25.5">
       <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
@@ -19750,7 +19753,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A3" s="12" t="s">
         <v>284</v>
       </c>
@@ -19773,7 +19776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="8" customFormat="1" ht="38.25">
       <c r="A4" s="12" t="s">
         <v>284</v>
       </c>
@@ -19796,7 +19799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A5" s="12" t="s">
         <v>284</v>
       </c>
@@ -19819,7 +19822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" ht="45">
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="51">
       <c r="A6" s="12" t="s">
         <v>284</v>
       </c>
@@ -19842,7 +19845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="120">
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="102">
       <c r="A7" s="12" t="s">
         <v>284</v>
       </c>
@@ -19876,7 +19879,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="9" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A9" s="18" t="s">
         <v>223</v>
       </c>
@@ -19899,7 +19902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="10" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A10" s="18" t="s">
         <v>223</v>
       </c>
@@ -19922,7 +19925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="11" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A11" s="18" t="s">
         <v>221</v>
       </c>
@@ -19945,7 +19948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="12" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A12" s="22" t="s">
         <v>221</v>
       </c>
@@ -19968,7 +19971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="13" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A13" s="22" t="s">
         <v>221</v>
       </c>
@@ -19991,7 +19994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="14" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A14" s="22" t="s">
         <v>221</v>
       </c>
@@ -20014,7 +20017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="15" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A15" s="18" t="s">
         <v>220</v>
       </c>
@@ -20037,7 +20040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="16" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A16" s="18" t="s">
         <v>220</v>
       </c>
@@ -20083,7 +20086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" ht="70.25" customHeight="1">
+    <row r="18" spans="1:7" s="7" customFormat="1" ht="70.349999999999994" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>220</v>
       </c>
@@ -20106,7 +20109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="19" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A19" s="21" t="s">
         <v>220</v>
       </c>
@@ -20129,7 +20132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="20" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A20" s="18" t="s">
         <v>224</v>
       </c>
@@ -20152,7 +20155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="21" spans="1:7" s="7" customFormat="1" ht="114.75">
       <c r="A21" s="18" t="s">
         <v>224</v>
       </c>
@@ -20175,7 +20178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="22" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A22" s="18" t="s">
         <v>224</v>
       </c>
@@ -20198,7 +20201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="23" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A23" s="18" t="s">
         <v>224</v>
       </c>
@@ -20221,7 +20224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" ht="30">
+    <row r="24" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A24" s="18" t="s">
         <v>224</v>
       </c>
@@ -20235,7 +20238,7 @@
         <v>239</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>648</v>
+        <v>636</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>32</v>
@@ -20244,7 +20247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" ht="165">
+    <row r="25" spans="1:7" s="7" customFormat="1" ht="140.25">
       <c r="A25" s="18" t="s">
         <v>224</v>
       </c>
@@ -20267,7 +20270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="26" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A26" s="18" t="s">
         <v>224</v>
       </c>
@@ -20290,7 +20293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="27" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A27" s="18" t="s">
         <v>224</v>
       </c>
@@ -20313,7 +20316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="28" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A28" s="18" t="s">
         <v>224</v>
       </c>
@@ -20336,7 +20339,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="29" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A29" s="18" t="s">
         <v>224</v>
       </c>
@@ -20359,7 +20362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="30" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A30" s="18" t="s">
         <v>224</v>
       </c>
@@ -20382,7 +20385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="31" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A31" s="18" t="s">
         <v>224</v>
       </c>
@@ -20405,7 +20408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="32" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A32" s="18" t="s">
         <v>224</v>
       </c>
@@ -20428,7 +20431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="33" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A33" s="18" t="s">
         <v>224</v>
       </c>
@@ -20451,7 +20454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="114.75">
       <c r="A34" s="18" t="s">
         <v>224</v>
       </c>
@@ -20474,7 +20477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="35" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A35" s="18" t="s">
         <v>224</v>
       </c>
@@ -20497,7 +20500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="36" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A36" s="18" t="s">
         <v>34</v>
       </c>
@@ -20520,7 +20523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="37" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A37" s="18" t="s">
         <v>34</v>
       </c>
@@ -20543,7 +20546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="38" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A38" s="18" t="s">
         <v>34</v>
       </c>
@@ -20566,7 +20569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="7" customFormat="1">
+    <row r="39" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A39" s="18" t="s">
         <v>34</v>
       </c>
@@ -20589,7 +20592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="40" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A40" s="18" t="s">
         <v>34</v>
       </c>
@@ -20612,7 +20615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="41" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A41" s="18" t="s">
         <v>71</v>
       </c>
@@ -20635,7 +20638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="42" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A42" s="18" t="s">
         <v>117</v>
       </c>
@@ -20658,7 +20661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="43" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A43" s="18" t="s">
         <v>60</v>
       </c>
@@ -20666,7 +20669,7 @@
         <v>244</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>242</v>
@@ -20681,7 +20684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="44" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A44" s="18" t="s">
         <v>60</v>
       </c>
@@ -20689,7 +20692,7 @@
         <v>245</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>243</v>
@@ -20704,7 +20707,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="45" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A45" s="18" t="s">
         <v>60</v>
       </c>
@@ -20712,13 +20715,13 @@
         <v>246</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>135</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>647</v>
+        <v>635</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>32</v>
@@ -20727,7 +20730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="46" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A46" s="18" t="s">
         <v>60</v>
       </c>
@@ -20750,21 +20753,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="47" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A47" s="18" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>644</v>
+        <v>632</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>646</v>
+        <v>634</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>133</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>645</v>
+        <v>633</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>32</v>
@@ -20773,7 +20776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="48" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A48" s="18" t="s">
         <v>60</v>
       </c>
@@ -20781,7 +20784,7 @@
         <v>248</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>249</v>
@@ -20796,7 +20799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="49" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A49" s="18" t="s">
         <v>60</v>
       </c>
@@ -20804,7 +20807,7 @@
         <v>247</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>250</v>
@@ -20819,7 +20822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="7" customFormat="1" ht="30">
+    <row r="50" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A50" s="18" t="s">
         <v>60</v>
       </c>
@@ -20842,7 +20845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="51" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A51" s="18" t="s">
         <v>227</v>
       </c>
@@ -20865,7 +20868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="52" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A52" s="18" t="s">
         <v>227</v>
       </c>
@@ -20888,7 +20891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="53" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A53" s="18" t="s">
         <v>227</v>
       </c>
@@ -20911,7 +20914,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="54" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A54" s="18" t="s">
         <v>227</v>
       </c>
@@ -20934,7 +20937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="7" customFormat="1" ht="105">
+    <row r="55" spans="1:7" s="7" customFormat="1" ht="89.25">
       <c r="A55" s="18" t="s">
         <v>227</v>
       </c>
@@ -20957,7 +20960,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="56" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A56" s="18" t="s">
         <v>222</v>
       </c>
@@ -20980,7 +20983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="7" customFormat="1" ht="165">
+    <row r="57" spans="1:7" s="7" customFormat="1" ht="153">
       <c r="A57" s="18" t="s">
         <v>222</v>
       </c>
@@ -21003,7 +21006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="58" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A58" s="18" t="s">
         <v>65</v>
       </c>
@@ -21049,7 +21052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="60" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A60" s="18" t="s">
         <v>228</v>
       </c>
@@ -21072,7 +21075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="61" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A61" s="18" t="s">
         <v>228</v>
       </c>
@@ -21095,7 +21098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="7" customFormat="1" ht="120">
+    <row r="62" spans="1:7" s="7" customFormat="1" ht="102">
       <c r="A62" s="18" t="s">
         <v>228</v>
       </c>
@@ -21118,7 +21121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="63" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A63" s="18" t="s">
         <v>228</v>
       </c>
@@ -21141,7 +21144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="64" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A64" s="18" t="s">
         <v>228</v>
       </c>
@@ -21164,7 +21167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="65" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A65" s="18" t="s">
         <v>228</v>
       </c>
@@ -21187,7 +21190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="66" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A66" s="18" t="s">
         <v>228</v>
       </c>
@@ -21210,7 +21213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="67" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A67" s="18" t="s">
         <v>228</v>
       </c>
@@ -21233,7 +21236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="7" customFormat="1" ht="165">
+    <row r="68" spans="1:7" s="7" customFormat="1" ht="140.25">
       <c r="A68" s="18" t="s">
         <v>228</v>
       </c>
@@ -21256,7 +21259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="69" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A69" s="18" t="s">
         <v>228</v>
       </c>
@@ -21279,7 +21282,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="7" customFormat="1" ht="120">
+    <row r="70" spans="1:7" s="7" customFormat="1" ht="102">
       <c r="A70" s="18" t="s">
         <v>228</v>
       </c>
@@ -21302,7 +21305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="71" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A71" s="18" t="s">
         <v>228</v>
       </c>
@@ -21325,7 +21328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="7" customFormat="1" ht="75">
+    <row r="72" spans="1:7" s="7" customFormat="1" ht="63.75">
       <c r="A72" s="18" t="s">
         <v>228</v>
       </c>
@@ -21348,7 +21351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="73" spans="1:7" s="7" customFormat="1" ht="114.75">
       <c r="A73" s="18" t="s">
         <v>91</v>
       </c>
@@ -21371,7 +21374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="7" customFormat="1" ht="135">
+    <row r="74" spans="1:7" s="7" customFormat="1" ht="127.5">
       <c r="A74" s="18" t="s">
         <v>91</v>
       </c>
@@ -21394,7 +21397,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="7" customFormat="1" ht="30">
+    <row r="75" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A75" s="18" t="s">
         <v>91</v>
       </c>
@@ -21417,7 +21420,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="7" customFormat="1" ht="60">
+    <row r="76" spans="1:7" s="7" customFormat="1" ht="51">
       <c r="A76" s="18" t="s">
         <v>91</v>
       </c>
@@ -21440,7 +21443,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="7" customFormat="1" ht="150">
+    <row r="77" spans="1:7" s="7" customFormat="1" ht="127.5">
       <c r="A77" s="18" t="s">
         <v>91</v>
       </c>
@@ -21463,7 +21466,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="7" customFormat="1" ht="90">
+    <row r="78" spans="1:7" s="7" customFormat="1" ht="76.5">
       <c r="A78" s="18" t="s">
         <v>91</v>
       </c>
@@ -21486,7 +21489,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="7" customFormat="1" ht="180">
+    <row r="79" spans="1:7" s="7" customFormat="1" ht="153">
       <c r="A79" s="18" t="s">
         <v>91</v>
       </c>
@@ -21509,7 +21512,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="7" customFormat="1" ht="45">
+    <row r="80" spans="1:7" s="7" customFormat="1" ht="38.25">
       <c r="A80" s="18" t="s">
         <v>91</v>
       </c>
@@ -21532,7 +21535,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:1022" s="7" customFormat="1" ht="75">
+    <row r="81" spans="1:1022" s="7" customFormat="1" ht="63.75">
       <c r="A81" s="18" t="s">
         <v>91</v>
       </c>
@@ -21555,7 +21558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:1022" s="7" customFormat="1" ht="30">
+    <row r="82" spans="1:1022" s="7" customFormat="1" ht="25.5">
       <c r="A82" s="18" t="s">
         <v>91</v>
       </c>
@@ -21578,7 +21581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:1022" s="7" customFormat="1" ht="60">
+    <row r="83" spans="1:1022" s="7" customFormat="1" ht="51">
       <c r="A83" s="18" t="s">
         <v>91</v>
       </c>
@@ -21601,7 +21604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:1022" s="7" customFormat="1" ht="30">
+    <row r="84" spans="1:1022" s="7" customFormat="1" ht="25.5">
       <c r="A84" s="18" t="s">
         <v>91</v>
       </c>
@@ -21624,7 +21627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:1022" s="7" customFormat="1" ht="30">
+    <row r="85" spans="1:1022" s="7" customFormat="1" ht="25.5">
       <c r="A85" s="18" t="s">
         <v>91</v>
       </c>
@@ -21647,7 +21650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:1022" s="7" customFormat="1" ht="60">
+    <row r="86" spans="1:1022" s="7" customFormat="1" ht="51">
       <c r="A86" s="18" t="s">
         <v>91</v>
       </c>
@@ -21670,7 +21673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:1022" s="7" customFormat="1" ht="45">
+    <row r="87" spans="1:1022" s="7" customFormat="1" ht="38.25">
       <c r="A87" s="18" t="s">
         <v>91</v>
       </c>
@@ -21704,7 +21707,7 @@
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
     </row>
-    <row r="89" spans="1:1022" s="8" customFormat="1" ht="60">
+    <row r="89" spans="1:1022" s="8" customFormat="1" ht="51">
       <c r="A89" s="12" t="s">
         <v>34</v>
       </c>
@@ -22742,7 +22745,7 @@
       <c r="AMG89" s="5"/>
       <c r="AMH89" s="5"/>
     </row>
-    <row r="90" spans="1:1022" s="8" customFormat="1" ht="45">
+    <row r="90" spans="1:1022" s="8" customFormat="1" ht="51">
       <c r="A90" s="12" t="s">
         <v>34</v>
       </c>
@@ -23780,7 +23783,7 @@
       <c r="AMG90" s="5"/>
       <c r="AMH90" s="5"/>
     </row>
-    <row r="91" spans="1:1022" s="8" customFormat="1" ht="75">
+    <row r="91" spans="1:1022" s="8" customFormat="1" ht="63.75">
       <c r="A91" s="12" t="s">
         <v>228</v>
       </c>
@@ -23803,7 +23806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:1022" s="7" customFormat="1" ht="75">
+    <row r="92" spans="1:1022" s="7" customFormat="1" ht="63.75">
       <c r="A92" s="12" t="s">
         <v>228</v>
       </c>
@@ -23826,7 +23829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:1022" s="8" customFormat="1" ht="105">
+    <row r="93" spans="1:1022" s="8" customFormat="1" ht="89.25">
       <c r="A93" s="12" t="s">
         <v>91</v>
       </c>
@@ -23849,7 +23852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:1022" s="8" customFormat="1" ht="90">
+    <row r="94" spans="1:1022" s="8" customFormat="1" ht="76.5">
       <c r="A94" s="12" t="s">
         <v>91</v>
       </c>
@@ -23872,7 +23875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:1022" s="8" customFormat="1" ht="75">
+    <row r="95" spans="1:1022" s="8" customFormat="1" ht="63.75">
       <c r="A95" s="12" t="s">
         <v>91</v>
       </c>
@@ -23895,7 +23898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:1022" s="8" customFormat="1" ht="37.25" customHeight="1">
+    <row r="96" spans="1:1022" s="8" customFormat="1" ht="37.35" customHeight="1">
       <c r="A96" s="15"/>
       <c r="B96" s="30"/>
       <c r="C96" s="16"/>
@@ -23906,7 +23909,7 @@
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
     </row>
-    <row r="97" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="97" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A97" s="12" t="s">
         <v>91</v>
       </c>
@@ -23929,7 +23932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="8" customFormat="1" ht="45">
+    <row r="98" spans="1:7" s="8" customFormat="1" ht="38.25">
       <c r="A98" s="12" t="s">
         <v>228</v>
       </c>
@@ -23952,7 +23955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="8" customFormat="1" ht="60">
+    <row r="99" spans="1:7" s="8" customFormat="1" ht="51">
       <c r="A99" s="12" t="s">
         <v>224</v>
       </c>
@@ -23975,18 +23978,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="8" customFormat="1" ht="37.25" customHeight="1">
+    <row r="100" spans="1:7" s="8" customFormat="1" ht="37.35" customHeight="1">
       <c r="A100" s="41"/>
       <c r="B100" s="42"/>
       <c r="C100" s="43"/>
       <c r="D100" s="44"/>
       <c r="E100" s="45" t="s">
-        <v>631</v>
+        <v>619</v>
       </c>
       <c r="F100" s="41"/>
       <c r="G100" s="41"/>
     </row>
-    <row r="101" spans="1:7" ht="120">
+    <row r="101" spans="1:7" ht="102">
       <c r="A101" s="18" t="s">
         <v>65</v>
       </c>
@@ -23998,7 +24001,7 @@
       </c>
       <c r="D101" s="19"/>
       <c r="E101" s="19" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="F101" s="18" t="s">
         <v>32</v>
@@ -24007,7 +24010,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="120">
+    <row r="102" spans="1:7" ht="102">
       <c r="A102" s="18" t="s">
         <v>65</v>
       </c>
@@ -24019,7 +24022,7 @@
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="18" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
       <c r="F102" s="18" t="s">
         <v>32</v>
@@ -24028,7 +24031,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="120">
+    <row r="103" spans="1:7" ht="102">
       <c r="A103" s="18" t="s">
         <v>65</v>
       </c>
@@ -24039,7 +24042,7 @@
         <v>395</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
       <c r="F103" s="18" t="s">
         <v>32</v>
@@ -24048,7 +24051,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="120">
+    <row r="104" spans="1:7" ht="102">
       <c r="A104" s="18" t="s">
         <v>65</v>
       </c>
@@ -24059,7 +24062,7 @@
         <v>396</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
       <c r="F104" s="18" t="s">
         <v>32</v>
@@ -24068,7 +24071,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="120">
+    <row r="105" spans="1:7" ht="102">
       <c r="A105" s="18" t="s">
         <v>65</v>
       </c>
@@ -24079,7 +24082,7 @@
         <v>400</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
       <c r="F105" s="18" t="s">
         <v>17</v>
@@ -24088,7 +24091,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="105">
+    <row r="106" spans="1:7" ht="102">
       <c r="A106" s="18" t="s">
         <v>65</v>
       </c>
@@ -24099,7 +24102,7 @@
         <v>401</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
       <c r="F106" s="18" t="s">
         <v>17</v>
@@ -24108,7 +24111,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="120">
+    <row r="107" spans="1:7" ht="102">
       <c r="A107" s="18" t="s">
         <v>65</v>
       </c>
@@ -24119,7 +24122,7 @@
         <v>402</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="F107" s="18" t="s">
         <v>17</v>
@@ -24128,7 +24131,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="120">
+    <row r="108" spans="1:7" ht="102">
       <c r="A108" s="18" t="s">
         <v>65</v>
       </c>
@@ -24139,7 +24142,7 @@
         <v>403</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
       <c r="F108" s="18" t="s">
         <v>17</v>
@@ -24148,18 +24151,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="120">
+    <row r="109" spans="1:7" ht="102">
       <c r="A109" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
       <c r="C109" s="19" t="s">
         <v>413</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>32</v>
@@ -24168,7 +24171,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="409.6">
+    <row r="110" spans="1:7" ht="382.5">
       <c r="A110" s="18" t="s">
         <v>65</v>
       </c>
@@ -24188,12 +24191,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="135">
+    <row r="111" spans="1:7" ht="127.5">
       <c r="A111" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="C111" s="19" t="s">
         <v>415</v>
@@ -24208,12 +24211,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="120">
+    <row r="112" spans="1:7" ht="114.75">
       <c r="A112" s="18" t="s">
         <v>65</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="C112" s="19" t="s">
         <v>416</v>
@@ -24228,16 +24231,16 @@
         <v>522</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="120">
+    <row r="113" spans="1:7" ht="102">
       <c r="A113" s="18"/>
       <c r="B113" s="40" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="E113" s="40" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>32</v>
@@ -24246,18 +24249,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="409.6">
+    <row r="114" spans="1:7" ht="395.25">
       <c r="A114" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="C114" s="39" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="E114" s="40" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>32</v>
@@ -24266,18 +24269,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="150">
+    <row r="115" spans="1:7" ht="127.5">
       <c r="A115" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B115" s="40" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="C115" s="39" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="E115" s="40" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>32</v>
@@ -24286,18 +24289,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="135">
+    <row r="116" spans="1:7" ht="127.5">
       <c r="A116" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B116" s="40" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="E116" s="40" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>32</v>
@@ -24306,7 +24309,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="75">
+    <row r="117" spans="1:7" ht="51.75">
       <c r="A117" s="18" t="s">
         <v>65</v>
       </c>
@@ -24327,7 +24330,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="75">
+    <row r="118" spans="1:7" ht="51.75">
       <c r="A118" s="18" t="s">
         <v>65</v>
       </c>
@@ -24348,7 +24351,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="75">
+    <row r="119" spans="1:7" ht="51.75">
       <c r="A119" s="18" t="s">
         <v>65</v>
       </c>
@@ -24369,7 +24372,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="75">
+    <row r="120" spans="1:7" ht="51.75">
       <c r="A120" s="18" t="s">
         <v>65</v>
       </c>
@@ -24390,7 +24393,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="75">
+    <row r="121" spans="1:7" ht="51.75">
       <c r="A121" s="18" t="s">
         <v>65</v>
       </c>
@@ -24411,7 +24414,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="105">
+    <row r="122" spans="1:7" ht="90">
       <c r="A122" s="18" t="s">
         <v>65</v>
       </c>
@@ -24432,7 +24435,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="135">
+    <row r="123" spans="1:7" ht="115.5">
       <c r="A123" s="18" t="s">
         <v>65</v>
       </c>
@@ -24453,7 +24456,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="105">
+    <row r="124" spans="1:7" ht="90">
       <c r="A124" s="18" t="s">
         <v>65</v>
       </c>
@@ -24474,7 +24477,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="75">
+    <row r="125" spans="1:7" ht="51.75">
       <c r="A125" s="18" t="s">
         <v>65</v>
       </c>
@@ -24495,7 +24498,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="75">
+    <row r="126" spans="1:7" ht="64.5">
       <c r="A126" s="18" t="s">
         <v>65</v>
       </c>
@@ -24516,7 +24519,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="105">
+    <row r="127" spans="1:7" ht="90">
       <c r="A127" s="18" t="s">
         <v>65</v>
       </c>
@@ -24537,7 +24540,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="409.6">
+    <row r="128" spans="1:7" ht="383.25">
       <c r="A128" s="18" t="s">
         <v>65</v>
       </c>
@@ -24558,7 +24561,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="135">
+    <row r="129" spans="1:7" ht="115.5">
       <c r="A129" s="18" t="s">
         <v>65</v>
       </c>
@@ -24579,7 +24582,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="120">
+    <row r="130" spans="1:7" ht="102.75">
       <c r="A130" s="18" t="s">
         <v>65</v>
       </c>
@@ -24600,7 +24603,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="75">
+    <row r="131" spans="1:7" ht="64.5">
       <c r="A131" s="18" t="s">
         <v>65</v>
       </c>
@@ -24620,7 +24623,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="180">
+    <row r="132" spans="1:7" ht="166.5">
       <c r="A132" s="18" t="s">
         <v>65</v>
       </c>
@@ -24640,9 +24643,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="75">
+    <row r="133" spans="1:7" ht="64.5">
       <c r="A133" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>478</v>
@@ -24660,9 +24663,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="75">
+    <row r="134" spans="1:7" ht="51">
       <c r="A134" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>469</v>
@@ -24680,9 +24683,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="75">
+    <row r="135" spans="1:7" ht="64.5">
       <c r="A135" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>477</v>
@@ -24700,9 +24703,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="75">
+    <row r="136" spans="1:7" ht="51">
       <c r="A136" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>479</v>
@@ -24720,9 +24723,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="75">
+    <row r="137" spans="1:7" ht="51.75">
       <c r="A137" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>480</v>
@@ -24740,9 +24743,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="75">
+    <row r="138" spans="1:7" ht="51">
       <c r="A138" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>481</v>
@@ -24760,9 +24763,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="75">
+    <row r="139" spans="1:7" ht="51">
       <c r="A139" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>482</v>
@@ -24780,9 +24783,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="75">
+    <row r="140" spans="1:7" ht="51">
       <c r="A140" s="18" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>483</v>
@@ -24802,7 +24805,7 @@
     </row>
     <row r="141" spans="1:7" ht="409.6">
       <c r="A141" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>508</v>
@@ -24821,9 +24824,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="180">
+    <row r="142" spans="1:7" ht="153.75">
       <c r="A142" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>493</v>
@@ -24844,7 +24847,7 @@
     </row>
     <row r="143" spans="1:7" ht="409.6">
       <c r="A143" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>495</v>
@@ -24863,9 +24866,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="90">
+    <row r="144" spans="1:7" ht="77.25">
       <c r="A144" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>497</v>
@@ -24884,9 +24887,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="145" spans="1:1027" ht="409.6">
+    <row r="145" spans="1:1027" ht="383.25">
       <c r="A145" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>499</v>
@@ -24905,9 +24908,9 @@
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="1:1027" ht="240">
+    <row r="146" spans="1:1027" ht="204.75">
       <c r="A146" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>501</v>
@@ -24926,9 +24929,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:1027" ht="135">
+    <row r="147" spans="1:1027" ht="115.5">
       <c r="A147" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>503</v>
@@ -24947,9 +24950,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="148" spans="1:1027" ht="195">
+    <row r="148" spans="1:1027" ht="166.5">
       <c r="A148" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>510</v>
@@ -24968,9 +24971,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="149" spans="1:1027" ht="105">
+    <row r="149" spans="1:1027" ht="76.5">
       <c r="A149" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>509</v>
@@ -24989,30 +24992,30 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:1027" ht="45">
+    <row r="150" spans="1:1027" ht="38.25">
       <c r="A150" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G150" s="19" t="s">
-        <v>630</v>
+        <v>618</v>
       </c>
     </row>
-    <row r="151" spans="1:1027" ht="180">
+    <row r="151" spans="1:1027" ht="166.5">
       <c r="A151" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>507</v>
@@ -25031,9 +25034,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="152" spans="1:1027" ht="75">
+    <row r="152" spans="1:1027" ht="51">
       <c r="A152" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>525</v>
@@ -25051,9 +25054,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="153" spans="1:1027" ht="75">
+    <row r="153" spans="1:1027" ht="51">
       <c r="A153" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>527</v>
@@ -25071,9 +25074,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="154" spans="1:1027" ht="75">
+    <row r="154" spans="1:1027" ht="51">
       <c r="A154" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>529</v>
@@ -25091,9 +25094,9 @@
         <v>522</v>
       </c>
     </row>
-    <row r="155" spans="1:1027" ht="75">
+    <row r="155" spans="1:1027" ht="51">
       <c r="A155" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>531</v>
@@ -25111,14 +25114,16 @@
         <v>522</v>
       </c>
     </row>
-    <row r="156" spans="1:1027" s="52" customFormat="1">
+    <row r="156" spans="1:1027" s="52" customFormat="1" ht="26.25">
       <c r="A156" s="46"/>
       <c r="B156" s="47"/>
       <c r="C156" s="46"/>
       <c r="D156" s="48" t="s">
-        <v>613</v>
-      </c>
-      <c r="E156" s="47"/>
+        <v>601</v>
+      </c>
+      <c r="E156" s="46" t="s">
+        <v>649</v>
+      </c>
       <c r="F156" s="46"/>
       <c r="G156" s="49"/>
       <c r="H156" s="46"/>
@@ -26142,118 +26147,118 @@
       <c r="AML156" s="46"/>
       <c r="AMM156" s="46"/>
     </row>
-    <row r="157" spans="1:1027" ht="75">
+    <row r="157" spans="1:1027" ht="51.75">
       <c r="A157" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>642</v>
+        <v>630</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="E157" s="37" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G157" s="6" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
-    <row r="158" spans="1:1027" ht="75">
+    <row r="158" spans="1:1027" ht="51.75">
       <c r="A158" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>643</v>
+        <v>631</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>640</v>
+        <v>628</v>
       </c>
       <c r="E158" s="37" t="s">
-        <v>641</v>
+        <v>629</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G158" s="6" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
-    <row r="159" spans="1:1027" ht="30">
+    <row r="159" spans="1:1027" ht="26.25">
       <c r="A159" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>536</v>
+        <v>647</v>
       </c>
       <c r="E159" s="37" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G159" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="160" spans="1:1027" ht="30">
+    <row r="160" spans="1:1027" ht="26.25">
       <c r="A160" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>537</v>
+        <v>648</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G160" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="30">
+    <row r="161" spans="1:7" ht="26.25">
       <c r="A161" s="18" t="s">
         <v>228</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>538</v>
+        <v>637</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G161" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="75">
+    <row r="162" spans="1:7" ht="51">
       <c r="A162" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>539</v>
+        <v>638</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>8</v>
@@ -26262,18 +26267,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="120">
+    <row r="163" spans="1:7" ht="102.75">
       <c r="A163" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>540</v>
+        <v>639</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>32</v>
@@ -26282,18 +26287,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="75">
+    <row r="164" spans="1:7" ht="64.5">
       <c r="A164" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B164" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="E164" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="C164" s="6" t="s">
-        <v>541</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>566</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>32</v>
@@ -26302,18 +26307,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="120">
+    <row r="165" spans="1:7" ht="102.75">
       <c r="A165" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B165" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="E165" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="C165" s="6" t="s">
-        <v>542</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>567</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>8</v>
@@ -26322,18 +26327,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="75">
+    <row r="166" spans="1:7" ht="64.5">
       <c r="A166" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B166" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="E166" s="37" t="s">
         <v>556</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>543</v>
-      </c>
-      <c r="E166" s="37" t="s">
-        <v>568</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>32</v>
@@ -26342,18 +26347,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="90">
+    <row r="167" spans="1:7" ht="77.25">
       <c r="A167" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B167" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="E167" s="37" t="s">
         <v>557</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>544</v>
-      </c>
-      <c r="E167" s="37" t="s">
-        <v>569</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>8</v>
@@ -26362,18 +26367,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="120">
+    <row r="168" spans="1:7" ht="102.75">
       <c r="A168" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>571</v>
+        <v>559</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>545</v>
+        <v>644</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>8</v>
@@ -26382,18 +26387,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="75">
+    <row r="169" spans="1:7" ht="64.5">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>558</v>
+        <v>546</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>546</v>
+        <v>645</v>
       </c>
       <c r="E169" s="37" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>32</v>
@@ -26402,18 +26407,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="75">
+    <row r="170" spans="1:7" ht="64.5">
       <c r="A170" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>547</v>
+        <v>646</v>
       </c>
       <c r="E170" s="37" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>32</v>
@@ -26422,164 +26427,164 @@
         <v>522</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="60">
+    <row r="171" spans="1:7" ht="51.75">
       <c r="A171" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="E171" s="37" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G171" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="75">
+    <row r="172" spans="1:7" ht="64.5">
       <c r="A172" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="E172" s="37" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G172" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="75">
+    <row r="173" spans="1:7" ht="64.5">
       <c r="A173" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="E173" s="37" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G173" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="60">
+    <row r="174" spans="1:7" ht="51.75">
       <c r="A174" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>597</v>
+        <v>585</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
       <c r="E174" s="37" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G174" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="60">
+    <row r="175" spans="1:7" ht="51.75">
       <c r="A175" s="1" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
       <c r="E175" s="37" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="75">
+    <row r="176" spans="1:7" ht="64.5">
       <c r="A176" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="E176" s="37" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G176" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="105">
+    <row r="177" spans="1:7" ht="90">
       <c r="A177" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="E177" s="37" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G177" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="75">
+    <row r="178" spans="1:7" ht="64.5">
       <c r="A178" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="E178" s="37" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G178" s="6" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
non tags first, fixed Ppother in excl
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27393D6-4C32-4731-872B-B0F270C9DC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EC6CFE-B4BD-4660-AC9A-09DDD38903EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18392,9 +18392,6 @@
     </r>
   </si>
   <si>
-    <t>Ppother</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Following Biber (1988), all occurrences of </t>
     </r>
@@ -18663,6 +18660,9 @@
   </si>
   <si>
     <t>The tags consist of aggregates of individual tags. To avoid false correlation, skew etc. in the data, they should not be used in combination with the tags they are made of.</t>
+  </si>
+  <si>
+    <t>PPother</t>
   </si>
 </sst>
 </file>
@@ -19696,8 +19696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15"/>
@@ -19845,7 +19845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" ht="102">
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="114.75">
       <c r="A7" s="12" t="s">
         <v>284</v>
       </c>
@@ -20238,7 +20238,7 @@
         <v>239</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>32</v>
@@ -20721,7 +20721,7 @@
         <v>135</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>32</v>
@@ -20761,7 +20761,7 @@
         <v>632</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>634</v>
+        <v>649</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>133</v>
@@ -25122,7 +25122,7 @@
         <v>601</v>
       </c>
       <c r="E156" s="46" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F156" s="46"/>
       <c r="G156" s="49"/>
@@ -26195,7 +26195,7 @@
         <v>614</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E159" s="37" t="s">
         <v>548</v>
@@ -26215,7 +26215,7 @@
         <v>539</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>549</v>
@@ -26235,7 +26235,7 @@
         <v>541</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>550</v>
@@ -26255,7 +26255,7 @@
         <v>540</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>551</v>
@@ -26275,7 +26275,7 @@
         <v>552</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>553</v>
@@ -26295,7 +26295,7 @@
         <v>542</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>554</v>
@@ -26315,7 +26315,7 @@
         <v>543</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>555</v>
@@ -26335,7 +26335,7 @@
         <v>544</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E166" s="37" t="s">
         <v>556</v>
@@ -26355,7 +26355,7 @@
         <v>545</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E167" s="37" t="s">
         <v>557</v>
@@ -26375,7 +26375,7 @@
         <v>559</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>558</v>
@@ -26395,7 +26395,7 @@
         <v>546</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E169" s="37" t="s">
         <v>560</v>
@@ -26415,7 +26415,7 @@
         <v>547</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E170" s="37" t="s">
         <v>561</v>

</xml_diff>

<commit_message>
Tidied up comments in script, corrected minor errors
Updated SUPER and COMPAR in table of counts
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Downloads/MFTE-master 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4283B6B-87F7-6D44-8850-81DFDB8F6B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0984A10-4D21-E047-A705-48FB44FC5D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4900" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18803,6 +18803,137 @@
   </si>
   <si>
     <r>
+      <t>All adjectives and adverbs ending in "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>est"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> except </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">honest, test, west, pest, lest </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> guest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, as well as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">worst </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">best </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">followed by a hypthen. Also constructions of the type: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the least/most </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ ADJ/ADV.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">All adjectives and adverbs ending in "er" except </t>
     </r>
     <r>
@@ -18887,117 +19018,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>followed by a hypthen.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>All adjectives and adverbs ending in "</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>est"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> except </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">honest, test, west, pest, lest </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> guest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, as well as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">worst </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">best </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>followed by a hypthen.</t>
+      <t xml:space="preserve">followed by a hypthen. Also constructions of the type: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">more/less </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ ADJ/ADV.</t>
     </r>
   </si>
 </sst>
@@ -19302,7 +19344,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -19445,16 +19487,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -20011,7 +20052,7 @@
   <dimension ref="A1:AMM180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
@@ -28383,51 +28424,2091 @@
       <c r="AML100" s="6"/>
       <c r="AMM100" s="6"/>
     </row>
-    <row r="101" spans="1:1027" s="43" customFormat="1" ht="37.25" customHeight="1">
-      <c r="A101" s="44" t="s">
+    <row r="101" spans="1:1027" ht="37.25" customHeight="1">
+      <c r="A101" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="B101" s="44" t="s">
+      <c r="B101" s="43" t="s">
         <v>650</v>
       </c>
-      <c r="C101" s="45" t="s">
+      <c r="C101" s="44" t="s">
         <v>652</v>
       </c>
-      <c r="D101" s="46" t="s">
+      <c r="D101" s="45" t="s">
         <v>655</v>
       </c>
       <c r="E101" s="14" t="s">
+        <v>656</v>
+      </c>
+      <c r="F101" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G101" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
+      <c r="O101" s="6"/>
+      <c r="P101" s="6"/>
+      <c r="Q101" s="6"/>
+      <c r="R101" s="6"/>
+      <c r="S101" s="6"/>
+      <c r="T101" s="6"/>
+      <c r="U101" s="6"/>
+      <c r="V101" s="6"/>
+      <c r="W101" s="6"/>
+      <c r="X101" s="6"/>
+      <c r="Y101" s="6"/>
+      <c r="Z101" s="6"/>
+      <c r="AA101" s="6"/>
+      <c r="AB101" s="6"/>
+      <c r="AC101" s="6"/>
+      <c r="AD101" s="6"/>
+      <c r="AE101" s="6"/>
+      <c r="AF101" s="6"/>
+      <c r="AG101" s="6"/>
+      <c r="AH101" s="6"/>
+      <c r="AI101" s="6"/>
+      <c r="AJ101" s="6"/>
+      <c r="AK101" s="6"/>
+      <c r="AL101" s="6"/>
+      <c r="AM101" s="6"/>
+      <c r="AN101" s="6"/>
+      <c r="AO101" s="6"/>
+      <c r="AP101" s="6"/>
+      <c r="AQ101" s="6"/>
+      <c r="AR101" s="6"/>
+      <c r="AS101" s="6"/>
+      <c r="AT101" s="6"/>
+      <c r="AU101" s="6"/>
+      <c r="AV101" s="6"/>
+      <c r="AW101" s="6"/>
+      <c r="AX101" s="6"/>
+      <c r="AY101" s="6"/>
+      <c r="AZ101" s="6"/>
+      <c r="BA101" s="6"/>
+      <c r="BB101" s="6"/>
+      <c r="BC101" s="6"/>
+      <c r="BD101" s="6"/>
+      <c r="BE101" s="6"/>
+      <c r="BF101" s="6"/>
+      <c r="BG101" s="6"/>
+      <c r="BH101" s="6"/>
+      <c r="BI101" s="6"/>
+      <c r="BJ101" s="6"/>
+      <c r="BK101" s="6"/>
+      <c r="BL101" s="6"/>
+      <c r="BM101" s="6"/>
+      <c r="BN101" s="6"/>
+      <c r="BO101" s="6"/>
+      <c r="BP101" s="6"/>
+      <c r="BQ101" s="6"/>
+      <c r="BR101" s="6"/>
+      <c r="BS101" s="6"/>
+      <c r="BT101" s="6"/>
+      <c r="BU101" s="6"/>
+      <c r="BV101" s="6"/>
+      <c r="BW101" s="6"/>
+      <c r="BX101" s="6"/>
+      <c r="BY101" s="6"/>
+      <c r="BZ101" s="6"/>
+      <c r="CA101" s="6"/>
+      <c r="CB101" s="6"/>
+      <c r="CC101" s="6"/>
+      <c r="CD101" s="6"/>
+      <c r="CE101" s="6"/>
+      <c r="CF101" s="6"/>
+      <c r="CG101" s="6"/>
+      <c r="CH101" s="6"/>
+      <c r="CI101" s="6"/>
+      <c r="CJ101" s="6"/>
+      <c r="CK101" s="6"/>
+      <c r="CL101" s="6"/>
+      <c r="CM101" s="6"/>
+      <c r="CN101" s="6"/>
+      <c r="CO101" s="6"/>
+      <c r="CP101" s="6"/>
+      <c r="CQ101" s="6"/>
+      <c r="CR101" s="6"/>
+      <c r="CS101" s="6"/>
+      <c r="CT101" s="6"/>
+      <c r="CU101" s="6"/>
+      <c r="CV101" s="6"/>
+      <c r="CW101" s="6"/>
+      <c r="CX101" s="6"/>
+      <c r="CY101" s="6"/>
+      <c r="CZ101" s="6"/>
+      <c r="DA101" s="6"/>
+      <c r="DB101" s="6"/>
+      <c r="DC101" s="6"/>
+      <c r="DD101" s="6"/>
+      <c r="DE101" s="6"/>
+      <c r="DF101" s="6"/>
+      <c r="DG101" s="6"/>
+      <c r="DH101" s="6"/>
+      <c r="DI101" s="6"/>
+      <c r="DJ101" s="6"/>
+      <c r="DK101" s="6"/>
+      <c r="DL101" s="6"/>
+      <c r="DM101" s="6"/>
+      <c r="DN101" s="6"/>
+      <c r="DO101" s="6"/>
+      <c r="DP101" s="6"/>
+      <c r="DQ101" s="6"/>
+      <c r="DR101" s="6"/>
+      <c r="DS101" s="6"/>
+      <c r="DT101" s="6"/>
+      <c r="DU101" s="6"/>
+      <c r="DV101" s="6"/>
+      <c r="DW101" s="6"/>
+      <c r="DX101" s="6"/>
+      <c r="DY101" s="6"/>
+      <c r="DZ101" s="6"/>
+      <c r="EA101" s="6"/>
+      <c r="EB101" s="6"/>
+      <c r="EC101" s="6"/>
+      <c r="ED101" s="6"/>
+      <c r="EE101" s="6"/>
+      <c r="EF101" s="6"/>
+      <c r="EG101" s="6"/>
+      <c r="EH101" s="6"/>
+      <c r="EI101" s="6"/>
+      <c r="EJ101" s="6"/>
+      <c r="EK101" s="6"/>
+      <c r="EL101" s="6"/>
+      <c r="EM101" s="6"/>
+      <c r="EN101" s="6"/>
+      <c r="EO101" s="6"/>
+      <c r="EP101" s="6"/>
+      <c r="EQ101" s="6"/>
+      <c r="ER101" s="6"/>
+      <c r="ES101" s="6"/>
+      <c r="ET101" s="6"/>
+      <c r="EU101" s="6"/>
+      <c r="EV101" s="6"/>
+      <c r="EW101" s="6"/>
+      <c r="EX101" s="6"/>
+      <c r="EY101" s="6"/>
+      <c r="EZ101" s="6"/>
+      <c r="FA101" s="6"/>
+      <c r="FB101" s="6"/>
+      <c r="FC101" s="6"/>
+      <c r="FD101" s="6"/>
+      <c r="FE101" s="6"/>
+      <c r="FF101" s="6"/>
+      <c r="FG101" s="6"/>
+      <c r="FH101" s="6"/>
+      <c r="FI101" s="6"/>
+      <c r="FJ101" s="6"/>
+      <c r="FK101" s="6"/>
+      <c r="FL101" s="6"/>
+      <c r="FM101" s="6"/>
+      <c r="FN101" s="6"/>
+      <c r="FO101" s="6"/>
+      <c r="FP101" s="6"/>
+      <c r="FQ101" s="6"/>
+      <c r="FR101" s="6"/>
+      <c r="FS101" s="6"/>
+      <c r="FT101" s="6"/>
+      <c r="FU101" s="6"/>
+      <c r="FV101" s="6"/>
+      <c r="FW101" s="6"/>
+      <c r="FX101" s="6"/>
+      <c r="FY101" s="6"/>
+      <c r="FZ101" s="6"/>
+      <c r="GA101" s="6"/>
+      <c r="GB101" s="6"/>
+      <c r="GC101" s="6"/>
+      <c r="GD101" s="6"/>
+      <c r="GE101" s="6"/>
+      <c r="GF101" s="6"/>
+      <c r="GG101" s="6"/>
+      <c r="GH101" s="6"/>
+      <c r="GI101" s="6"/>
+      <c r="GJ101" s="6"/>
+      <c r="GK101" s="6"/>
+      <c r="GL101" s="6"/>
+      <c r="GM101" s="6"/>
+      <c r="GN101" s="6"/>
+      <c r="GO101" s="6"/>
+      <c r="GP101" s="6"/>
+      <c r="GQ101" s="6"/>
+      <c r="GR101" s="6"/>
+      <c r="GS101" s="6"/>
+      <c r="GT101" s="6"/>
+      <c r="GU101" s="6"/>
+      <c r="GV101" s="6"/>
+      <c r="GW101" s="6"/>
+      <c r="GX101" s="6"/>
+      <c r="GY101" s="6"/>
+      <c r="GZ101" s="6"/>
+      <c r="HA101" s="6"/>
+      <c r="HB101" s="6"/>
+      <c r="HC101" s="6"/>
+      <c r="HD101" s="6"/>
+      <c r="HE101" s="6"/>
+      <c r="HF101" s="6"/>
+      <c r="HG101" s="6"/>
+      <c r="HH101" s="6"/>
+      <c r="HI101" s="6"/>
+      <c r="HJ101" s="6"/>
+      <c r="HK101" s="6"/>
+      <c r="HL101" s="6"/>
+      <c r="HM101" s="6"/>
+      <c r="HN101" s="6"/>
+      <c r="HO101" s="6"/>
+      <c r="HP101" s="6"/>
+      <c r="HQ101" s="6"/>
+      <c r="HR101" s="6"/>
+      <c r="HS101" s="6"/>
+      <c r="HT101" s="6"/>
+      <c r="HU101" s="6"/>
+      <c r="HV101" s="6"/>
+      <c r="HW101" s="6"/>
+      <c r="HX101" s="6"/>
+      <c r="HY101" s="6"/>
+      <c r="HZ101" s="6"/>
+      <c r="IA101" s="6"/>
+      <c r="IB101" s="6"/>
+      <c r="IC101" s="6"/>
+      <c r="ID101" s="6"/>
+      <c r="IE101" s="6"/>
+      <c r="IF101" s="6"/>
+      <c r="IG101" s="6"/>
+      <c r="IH101" s="6"/>
+      <c r="II101" s="6"/>
+      <c r="IJ101" s="6"/>
+      <c r="IK101" s="6"/>
+      <c r="IL101" s="6"/>
+      <c r="IM101" s="6"/>
+      <c r="IN101" s="6"/>
+      <c r="IO101" s="6"/>
+      <c r="IP101" s="6"/>
+      <c r="IQ101" s="6"/>
+      <c r="IR101" s="6"/>
+      <c r="IS101" s="6"/>
+      <c r="IT101" s="6"/>
+      <c r="IU101" s="6"/>
+      <c r="IV101" s="6"/>
+      <c r="IW101" s="6"/>
+      <c r="IX101" s="6"/>
+      <c r="IY101" s="6"/>
+      <c r="IZ101" s="6"/>
+      <c r="JA101" s="6"/>
+      <c r="JB101" s="6"/>
+      <c r="JC101" s="6"/>
+      <c r="JD101" s="6"/>
+      <c r="JE101" s="6"/>
+      <c r="JF101" s="6"/>
+      <c r="JG101" s="6"/>
+      <c r="JH101" s="6"/>
+      <c r="JI101" s="6"/>
+      <c r="JJ101" s="6"/>
+      <c r="JK101" s="6"/>
+      <c r="JL101" s="6"/>
+      <c r="JM101" s="6"/>
+      <c r="JN101" s="6"/>
+      <c r="JO101" s="6"/>
+      <c r="JP101" s="6"/>
+      <c r="JQ101" s="6"/>
+      <c r="JR101" s="6"/>
+      <c r="JS101" s="6"/>
+      <c r="JT101" s="6"/>
+      <c r="JU101" s="6"/>
+      <c r="JV101" s="6"/>
+      <c r="JW101" s="6"/>
+      <c r="JX101" s="6"/>
+      <c r="JY101" s="6"/>
+      <c r="JZ101" s="6"/>
+      <c r="KA101" s="6"/>
+      <c r="KB101" s="6"/>
+      <c r="KC101" s="6"/>
+      <c r="KD101" s="6"/>
+      <c r="KE101" s="6"/>
+      <c r="KF101" s="6"/>
+      <c r="KG101" s="6"/>
+      <c r="KH101" s="6"/>
+      <c r="KI101" s="6"/>
+      <c r="KJ101" s="6"/>
+      <c r="KK101" s="6"/>
+      <c r="KL101" s="6"/>
+      <c r="KM101" s="6"/>
+      <c r="KN101" s="6"/>
+      <c r="KO101" s="6"/>
+      <c r="KP101" s="6"/>
+      <c r="KQ101" s="6"/>
+      <c r="KR101" s="6"/>
+      <c r="KS101" s="6"/>
+      <c r="KT101" s="6"/>
+      <c r="KU101" s="6"/>
+      <c r="KV101" s="6"/>
+      <c r="KW101" s="6"/>
+      <c r="KX101" s="6"/>
+      <c r="KY101" s="6"/>
+      <c r="KZ101" s="6"/>
+      <c r="LA101" s="6"/>
+      <c r="LB101" s="6"/>
+      <c r="LC101" s="6"/>
+      <c r="LD101" s="6"/>
+      <c r="LE101" s="6"/>
+      <c r="LF101" s="6"/>
+      <c r="LG101" s="6"/>
+      <c r="LH101" s="6"/>
+      <c r="LI101" s="6"/>
+      <c r="LJ101" s="6"/>
+      <c r="LK101" s="6"/>
+      <c r="LL101" s="6"/>
+      <c r="LM101" s="6"/>
+      <c r="LN101" s="6"/>
+      <c r="LO101" s="6"/>
+      <c r="LP101" s="6"/>
+      <c r="LQ101" s="6"/>
+      <c r="LR101" s="6"/>
+      <c r="LS101" s="6"/>
+      <c r="LT101" s="6"/>
+      <c r="LU101" s="6"/>
+      <c r="LV101" s="6"/>
+      <c r="LW101" s="6"/>
+      <c r="LX101" s="6"/>
+      <c r="LY101" s="6"/>
+      <c r="LZ101" s="6"/>
+      <c r="MA101" s="6"/>
+      <c r="MB101" s="6"/>
+      <c r="MC101" s="6"/>
+      <c r="MD101" s="6"/>
+      <c r="ME101" s="6"/>
+      <c r="MF101" s="6"/>
+      <c r="MG101" s="6"/>
+      <c r="MH101" s="6"/>
+      <c r="MI101" s="6"/>
+      <c r="MJ101" s="6"/>
+      <c r="MK101" s="6"/>
+      <c r="ML101" s="6"/>
+      <c r="MM101" s="6"/>
+      <c r="MN101" s="6"/>
+      <c r="MO101" s="6"/>
+      <c r="MP101" s="6"/>
+      <c r="MQ101" s="6"/>
+      <c r="MR101" s="6"/>
+      <c r="MS101" s="6"/>
+      <c r="MT101" s="6"/>
+      <c r="MU101" s="6"/>
+      <c r="MV101" s="6"/>
+      <c r="MW101" s="6"/>
+      <c r="MX101" s="6"/>
+      <c r="MY101" s="6"/>
+      <c r="MZ101" s="6"/>
+      <c r="NA101" s="6"/>
+      <c r="NB101" s="6"/>
+      <c r="NC101" s="6"/>
+      <c r="ND101" s="6"/>
+      <c r="NE101" s="6"/>
+      <c r="NF101" s="6"/>
+      <c r="NG101" s="6"/>
+      <c r="NH101" s="6"/>
+      <c r="NI101" s="6"/>
+      <c r="NJ101" s="6"/>
+      <c r="NK101" s="6"/>
+      <c r="NL101" s="6"/>
+      <c r="NM101" s="6"/>
+      <c r="NN101" s="6"/>
+      <c r="NO101" s="6"/>
+      <c r="NP101" s="6"/>
+      <c r="NQ101" s="6"/>
+      <c r="NR101" s="6"/>
+      <c r="NS101" s="6"/>
+      <c r="NT101" s="6"/>
+      <c r="NU101" s="6"/>
+      <c r="NV101" s="6"/>
+      <c r="NW101" s="6"/>
+      <c r="NX101" s="6"/>
+      <c r="NY101" s="6"/>
+      <c r="NZ101" s="6"/>
+      <c r="OA101" s="6"/>
+      <c r="OB101" s="6"/>
+      <c r="OC101" s="6"/>
+      <c r="OD101" s="6"/>
+      <c r="OE101" s="6"/>
+      <c r="OF101" s="6"/>
+      <c r="OG101" s="6"/>
+      <c r="OH101" s="6"/>
+      <c r="OI101" s="6"/>
+      <c r="OJ101" s="6"/>
+      <c r="OK101" s="6"/>
+      <c r="OL101" s="6"/>
+      <c r="OM101" s="6"/>
+      <c r="ON101" s="6"/>
+      <c r="OO101" s="6"/>
+      <c r="OP101" s="6"/>
+      <c r="OQ101" s="6"/>
+      <c r="OR101" s="6"/>
+      <c r="OS101" s="6"/>
+      <c r="OT101" s="6"/>
+      <c r="OU101" s="6"/>
+      <c r="OV101" s="6"/>
+      <c r="OW101" s="6"/>
+      <c r="OX101" s="6"/>
+      <c r="OY101" s="6"/>
+      <c r="OZ101" s="6"/>
+      <c r="PA101" s="6"/>
+      <c r="PB101" s="6"/>
+      <c r="PC101" s="6"/>
+      <c r="PD101" s="6"/>
+      <c r="PE101" s="6"/>
+      <c r="PF101" s="6"/>
+      <c r="PG101" s="6"/>
+      <c r="PH101" s="6"/>
+      <c r="PI101" s="6"/>
+      <c r="PJ101" s="6"/>
+      <c r="PK101" s="6"/>
+      <c r="PL101" s="6"/>
+      <c r="PM101" s="6"/>
+      <c r="PN101" s="6"/>
+      <c r="PO101" s="6"/>
+      <c r="PP101" s="6"/>
+      <c r="PQ101" s="6"/>
+      <c r="PR101" s="6"/>
+      <c r="PS101" s="6"/>
+      <c r="PT101" s="6"/>
+      <c r="PU101" s="6"/>
+      <c r="PV101" s="6"/>
+      <c r="PW101" s="6"/>
+      <c r="PX101" s="6"/>
+      <c r="PY101" s="6"/>
+      <c r="PZ101" s="6"/>
+      <c r="QA101" s="6"/>
+      <c r="QB101" s="6"/>
+      <c r="QC101" s="6"/>
+      <c r="QD101" s="6"/>
+      <c r="QE101" s="6"/>
+      <c r="QF101" s="6"/>
+      <c r="QG101" s="6"/>
+      <c r="QH101" s="6"/>
+      <c r="QI101" s="6"/>
+      <c r="QJ101" s="6"/>
+      <c r="QK101" s="6"/>
+      <c r="QL101" s="6"/>
+      <c r="QM101" s="6"/>
+      <c r="QN101" s="6"/>
+      <c r="QO101" s="6"/>
+      <c r="QP101" s="6"/>
+      <c r="QQ101" s="6"/>
+      <c r="QR101" s="6"/>
+      <c r="QS101" s="6"/>
+      <c r="QT101" s="6"/>
+      <c r="QU101" s="6"/>
+      <c r="QV101" s="6"/>
+      <c r="QW101" s="6"/>
+      <c r="QX101" s="6"/>
+      <c r="QY101" s="6"/>
+      <c r="QZ101" s="6"/>
+      <c r="RA101" s="6"/>
+      <c r="RB101" s="6"/>
+      <c r="RC101" s="6"/>
+      <c r="RD101" s="6"/>
+      <c r="RE101" s="6"/>
+      <c r="RF101" s="6"/>
+      <c r="RG101" s="6"/>
+      <c r="RH101" s="6"/>
+      <c r="RI101" s="6"/>
+      <c r="RJ101" s="6"/>
+      <c r="RK101" s="6"/>
+      <c r="RL101" s="6"/>
+      <c r="RM101" s="6"/>
+      <c r="RN101" s="6"/>
+      <c r="RO101" s="6"/>
+      <c r="RP101" s="6"/>
+      <c r="RQ101" s="6"/>
+      <c r="RR101" s="6"/>
+      <c r="RS101" s="6"/>
+      <c r="RT101" s="6"/>
+      <c r="RU101" s="6"/>
+      <c r="RV101" s="6"/>
+      <c r="RW101" s="6"/>
+      <c r="RX101" s="6"/>
+      <c r="RY101" s="6"/>
+      <c r="RZ101" s="6"/>
+      <c r="SA101" s="6"/>
+      <c r="SB101" s="6"/>
+      <c r="SC101" s="6"/>
+      <c r="SD101" s="6"/>
+      <c r="SE101" s="6"/>
+      <c r="SF101" s="6"/>
+      <c r="SG101" s="6"/>
+      <c r="SH101" s="6"/>
+      <c r="SI101" s="6"/>
+      <c r="SJ101" s="6"/>
+      <c r="SK101" s="6"/>
+      <c r="SL101" s="6"/>
+      <c r="SM101" s="6"/>
+      <c r="SN101" s="6"/>
+      <c r="SO101" s="6"/>
+      <c r="SP101" s="6"/>
+      <c r="SQ101" s="6"/>
+      <c r="SR101" s="6"/>
+      <c r="SS101" s="6"/>
+      <c r="ST101" s="6"/>
+      <c r="SU101" s="6"/>
+      <c r="SV101" s="6"/>
+      <c r="SW101" s="6"/>
+      <c r="SX101" s="6"/>
+      <c r="SY101" s="6"/>
+      <c r="SZ101" s="6"/>
+      <c r="TA101" s="6"/>
+      <c r="TB101" s="6"/>
+      <c r="TC101" s="6"/>
+      <c r="TD101" s="6"/>
+      <c r="TE101" s="6"/>
+      <c r="TF101" s="6"/>
+      <c r="TG101" s="6"/>
+      <c r="TH101" s="6"/>
+      <c r="TI101" s="6"/>
+      <c r="TJ101" s="6"/>
+      <c r="TK101" s="6"/>
+      <c r="TL101" s="6"/>
+      <c r="TM101" s="6"/>
+      <c r="TN101" s="6"/>
+      <c r="TO101" s="6"/>
+      <c r="TP101" s="6"/>
+      <c r="TQ101" s="6"/>
+      <c r="TR101" s="6"/>
+      <c r="TS101" s="6"/>
+      <c r="TT101" s="6"/>
+      <c r="TU101" s="6"/>
+      <c r="TV101" s="6"/>
+      <c r="TW101" s="6"/>
+      <c r="TX101" s="6"/>
+      <c r="TY101" s="6"/>
+      <c r="TZ101" s="6"/>
+      <c r="UA101" s="6"/>
+      <c r="UB101" s="6"/>
+      <c r="UC101" s="6"/>
+      <c r="UD101" s="6"/>
+      <c r="UE101" s="6"/>
+      <c r="UF101" s="6"/>
+      <c r="UG101" s="6"/>
+      <c r="UH101" s="6"/>
+      <c r="UI101" s="6"/>
+      <c r="UJ101" s="6"/>
+      <c r="UK101" s="6"/>
+      <c r="UL101" s="6"/>
+      <c r="UM101" s="6"/>
+      <c r="UN101" s="6"/>
+      <c r="UO101" s="6"/>
+      <c r="UP101" s="6"/>
+      <c r="UQ101" s="6"/>
+      <c r="UR101" s="6"/>
+      <c r="US101" s="6"/>
+      <c r="UT101" s="6"/>
+      <c r="UU101" s="6"/>
+      <c r="UV101" s="6"/>
+      <c r="UW101" s="6"/>
+      <c r="UX101" s="6"/>
+      <c r="UY101" s="6"/>
+      <c r="UZ101" s="6"/>
+      <c r="VA101" s="6"/>
+      <c r="VB101" s="6"/>
+      <c r="VC101" s="6"/>
+      <c r="VD101" s="6"/>
+      <c r="VE101" s="6"/>
+      <c r="VF101" s="6"/>
+      <c r="VG101" s="6"/>
+      <c r="VH101" s="6"/>
+      <c r="VI101" s="6"/>
+      <c r="VJ101" s="6"/>
+      <c r="VK101" s="6"/>
+      <c r="VL101" s="6"/>
+      <c r="VM101" s="6"/>
+      <c r="VN101" s="6"/>
+      <c r="VO101" s="6"/>
+      <c r="VP101" s="6"/>
+      <c r="VQ101" s="6"/>
+      <c r="VR101" s="6"/>
+      <c r="VS101" s="6"/>
+      <c r="VT101" s="6"/>
+      <c r="VU101" s="6"/>
+      <c r="VV101" s="6"/>
+      <c r="VW101" s="6"/>
+      <c r="VX101" s="6"/>
+      <c r="VY101" s="6"/>
+      <c r="VZ101" s="6"/>
+      <c r="WA101" s="6"/>
+      <c r="WB101" s="6"/>
+      <c r="WC101" s="6"/>
+      <c r="WD101" s="6"/>
+      <c r="WE101" s="6"/>
+      <c r="WF101" s="6"/>
+      <c r="WG101" s="6"/>
+      <c r="WH101" s="6"/>
+      <c r="WI101" s="6"/>
+      <c r="WJ101" s="6"/>
+      <c r="WK101" s="6"/>
+      <c r="WL101" s="6"/>
+      <c r="WM101" s="6"/>
+      <c r="WN101" s="6"/>
+      <c r="WO101" s="6"/>
+      <c r="WP101" s="6"/>
+      <c r="WQ101" s="6"/>
+      <c r="WR101" s="6"/>
+      <c r="WS101" s="6"/>
+      <c r="WT101" s="6"/>
+      <c r="WU101" s="6"/>
+      <c r="WV101" s="6"/>
+      <c r="WW101" s="6"/>
+      <c r="WX101" s="6"/>
+      <c r="WY101" s="6"/>
+      <c r="WZ101" s="6"/>
+      <c r="XA101" s="6"/>
+      <c r="XB101" s="6"/>
+      <c r="XC101" s="6"/>
+      <c r="XD101" s="6"/>
+      <c r="XE101" s="6"/>
+      <c r="XF101" s="6"/>
+      <c r="XG101" s="6"/>
+      <c r="XH101" s="6"/>
+      <c r="XI101" s="6"/>
+      <c r="XJ101" s="6"/>
+      <c r="XK101" s="6"/>
+      <c r="XL101" s="6"/>
+      <c r="XM101" s="6"/>
+      <c r="XN101" s="6"/>
+      <c r="XO101" s="6"/>
+      <c r="XP101" s="6"/>
+      <c r="XQ101" s="6"/>
+      <c r="XR101" s="6"/>
+      <c r="XS101" s="6"/>
+      <c r="XT101" s="6"/>
+      <c r="XU101" s="6"/>
+      <c r="XV101" s="6"/>
+      <c r="XW101" s="6"/>
+      <c r="XX101" s="6"/>
+      <c r="XY101" s="6"/>
+      <c r="XZ101" s="6"/>
+      <c r="YA101" s="6"/>
+      <c r="YB101" s="6"/>
+      <c r="YC101" s="6"/>
+      <c r="YD101" s="6"/>
+      <c r="YE101" s="6"/>
+      <c r="YF101" s="6"/>
+      <c r="YG101" s="6"/>
+      <c r="YH101" s="6"/>
+      <c r="YI101" s="6"/>
+      <c r="YJ101" s="6"/>
+      <c r="YK101" s="6"/>
+      <c r="YL101" s="6"/>
+      <c r="YM101" s="6"/>
+      <c r="YN101" s="6"/>
+      <c r="YO101" s="6"/>
+      <c r="YP101" s="6"/>
+      <c r="YQ101" s="6"/>
+      <c r="YR101" s="6"/>
+      <c r="YS101" s="6"/>
+      <c r="YT101" s="6"/>
+      <c r="YU101" s="6"/>
+      <c r="YV101" s="6"/>
+      <c r="YW101" s="6"/>
+      <c r="YX101" s="6"/>
+      <c r="YY101" s="6"/>
+      <c r="YZ101" s="6"/>
+      <c r="ZA101" s="6"/>
+      <c r="ZB101" s="6"/>
+      <c r="ZC101" s="6"/>
+      <c r="ZD101" s="6"/>
+      <c r="ZE101" s="6"/>
+      <c r="ZF101" s="6"/>
+      <c r="ZG101" s="6"/>
+      <c r="ZH101" s="6"/>
+      <c r="ZI101" s="6"/>
+      <c r="ZJ101" s="6"/>
+      <c r="ZK101" s="6"/>
+      <c r="ZL101" s="6"/>
+      <c r="ZM101" s="6"/>
+      <c r="ZN101" s="6"/>
+      <c r="ZO101" s="6"/>
+      <c r="ZP101" s="6"/>
+      <c r="ZQ101" s="6"/>
+      <c r="ZR101" s="6"/>
+      <c r="ZS101" s="6"/>
+      <c r="ZT101" s="6"/>
+      <c r="ZU101" s="6"/>
+      <c r="ZV101" s="6"/>
+      <c r="ZW101" s="6"/>
+      <c r="ZX101" s="6"/>
+      <c r="ZY101" s="6"/>
+      <c r="ZZ101" s="6"/>
+      <c r="AAA101" s="6"/>
+      <c r="AAB101" s="6"/>
+      <c r="AAC101" s="6"/>
+      <c r="AAD101" s="6"/>
+      <c r="AAE101" s="6"/>
+      <c r="AAF101" s="6"/>
+      <c r="AAG101" s="6"/>
+      <c r="AAH101" s="6"/>
+      <c r="AAI101" s="6"/>
+      <c r="AAJ101" s="6"/>
+      <c r="AAK101" s="6"/>
+      <c r="AAL101" s="6"/>
+      <c r="AAM101" s="6"/>
+      <c r="AAN101" s="6"/>
+      <c r="AAO101" s="6"/>
+      <c r="AAP101" s="6"/>
+      <c r="AAQ101" s="6"/>
+      <c r="AAR101" s="6"/>
+      <c r="AAS101" s="6"/>
+      <c r="AAT101" s="6"/>
+      <c r="AAU101" s="6"/>
+      <c r="AAV101" s="6"/>
+      <c r="AAW101" s="6"/>
+      <c r="AAX101" s="6"/>
+      <c r="AAY101" s="6"/>
+      <c r="AAZ101" s="6"/>
+      <c r="ABA101" s="6"/>
+      <c r="ABB101" s="6"/>
+      <c r="ABC101" s="6"/>
+      <c r="ABD101" s="6"/>
+      <c r="ABE101" s="6"/>
+      <c r="ABF101" s="6"/>
+      <c r="ABG101" s="6"/>
+      <c r="ABH101" s="6"/>
+      <c r="ABI101" s="6"/>
+      <c r="ABJ101" s="6"/>
+      <c r="ABK101" s="6"/>
+      <c r="ABL101" s="6"/>
+      <c r="ABM101" s="6"/>
+      <c r="ABN101" s="6"/>
+      <c r="ABO101" s="6"/>
+      <c r="ABP101" s="6"/>
+      <c r="ABQ101" s="6"/>
+      <c r="ABR101" s="6"/>
+      <c r="ABS101" s="6"/>
+      <c r="ABT101" s="6"/>
+      <c r="ABU101" s="6"/>
+      <c r="ABV101" s="6"/>
+      <c r="ABW101" s="6"/>
+      <c r="ABX101" s="6"/>
+      <c r="ABY101" s="6"/>
+      <c r="ABZ101" s="6"/>
+      <c r="ACA101" s="6"/>
+      <c r="ACB101" s="6"/>
+      <c r="ACC101" s="6"/>
+      <c r="ACD101" s="6"/>
+      <c r="ACE101" s="6"/>
+      <c r="ACF101" s="6"/>
+      <c r="ACG101" s="6"/>
+      <c r="ACH101" s="6"/>
+      <c r="ACI101" s="6"/>
+      <c r="ACJ101" s="6"/>
+      <c r="ACK101" s="6"/>
+      <c r="ACL101" s="6"/>
+      <c r="ACM101" s="6"/>
+      <c r="ACN101" s="6"/>
+      <c r="ACO101" s="6"/>
+      <c r="ACP101" s="6"/>
+      <c r="ACQ101" s="6"/>
+      <c r="ACR101" s="6"/>
+      <c r="ACS101" s="6"/>
+      <c r="ACT101" s="6"/>
+      <c r="ACU101" s="6"/>
+      <c r="ACV101" s="6"/>
+      <c r="ACW101" s="6"/>
+      <c r="ACX101" s="6"/>
+      <c r="ACY101" s="6"/>
+      <c r="ACZ101" s="6"/>
+      <c r="ADA101" s="6"/>
+      <c r="ADB101" s="6"/>
+      <c r="ADC101" s="6"/>
+      <c r="ADD101" s="6"/>
+      <c r="ADE101" s="6"/>
+      <c r="ADF101" s="6"/>
+      <c r="ADG101" s="6"/>
+      <c r="ADH101" s="6"/>
+      <c r="ADI101" s="6"/>
+      <c r="ADJ101" s="6"/>
+      <c r="ADK101" s="6"/>
+      <c r="ADL101" s="6"/>
+      <c r="ADM101" s="6"/>
+      <c r="ADN101" s="6"/>
+      <c r="ADO101" s="6"/>
+      <c r="ADP101" s="6"/>
+      <c r="ADQ101" s="6"/>
+      <c r="ADR101" s="6"/>
+      <c r="ADS101" s="6"/>
+      <c r="ADT101" s="6"/>
+      <c r="ADU101" s="6"/>
+      <c r="ADV101" s="6"/>
+      <c r="ADW101" s="6"/>
+      <c r="ADX101" s="6"/>
+      <c r="ADY101" s="6"/>
+      <c r="ADZ101" s="6"/>
+      <c r="AEA101" s="6"/>
+      <c r="AEB101" s="6"/>
+      <c r="AEC101" s="6"/>
+      <c r="AED101" s="6"/>
+      <c r="AEE101" s="6"/>
+      <c r="AEF101" s="6"/>
+      <c r="AEG101" s="6"/>
+      <c r="AEH101" s="6"/>
+      <c r="AEI101" s="6"/>
+      <c r="AEJ101" s="6"/>
+      <c r="AEK101" s="6"/>
+      <c r="AEL101" s="6"/>
+      <c r="AEM101" s="6"/>
+      <c r="AEN101" s="6"/>
+      <c r="AEO101" s="6"/>
+      <c r="AEP101" s="6"/>
+      <c r="AEQ101" s="6"/>
+      <c r="AER101" s="6"/>
+      <c r="AES101" s="6"/>
+      <c r="AET101" s="6"/>
+      <c r="AEU101" s="6"/>
+      <c r="AEV101" s="6"/>
+      <c r="AEW101" s="6"/>
+      <c r="AEX101" s="6"/>
+      <c r="AEY101" s="6"/>
+      <c r="AEZ101" s="6"/>
+      <c r="AFA101" s="6"/>
+      <c r="AFB101" s="6"/>
+      <c r="AFC101" s="6"/>
+      <c r="AFD101" s="6"/>
+      <c r="AFE101" s="6"/>
+      <c r="AFF101" s="6"/>
+      <c r="AFG101" s="6"/>
+      <c r="AFH101" s="6"/>
+      <c r="AFI101" s="6"/>
+      <c r="AFJ101" s="6"/>
+      <c r="AFK101" s="6"/>
+      <c r="AFL101" s="6"/>
+      <c r="AFM101" s="6"/>
+      <c r="AFN101" s="6"/>
+      <c r="AFO101" s="6"/>
+      <c r="AFP101" s="6"/>
+      <c r="AFQ101" s="6"/>
+      <c r="AFR101" s="6"/>
+      <c r="AFS101" s="6"/>
+      <c r="AFT101" s="6"/>
+      <c r="AFU101" s="6"/>
+      <c r="AFV101" s="6"/>
+      <c r="AFW101" s="6"/>
+      <c r="AFX101" s="6"/>
+      <c r="AFY101" s="6"/>
+      <c r="AFZ101" s="6"/>
+      <c r="AGA101" s="6"/>
+      <c r="AGB101" s="6"/>
+      <c r="AGC101" s="6"/>
+      <c r="AGD101" s="6"/>
+      <c r="AGE101" s="6"/>
+      <c r="AGF101" s="6"/>
+      <c r="AGG101" s="6"/>
+      <c r="AGH101" s="6"/>
+      <c r="AGI101" s="6"/>
+      <c r="AGJ101" s="6"/>
+      <c r="AGK101" s="6"/>
+      <c r="AGL101" s="6"/>
+      <c r="AGM101" s="6"/>
+      <c r="AGN101" s="6"/>
+      <c r="AGO101" s="6"/>
+      <c r="AGP101" s="6"/>
+      <c r="AGQ101" s="6"/>
+      <c r="AGR101" s="6"/>
+      <c r="AGS101" s="6"/>
+      <c r="AGT101" s="6"/>
+      <c r="AGU101" s="6"/>
+      <c r="AGV101" s="6"/>
+      <c r="AGW101" s="6"/>
+      <c r="AGX101" s="6"/>
+      <c r="AGY101" s="6"/>
+      <c r="AGZ101" s="6"/>
+      <c r="AHA101" s="6"/>
+      <c r="AHB101" s="6"/>
+      <c r="AHC101" s="6"/>
+      <c r="AHD101" s="6"/>
+      <c r="AHE101" s="6"/>
+      <c r="AHF101" s="6"/>
+      <c r="AHG101" s="6"/>
+      <c r="AHH101" s="6"/>
+      <c r="AHI101" s="6"/>
+      <c r="AHJ101" s="6"/>
+      <c r="AHK101" s="6"/>
+      <c r="AHL101" s="6"/>
+      <c r="AHM101" s="6"/>
+      <c r="AHN101" s="6"/>
+      <c r="AHO101" s="6"/>
+      <c r="AHP101" s="6"/>
+      <c r="AHQ101" s="6"/>
+      <c r="AHR101" s="6"/>
+      <c r="AHS101" s="6"/>
+      <c r="AHT101" s="6"/>
+      <c r="AHU101" s="6"/>
+      <c r="AHV101" s="6"/>
+      <c r="AHW101" s="6"/>
+      <c r="AHX101" s="6"/>
+      <c r="AHY101" s="6"/>
+      <c r="AHZ101" s="6"/>
+      <c r="AIA101" s="6"/>
+      <c r="AIB101" s="6"/>
+      <c r="AIC101" s="6"/>
+      <c r="AID101" s="6"/>
+      <c r="AIE101" s="6"/>
+      <c r="AIF101" s="6"/>
+      <c r="AIG101" s="6"/>
+      <c r="AIH101" s="6"/>
+      <c r="AII101" s="6"/>
+      <c r="AIJ101" s="6"/>
+      <c r="AIK101" s="6"/>
+      <c r="AIL101" s="6"/>
+      <c r="AIM101" s="6"/>
+      <c r="AIN101" s="6"/>
+      <c r="AIO101" s="6"/>
+      <c r="AIP101" s="6"/>
+      <c r="AIQ101" s="6"/>
+      <c r="AIR101" s="6"/>
+      <c r="AIS101" s="6"/>
+      <c r="AIT101" s="6"/>
+      <c r="AIU101" s="6"/>
+      <c r="AIV101" s="6"/>
+      <c r="AIW101" s="6"/>
+      <c r="AIX101" s="6"/>
+      <c r="AIY101" s="6"/>
+      <c r="AIZ101" s="6"/>
+      <c r="AJA101" s="6"/>
+      <c r="AJB101" s="6"/>
+      <c r="AJC101" s="6"/>
+      <c r="AJD101" s="6"/>
+      <c r="AJE101" s="6"/>
+      <c r="AJF101" s="6"/>
+      <c r="AJG101" s="6"/>
+      <c r="AJH101" s="6"/>
+      <c r="AJI101" s="6"/>
+      <c r="AJJ101" s="6"/>
+      <c r="AJK101" s="6"/>
+      <c r="AJL101" s="6"/>
+      <c r="AJM101" s="6"/>
+      <c r="AJN101" s="6"/>
+      <c r="AJO101" s="6"/>
+      <c r="AJP101" s="6"/>
+      <c r="AJQ101" s="6"/>
+      <c r="AJR101" s="6"/>
+      <c r="AJS101" s="6"/>
+      <c r="AJT101" s="6"/>
+      <c r="AJU101" s="6"/>
+      <c r="AJV101" s="6"/>
+      <c r="AJW101" s="6"/>
+      <c r="AJX101" s="6"/>
+      <c r="AJY101" s="6"/>
+      <c r="AJZ101" s="6"/>
+      <c r="AKA101" s="6"/>
+      <c r="AKB101" s="6"/>
+      <c r="AKC101" s="6"/>
+      <c r="AKD101" s="6"/>
+      <c r="AKE101" s="6"/>
+      <c r="AKF101" s="6"/>
+      <c r="AKG101" s="6"/>
+      <c r="AKH101" s="6"/>
+      <c r="AKI101" s="6"/>
+      <c r="AKJ101" s="6"/>
+      <c r="AKK101" s="6"/>
+      <c r="AKL101" s="6"/>
+      <c r="AKM101" s="6"/>
+      <c r="AKN101" s="6"/>
+      <c r="AKO101" s="6"/>
+      <c r="AKP101" s="6"/>
+      <c r="AKQ101" s="6"/>
+      <c r="AKR101" s="6"/>
+      <c r="AKS101" s="6"/>
+      <c r="AKT101" s="6"/>
+      <c r="AKU101" s="6"/>
+      <c r="AKV101" s="6"/>
+      <c r="AKW101" s="6"/>
+      <c r="AKX101" s="6"/>
+      <c r="AKY101" s="6"/>
+      <c r="AKZ101" s="6"/>
+      <c r="ALA101" s="6"/>
+      <c r="ALB101" s="6"/>
+      <c r="ALC101" s="6"/>
+      <c r="ALD101" s="6"/>
+      <c r="ALE101" s="6"/>
+      <c r="ALF101" s="6"/>
+      <c r="ALG101" s="6"/>
+      <c r="ALH101" s="6"/>
+      <c r="ALI101" s="6"/>
+      <c r="ALJ101" s="6"/>
+      <c r="ALK101" s="6"/>
+      <c r="ALL101" s="6"/>
+      <c r="ALM101" s="6"/>
+      <c r="ALN101" s="6"/>
+      <c r="ALO101" s="6"/>
+      <c r="ALP101" s="6"/>
+      <c r="ALQ101" s="6"/>
+      <c r="ALR101" s="6"/>
+      <c r="ALS101" s="6"/>
+      <c r="ALT101" s="6"/>
+      <c r="ALU101" s="6"/>
+      <c r="ALV101" s="6"/>
+      <c r="ALW101" s="6"/>
+      <c r="ALX101" s="6"/>
+      <c r="ALY101" s="6"/>
+      <c r="ALZ101" s="6"/>
+      <c r="AMA101" s="6"/>
+      <c r="AMB101" s="6"/>
+      <c r="AMC101" s="6"/>
+      <c r="AMD101" s="6"/>
+      <c r="AME101" s="6"/>
+      <c r="AMF101" s="6"/>
+      <c r="AMG101" s="6"/>
+      <c r="AMH101" s="6"/>
+      <c r="AMI101" s="6"/>
+      <c r="AMJ101" s="6"/>
+      <c r="AMK101" s="6"/>
+      <c r="AML101" s="6"/>
+      <c r="AMM101" s="6"/>
+    </row>
+    <row r="102" spans="1:1027" ht="37.25" customHeight="1">
+      <c r="A102" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>651</v>
+      </c>
+      <c r="C102" s="44" t="s">
+        <v>653</v>
+      </c>
+      <c r="D102" s="45" t="s">
+        <v>654</v>
+      </c>
+      <c r="E102" s="14" t="s">
         <v>657</v>
       </c>
-      <c r="F101" s="44" t="s">
+      <c r="F102" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G101" s="44" t="s">
+      <c r="G102" s="43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:1027" s="43" customFormat="1" ht="37.25" customHeight="1">
-      <c r="A102" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="B102" s="44" t="s">
-        <v>651</v>
-      </c>
-      <c r="C102" s="45" t="s">
-        <v>653</v>
-      </c>
-      <c r="D102" s="46" t="s">
-        <v>654</v>
-      </c>
-      <c r="E102" s="14" t="s">
-        <v>656</v>
-      </c>
-      <c r="F102" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G102" s="44" t="s">
-        <v>9</v>
-      </c>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
+      <c r="P102" s="6"/>
+      <c r="Q102" s="6"/>
+      <c r="R102" s="6"/>
+      <c r="S102" s="6"/>
+      <c r="T102" s="6"/>
+      <c r="U102" s="6"/>
+      <c r="V102" s="6"/>
+      <c r="W102" s="6"/>
+      <c r="X102" s="6"/>
+      <c r="Y102" s="6"/>
+      <c r="Z102" s="6"/>
+      <c r="AA102" s="6"/>
+      <c r="AB102" s="6"/>
+      <c r="AC102" s="6"/>
+      <c r="AD102" s="6"/>
+      <c r="AE102" s="6"/>
+      <c r="AF102" s="6"/>
+      <c r="AG102" s="6"/>
+      <c r="AH102" s="6"/>
+      <c r="AI102" s="6"/>
+      <c r="AJ102" s="6"/>
+      <c r="AK102" s="6"/>
+      <c r="AL102" s="6"/>
+      <c r="AM102" s="6"/>
+      <c r="AN102" s="6"/>
+      <c r="AO102" s="6"/>
+      <c r="AP102" s="6"/>
+      <c r="AQ102" s="6"/>
+      <c r="AR102" s="6"/>
+      <c r="AS102" s="6"/>
+      <c r="AT102" s="6"/>
+      <c r="AU102" s="6"/>
+      <c r="AV102" s="6"/>
+      <c r="AW102" s="6"/>
+      <c r="AX102" s="6"/>
+      <c r="AY102" s="6"/>
+      <c r="AZ102" s="6"/>
+      <c r="BA102" s="6"/>
+      <c r="BB102" s="6"/>
+      <c r="BC102" s="6"/>
+      <c r="BD102" s="6"/>
+      <c r="BE102" s="6"/>
+      <c r="BF102" s="6"/>
+      <c r="BG102" s="6"/>
+      <c r="BH102" s="6"/>
+      <c r="BI102" s="6"/>
+      <c r="BJ102" s="6"/>
+      <c r="BK102" s="6"/>
+      <c r="BL102" s="6"/>
+      <c r="BM102" s="6"/>
+      <c r="BN102" s="6"/>
+      <c r="BO102" s="6"/>
+      <c r="BP102" s="6"/>
+      <c r="BQ102" s="6"/>
+      <c r="BR102" s="6"/>
+      <c r="BS102" s="6"/>
+      <c r="BT102" s="6"/>
+      <c r="BU102" s="6"/>
+      <c r="BV102" s="6"/>
+      <c r="BW102" s="6"/>
+      <c r="BX102" s="6"/>
+      <c r="BY102" s="6"/>
+      <c r="BZ102" s="6"/>
+      <c r="CA102" s="6"/>
+      <c r="CB102" s="6"/>
+      <c r="CC102" s="6"/>
+      <c r="CD102" s="6"/>
+      <c r="CE102" s="6"/>
+      <c r="CF102" s="6"/>
+      <c r="CG102" s="6"/>
+      <c r="CH102" s="6"/>
+      <c r="CI102" s="6"/>
+      <c r="CJ102" s="6"/>
+      <c r="CK102" s="6"/>
+      <c r="CL102" s="6"/>
+      <c r="CM102" s="6"/>
+      <c r="CN102" s="6"/>
+      <c r="CO102" s="6"/>
+      <c r="CP102" s="6"/>
+      <c r="CQ102" s="6"/>
+      <c r="CR102" s="6"/>
+      <c r="CS102" s="6"/>
+      <c r="CT102" s="6"/>
+      <c r="CU102" s="6"/>
+      <c r="CV102" s="6"/>
+      <c r="CW102" s="6"/>
+      <c r="CX102" s="6"/>
+      <c r="CY102" s="6"/>
+      <c r="CZ102" s="6"/>
+      <c r="DA102" s="6"/>
+      <c r="DB102" s="6"/>
+      <c r="DC102" s="6"/>
+      <c r="DD102" s="6"/>
+      <c r="DE102" s="6"/>
+      <c r="DF102" s="6"/>
+      <c r="DG102" s="6"/>
+      <c r="DH102" s="6"/>
+      <c r="DI102" s="6"/>
+      <c r="DJ102" s="6"/>
+      <c r="DK102" s="6"/>
+      <c r="DL102" s="6"/>
+      <c r="DM102" s="6"/>
+      <c r="DN102" s="6"/>
+      <c r="DO102" s="6"/>
+      <c r="DP102" s="6"/>
+      <c r="DQ102" s="6"/>
+      <c r="DR102" s="6"/>
+      <c r="DS102" s="6"/>
+      <c r="DT102" s="6"/>
+      <c r="DU102" s="6"/>
+      <c r="DV102" s="6"/>
+      <c r="DW102" s="6"/>
+      <c r="DX102" s="6"/>
+      <c r="DY102" s="6"/>
+      <c r="DZ102" s="6"/>
+      <c r="EA102" s="6"/>
+      <c r="EB102" s="6"/>
+      <c r="EC102" s="6"/>
+      <c r="ED102" s="6"/>
+      <c r="EE102" s="6"/>
+      <c r="EF102" s="6"/>
+      <c r="EG102" s="6"/>
+      <c r="EH102" s="6"/>
+      <c r="EI102" s="6"/>
+      <c r="EJ102" s="6"/>
+      <c r="EK102" s="6"/>
+      <c r="EL102" s="6"/>
+      <c r="EM102" s="6"/>
+      <c r="EN102" s="6"/>
+      <c r="EO102" s="6"/>
+      <c r="EP102" s="6"/>
+      <c r="EQ102" s="6"/>
+      <c r="ER102" s="6"/>
+      <c r="ES102" s="6"/>
+      <c r="ET102" s="6"/>
+      <c r="EU102" s="6"/>
+      <c r="EV102" s="6"/>
+      <c r="EW102" s="6"/>
+      <c r="EX102" s="6"/>
+      <c r="EY102" s="6"/>
+      <c r="EZ102" s="6"/>
+      <c r="FA102" s="6"/>
+      <c r="FB102" s="6"/>
+      <c r="FC102" s="6"/>
+      <c r="FD102" s="6"/>
+      <c r="FE102" s="6"/>
+      <c r="FF102" s="6"/>
+      <c r="FG102" s="6"/>
+      <c r="FH102" s="6"/>
+      <c r="FI102" s="6"/>
+      <c r="FJ102" s="6"/>
+      <c r="FK102" s="6"/>
+      <c r="FL102" s="6"/>
+      <c r="FM102" s="6"/>
+      <c r="FN102" s="6"/>
+      <c r="FO102" s="6"/>
+      <c r="FP102" s="6"/>
+      <c r="FQ102" s="6"/>
+      <c r="FR102" s="6"/>
+      <c r="FS102" s="6"/>
+      <c r="FT102" s="6"/>
+      <c r="FU102" s="6"/>
+      <c r="FV102" s="6"/>
+      <c r="FW102" s="6"/>
+      <c r="FX102" s="6"/>
+      <c r="FY102" s="6"/>
+      <c r="FZ102" s="6"/>
+      <c r="GA102" s="6"/>
+      <c r="GB102" s="6"/>
+      <c r="GC102" s="6"/>
+      <c r="GD102" s="6"/>
+      <c r="GE102" s="6"/>
+      <c r="GF102" s="6"/>
+      <c r="GG102" s="6"/>
+      <c r="GH102" s="6"/>
+      <c r="GI102" s="6"/>
+      <c r="GJ102" s="6"/>
+      <c r="GK102" s="6"/>
+      <c r="GL102" s="6"/>
+      <c r="GM102" s="6"/>
+      <c r="GN102" s="6"/>
+      <c r="GO102" s="6"/>
+      <c r="GP102" s="6"/>
+      <c r="GQ102" s="6"/>
+      <c r="GR102" s="6"/>
+      <c r="GS102" s="6"/>
+      <c r="GT102" s="6"/>
+      <c r="GU102" s="6"/>
+      <c r="GV102" s="6"/>
+      <c r="GW102" s="6"/>
+      <c r="GX102" s="6"/>
+      <c r="GY102" s="6"/>
+      <c r="GZ102" s="6"/>
+      <c r="HA102" s="6"/>
+      <c r="HB102" s="6"/>
+      <c r="HC102" s="6"/>
+      <c r="HD102" s="6"/>
+      <c r="HE102" s="6"/>
+      <c r="HF102" s="6"/>
+      <c r="HG102" s="6"/>
+      <c r="HH102" s="6"/>
+      <c r="HI102" s="6"/>
+      <c r="HJ102" s="6"/>
+      <c r="HK102" s="6"/>
+      <c r="HL102" s="6"/>
+      <c r="HM102" s="6"/>
+      <c r="HN102" s="6"/>
+      <c r="HO102" s="6"/>
+      <c r="HP102" s="6"/>
+      <c r="HQ102" s="6"/>
+      <c r="HR102" s="6"/>
+      <c r="HS102" s="6"/>
+      <c r="HT102" s="6"/>
+      <c r="HU102" s="6"/>
+      <c r="HV102" s="6"/>
+      <c r="HW102" s="6"/>
+      <c r="HX102" s="6"/>
+      <c r="HY102" s="6"/>
+      <c r="HZ102" s="6"/>
+      <c r="IA102" s="6"/>
+      <c r="IB102" s="6"/>
+      <c r="IC102" s="6"/>
+      <c r="ID102" s="6"/>
+      <c r="IE102" s="6"/>
+      <c r="IF102" s="6"/>
+      <c r="IG102" s="6"/>
+      <c r="IH102" s="6"/>
+      <c r="II102" s="6"/>
+      <c r="IJ102" s="6"/>
+      <c r="IK102" s="6"/>
+      <c r="IL102" s="6"/>
+      <c r="IM102" s="6"/>
+      <c r="IN102" s="6"/>
+      <c r="IO102" s="6"/>
+      <c r="IP102" s="6"/>
+      <c r="IQ102" s="6"/>
+      <c r="IR102" s="6"/>
+      <c r="IS102" s="6"/>
+      <c r="IT102" s="6"/>
+      <c r="IU102" s="6"/>
+      <c r="IV102" s="6"/>
+      <c r="IW102" s="6"/>
+      <c r="IX102" s="6"/>
+      <c r="IY102" s="6"/>
+      <c r="IZ102" s="6"/>
+      <c r="JA102" s="6"/>
+      <c r="JB102" s="6"/>
+      <c r="JC102" s="6"/>
+      <c r="JD102" s="6"/>
+      <c r="JE102" s="6"/>
+      <c r="JF102" s="6"/>
+      <c r="JG102" s="6"/>
+      <c r="JH102" s="6"/>
+      <c r="JI102" s="6"/>
+      <c r="JJ102" s="6"/>
+      <c r="JK102" s="6"/>
+      <c r="JL102" s="6"/>
+      <c r="JM102" s="6"/>
+      <c r="JN102" s="6"/>
+      <c r="JO102" s="6"/>
+      <c r="JP102" s="6"/>
+      <c r="JQ102" s="6"/>
+      <c r="JR102" s="6"/>
+      <c r="JS102" s="6"/>
+      <c r="JT102" s="6"/>
+      <c r="JU102" s="6"/>
+      <c r="JV102" s="6"/>
+      <c r="JW102" s="6"/>
+      <c r="JX102" s="6"/>
+      <c r="JY102" s="6"/>
+      <c r="JZ102" s="6"/>
+      <c r="KA102" s="6"/>
+      <c r="KB102" s="6"/>
+      <c r="KC102" s="6"/>
+      <c r="KD102" s="6"/>
+      <c r="KE102" s="6"/>
+      <c r="KF102" s="6"/>
+      <c r="KG102" s="6"/>
+      <c r="KH102" s="6"/>
+      <c r="KI102" s="6"/>
+      <c r="KJ102" s="6"/>
+      <c r="KK102" s="6"/>
+      <c r="KL102" s="6"/>
+      <c r="KM102" s="6"/>
+      <c r="KN102" s="6"/>
+      <c r="KO102" s="6"/>
+      <c r="KP102" s="6"/>
+      <c r="KQ102" s="6"/>
+      <c r="KR102" s="6"/>
+      <c r="KS102" s="6"/>
+      <c r="KT102" s="6"/>
+      <c r="KU102" s="6"/>
+      <c r="KV102" s="6"/>
+      <c r="KW102" s="6"/>
+      <c r="KX102" s="6"/>
+      <c r="KY102" s="6"/>
+      <c r="KZ102" s="6"/>
+      <c r="LA102" s="6"/>
+      <c r="LB102" s="6"/>
+      <c r="LC102" s="6"/>
+      <c r="LD102" s="6"/>
+      <c r="LE102" s="6"/>
+      <c r="LF102" s="6"/>
+      <c r="LG102" s="6"/>
+      <c r="LH102" s="6"/>
+      <c r="LI102" s="6"/>
+      <c r="LJ102" s="6"/>
+      <c r="LK102" s="6"/>
+      <c r="LL102" s="6"/>
+      <c r="LM102" s="6"/>
+      <c r="LN102" s="6"/>
+      <c r="LO102" s="6"/>
+      <c r="LP102" s="6"/>
+      <c r="LQ102" s="6"/>
+      <c r="LR102" s="6"/>
+      <c r="LS102" s="6"/>
+      <c r="LT102" s="6"/>
+      <c r="LU102" s="6"/>
+      <c r="LV102" s="6"/>
+      <c r="LW102" s="6"/>
+      <c r="LX102" s="6"/>
+      <c r="LY102" s="6"/>
+      <c r="LZ102" s="6"/>
+      <c r="MA102" s="6"/>
+      <c r="MB102" s="6"/>
+      <c r="MC102" s="6"/>
+      <c r="MD102" s="6"/>
+      <c r="ME102" s="6"/>
+      <c r="MF102" s="6"/>
+      <c r="MG102" s="6"/>
+      <c r="MH102" s="6"/>
+      <c r="MI102" s="6"/>
+      <c r="MJ102" s="6"/>
+      <c r="MK102" s="6"/>
+      <c r="ML102" s="6"/>
+      <c r="MM102" s="6"/>
+      <c r="MN102" s="6"/>
+      <c r="MO102" s="6"/>
+      <c r="MP102" s="6"/>
+      <c r="MQ102" s="6"/>
+      <c r="MR102" s="6"/>
+      <c r="MS102" s="6"/>
+      <c r="MT102" s="6"/>
+      <c r="MU102" s="6"/>
+      <c r="MV102" s="6"/>
+      <c r="MW102" s="6"/>
+      <c r="MX102" s="6"/>
+      <c r="MY102" s="6"/>
+      <c r="MZ102" s="6"/>
+      <c r="NA102" s="6"/>
+      <c r="NB102" s="6"/>
+      <c r="NC102" s="6"/>
+      <c r="ND102" s="6"/>
+      <c r="NE102" s="6"/>
+      <c r="NF102" s="6"/>
+      <c r="NG102" s="6"/>
+      <c r="NH102" s="6"/>
+      <c r="NI102" s="6"/>
+      <c r="NJ102" s="6"/>
+      <c r="NK102" s="6"/>
+      <c r="NL102" s="6"/>
+      <c r="NM102" s="6"/>
+      <c r="NN102" s="6"/>
+      <c r="NO102" s="6"/>
+      <c r="NP102" s="6"/>
+      <c r="NQ102" s="6"/>
+      <c r="NR102" s="6"/>
+      <c r="NS102" s="6"/>
+      <c r="NT102" s="6"/>
+      <c r="NU102" s="6"/>
+      <c r="NV102" s="6"/>
+      <c r="NW102" s="6"/>
+      <c r="NX102" s="6"/>
+      <c r="NY102" s="6"/>
+      <c r="NZ102" s="6"/>
+      <c r="OA102" s="6"/>
+      <c r="OB102" s="6"/>
+      <c r="OC102" s="6"/>
+      <c r="OD102" s="6"/>
+      <c r="OE102" s="6"/>
+      <c r="OF102" s="6"/>
+      <c r="OG102" s="6"/>
+      <c r="OH102" s="6"/>
+      <c r="OI102" s="6"/>
+      <c r="OJ102" s="6"/>
+      <c r="OK102" s="6"/>
+      <c r="OL102" s="6"/>
+      <c r="OM102" s="6"/>
+      <c r="ON102" s="6"/>
+      <c r="OO102" s="6"/>
+      <c r="OP102" s="6"/>
+      <c r="OQ102" s="6"/>
+      <c r="OR102" s="6"/>
+      <c r="OS102" s="6"/>
+      <c r="OT102" s="6"/>
+      <c r="OU102" s="6"/>
+      <c r="OV102" s="6"/>
+      <c r="OW102" s="6"/>
+      <c r="OX102" s="6"/>
+      <c r="OY102" s="6"/>
+      <c r="OZ102" s="6"/>
+      <c r="PA102" s="6"/>
+      <c r="PB102" s="6"/>
+      <c r="PC102" s="6"/>
+      <c r="PD102" s="6"/>
+      <c r="PE102" s="6"/>
+      <c r="PF102" s="6"/>
+      <c r="PG102" s="6"/>
+      <c r="PH102" s="6"/>
+      <c r="PI102" s="6"/>
+      <c r="PJ102" s="6"/>
+      <c r="PK102" s="6"/>
+      <c r="PL102" s="6"/>
+      <c r="PM102" s="6"/>
+      <c r="PN102" s="6"/>
+      <c r="PO102" s="6"/>
+      <c r="PP102" s="6"/>
+      <c r="PQ102" s="6"/>
+      <c r="PR102" s="6"/>
+      <c r="PS102" s="6"/>
+      <c r="PT102" s="6"/>
+      <c r="PU102" s="6"/>
+      <c r="PV102" s="6"/>
+      <c r="PW102" s="6"/>
+      <c r="PX102" s="6"/>
+      <c r="PY102" s="6"/>
+      <c r="PZ102" s="6"/>
+      <c r="QA102" s="6"/>
+      <c r="QB102" s="6"/>
+      <c r="QC102" s="6"/>
+      <c r="QD102" s="6"/>
+      <c r="QE102" s="6"/>
+      <c r="QF102" s="6"/>
+      <c r="QG102" s="6"/>
+      <c r="QH102" s="6"/>
+      <c r="QI102" s="6"/>
+      <c r="QJ102" s="6"/>
+      <c r="QK102" s="6"/>
+      <c r="QL102" s="6"/>
+      <c r="QM102" s="6"/>
+      <c r="QN102" s="6"/>
+      <c r="QO102" s="6"/>
+      <c r="QP102" s="6"/>
+      <c r="QQ102" s="6"/>
+      <c r="QR102" s="6"/>
+      <c r="QS102" s="6"/>
+      <c r="QT102" s="6"/>
+      <c r="QU102" s="6"/>
+      <c r="QV102" s="6"/>
+      <c r="QW102" s="6"/>
+      <c r="QX102" s="6"/>
+      <c r="QY102" s="6"/>
+      <c r="QZ102" s="6"/>
+      <c r="RA102" s="6"/>
+      <c r="RB102" s="6"/>
+      <c r="RC102" s="6"/>
+      <c r="RD102" s="6"/>
+      <c r="RE102" s="6"/>
+      <c r="RF102" s="6"/>
+      <c r="RG102" s="6"/>
+      <c r="RH102" s="6"/>
+      <c r="RI102" s="6"/>
+      <c r="RJ102" s="6"/>
+      <c r="RK102" s="6"/>
+      <c r="RL102" s="6"/>
+      <c r="RM102" s="6"/>
+      <c r="RN102" s="6"/>
+      <c r="RO102" s="6"/>
+      <c r="RP102" s="6"/>
+      <c r="RQ102" s="6"/>
+      <c r="RR102" s="6"/>
+      <c r="RS102" s="6"/>
+      <c r="RT102" s="6"/>
+      <c r="RU102" s="6"/>
+      <c r="RV102" s="6"/>
+      <c r="RW102" s="6"/>
+      <c r="RX102" s="6"/>
+      <c r="RY102" s="6"/>
+      <c r="RZ102" s="6"/>
+      <c r="SA102" s="6"/>
+      <c r="SB102" s="6"/>
+      <c r="SC102" s="6"/>
+      <c r="SD102" s="6"/>
+      <c r="SE102" s="6"/>
+      <c r="SF102" s="6"/>
+      <c r="SG102" s="6"/>
+      <c r="SH102" s="6"/>
+      <c r="SI102" s="6"/>
+      <c r="SJ102" s="6"/>
+      <c r="SK102" s="6"/>
+      <c r="SL102" s="6"/>
+      <c r="SM102" s="6"/>
+      <c r="SN102" s="6"/>
+      <c r="SO102" s="6"/>
+      <c r="SP102" s="6"/>
+      <c r="SQ102" s="6"/>
+      <c r="SR102" s="6"/>
+      <c r="SS102" s="6"/>
+      <c r="ST102" s="6"/>
+      <c r="SU102" s="6"/>
+      <c r="SV102" s="6"/>
+      <c r="SW102" s="6"/>
+      <c r="SX102" s="6"/>
+      <c r="SY102" s="6"/>
+      <c r="SZ102" s="6"/>
+      <c r="TA102" s="6"/>
+      <c r="TB102" s="6"/>
+      <c r="TC102" s="6"/>
+      <c r="TD102" s="6"/>
+      <c r="TE102" s="6"/>
+      <c r="TF102" s="6"/>
+      <c r="TG102" s="6"/>
+      <c r="TH102" s="6"/>
+      <c r="TI102" s="6"/>
+      <c r="TJ102" s="6"/>
+      <c r="TK102" s="6"/>
+      <c r="TL102" s="6"/>
+      <c r="TM102" s="6"/>
+      <c r="TN102" s="6"/>
+      <c r="TO102" s="6"/>
+      <c r="TP102" s="6"/>
+      <c r="TQ102" s="6"/>
+      <c r="TR102" s="6"/>
+      <c r="TS102" s="6"/>
+      <c r="TT102" s="6"/>
+      <c r="TU102" s="6"/>
+      <c r="TV102" s="6"/>
+      <c r="TW102" s="6"/>
+      <c r="TX102" s="6"/>
+      <c r="TY102" s="6"/>
+      <c r="TZ102" s="6"/>
+      <c r="UA102" s="6"/>
+      <c r="UB102" s="6"/>
+      <c r="UC102" s="6"/>
+      <c r="UD102" s="6"/>
+      <c r="UE102" s="6"/>
+      <c r="UF102" s="6"/>
+      <c r="UG102" s="6"/>
+      <c r="UH102" s="6"/>
+      <c r="UI102" s="6"/>
+      <c r="UJ102" s="6"/>
+      <c r="UK102" s="6"/>
+      <c r="UL102" s="6"/>
+      <c r="UM102" s="6"/>
+      <c r="UN102" s="6"/>
+      <c r="UO102" s="6"/>
+      <c r="UP102" s="6"/>
+      <c r="UQ102" s="6"/>
+      <c r="UR102" s="6"/>
+      <c r="US102" s="6"/>
+      <c r="UT102" s="6"/>
+      <c r="UU102" s="6"/>
+      <c r="UV102" s="6"/>
+      <c r="UW102" s="6"/>
+      <c r="UX102" s="6"/>
+      <c r="UY102" s="6"/>
+      <c r="UZ102" s="6"/>
+      <c r="VA102" s="6"/>
+      <c r="VB102" s="6"/>
+      <c r="VC102" s="6"/>
+      <c r="VD102" s="6"/>
+      <c r="VE102" s="6"/>
+      <c r="VF102" s="6"/>
+      <c r="VG102" s="6"/>
+      <c r="VH102" s="6"/>
+      <c r="VI102" s="6"/>
+      <c r="VJ102" s="6"/>
+      <c r="VK102" s="6"/>
+      <c r="VL102" s="6"/>
+      <c r="VM102" s="6"/>
+      <c r="VN102" s="6"/>
+      <c r="VO102" s="6"/>
+      <c r="VP102" s="6"/>
+      <c r="VQ102" s="6"/>
+      <c r="VR102" s="6"/>
+      <c r="VS102" s="6"/>
+      <c r="VT102" s="6"/>
+      <c r="VU102" s="6"/>
+      <c r="VV102" s="6"/>
+      <c r="VW102" s="6"/>
+      <c r="VX102" s="6"/>
+      <c r="VY102" s="6"/>
+      <c r="VZ102" s="6"/>
+      <c r="WA102" s="6"/>
+      <c r="WB102" s="6"/>
+      <c r="WC102" s="6"/>
+      <c r="WD102" s="6"/>
+      <c r="WE102" s="6"/>
+      <c r="WF102" s="6"/>
+      <c r="WG102" s="6"/>
+      <c r="WH102" s="6"/>
+      <c r="WI102" s="6"/>
+      <c r="WJ102" s="6"/>
+      <c r="WK102" s="6"/>
+      <c r="WL102" s="6"/>
+      <c r="WM102" s="6"/>
+      <c r="WN102" s="6"/>
+      <c r="WO102" s="6"/>
+      <c r="WP102" s="6"/>
+      <c r="WQ102" s="6"/>
+      <c r="WR102" s="6"/>
+      <c r="WS102" s="6"/>
+      <c r="WT102" s="6"/>
+      <c r="WU102" s="6"/>
+      <c r="WV102" s="6"/>
+      <c r="WW102" s="6"/>
+      <c r="WX102" s="6"/>
+      <c r="WY102" s="6"/>
+      <c r="WZ102" s="6"/>
+      <c r="XA102" s="6"/>
+      <c r="XB102" s="6"/>
+      <c r="XC102" s="6"/>
+      <c r="XD102" s="6"/>
+      <c r="XE102" s="6"/>
+      <c r="XF102" s="6"/>
+      <c r="XG102" s="6"/>
+      <c r="XH102" s="6"/>
+      <c r="XI102" s="6"/>
+      <c r="XJ102" s="6"/>
+      <c r="XK102" s="6"/>
+      <c r="XL102" s="6"/>
+      <c r="XM102" s="6"/>
+      <c r="XN102" s="6"/>
+      <c r="XO102" s="6"/>
+      <c r="XP102" s="6"/>
+      <c r="XQ102" s="6"/>
+      <c r="XR102" s="6"/>
+      <c r="XS102" s="6"/>
+      <c r="XT102" s="6"/>
+      <c r="XU102" s="6"/>
+      <c r="XV102" s="6"/>
+      <c r="XW102" s="6"/>
+      <c r="XX102" s="6"/>
+      <c r="XY102" s="6"/>
+      <c r="XZ102" s="6"/>
+      <c r="YA102" s="6"/>
+      <c r="YB102" s="6"/>
+      <c r="YC102" s="6"/>
+      <c r="YD102" s="6"/>
+      <c r="YE102" s="6"/>
+      <c r="YF102" s="6"/>
+      <c r="YG102" s="6"/>
+      <c r="YH102" s="6"/>
+      <c r="YI102" s="6"/>
+      <c r="YJ102" s="6"/>
+      <c r="YK102" s="6"/>
+      <c r="YL102" s="6"/>
+      <c r="YM102" s="6"/>
+      <c r="YN102" s="6"/>
+      <c r="YO102" s="6"/>
+      <c r="YP102" s="6"/>
+      <c r="YQ102" s="6"/>
+      <c r="YR102" s="6"/>
+      <c r="YS102" s="6"/>
+      <c r="YT102" s="6"/>
+      <c r="YU102" s="6"/>
+      <c r="YV102" s="6"/>
+      <c r="YW102" s="6"/>
+      <c r="YX102" s="6"/>
+      <c r="YY102" s="6"/>
+      <c r="YZ102" s="6"/>
+      <c r="ZA102" s="6"/>
+      <c r="ZB102" s="6"/>
+      <c r="ZC102" s="6"/>
+      <c r="ZD102" s="6"/>
+      <c r="ZE102" s="6"/>
+      <c r="ZF102" s="6"/>
+      <c r="ZG102" s="6"/>
+      <c r="ZH102" s="6"/>
+      <c r="ZI102" s="6"/>
+      <c r="ZJ102" s="6"/>
+      <c r="ZK102" s="6"/>
+      <c r="ZL102" s="6"/>
+      <c r="ZM102" s="6"/>
+      <c r="ZN102" s="6"/>
+      <c r="ZO102" s="6"/>
+      <c r="ZP102" s="6"/>
+      <c r="ZQ102" s="6"/>
+      <c r="ZR102" s="6"/>
+      <c r="ZS102" s="6"/>
+      <c r="ZT102" s="6"/>
+      <c r="ZU102" s="6"/>
+      <c r="ZV102" s="6"/>
+      <c r="ZW102" s="6"/>
+      <c r="ZX102" s="6"/>
+      <c r="ZY102" s="6"/>
+      <c r="ZZ102" s="6"/>
+      <c r="AAA102" s="6"/>
+      <c r="AAB102" s="6"/>
+      <c r="AAC102" s="6"/>
+      <c r="AAD102" s="6"/>
+      <c r="AAE102" s="6"/>
+      <c r="AAF102" s="6"/>
+      <c r="AAG102" s="6"/>
+      <c r="AAH102" s="6"/>
+      <c r="AAI102" s="6"/>
+      <c r="AAJ102" s="6"/>
+      <c r="AAK102" s="6"/>
+      <c r="AAL102" s="6"/>
+      <c r="AAM102" s="6"/>
+      <c r="AAN102" s="6"/>
+      <c r="AAO102" s="6"/>
+      <c r="AAP102" s="6"/>
+      <c r="AAQ102" s="6"/>
+      <c r="AAR102" s="6"/>
+      <c r="AAS102" s="6"/>
+      <c r="AAT102" s="6"/>
+      <c r="AAU102" s="6"/>
+      <c r="AAV102" s="6"/>
+      <c r="AAW102" s="6"/>
+      <c r="AAX102" s="6"/>
+      <c r="AAY102" s="6"/>
+      <c r="AAZ102" s="6"/>
+      <c r="ABA102" s="6"/>
+      <c r="ABB102" s="6"/>
+      <c r="ABC102" s="6"/>
+      <c r="ABD102" s="6"/>
+      <c r="ABE102" s="6"/>
+      <c r="ABF102" s="6"/>
+      <c r="ABG102" s="6"/>
+      <c r="ABH102" s="6"/>
+      <c r="ABI102" s="6"/>
+      <c r="ABJ102" s="6"/>
+      <c r="ABK102" s="6"/>
+      <c r="ABL102" s="6"/>
+      <c r="ABM102" s="6"/>
+      <c r="ABN102" s="6"/>
+      <c r="ABO102" s="6"/>
+      <c r="ABP102" s="6"/>
+      <c r="ABQ102" s="6"/>
+      <c r="ABR102" s="6"/>
+      <c r="ABS102" s="6"/>
+      <c r="ABT102" s="6"/>
+      <c r="ABU102" s="6"/>
+      <c r="ABV102" s="6"/>
+      <c r="ABW102" s="6"/>
+      <c r="ABX102" s="6"/>
+      <c r="ABY102" s="6"/>
+      <c r="ABZ102" s="6"/>
+      <c r="ACA102" s="6"/>
+      <c r="ACB102" s="6"/>
+      <c r="ACC102" s="6"/>
+      <c r="ACD102" s="6"/>
+      <c r="ACE102" s="6"/>
+      <c r="ACF102" s="6"/>
+      <c r="ACG102" s="6"/>
+      <c r="ACH102" s="6"/>
+      <c r="ACI102" s="6"/>
+      <c r="ACJ102" s="6"/>
+      <c r="ACK102" s="6"/>
+      <c r="ACL102" s="6"/>
+      <c r="ACM102" s="6"/>
+      <c r="ACN102" s="6"/>
+      <c r="ACO102" s="6"/>
+      <c r="ACP102" s="6"/>
+      <c r="ACQ102" s="6"/>
+      <c r="ACR102" s="6"/>
+      <c r="ACS102" s="6"/>
+      <c r="ACT102" s="6"/>
+      <c r="ACU102" s="6"/>
+      <c r="ACV102" s="6"/>
+      <c r="ACW102" s="6"/>
+      <c r="ACX102" s="6"/>
+      <c r="ACY102" s="6"/>
+      <c r="ACZ102" s="6"/>
+      <c r="ADA102" s="6"/>
+      <c r="ADB102" s="6"/>
+      <c r="ADC102" s="6"/>
+      <c r="ADD102" s="6"/>
+      <c r="ADE102" s="6"/>
+      <c r="ADF102" s="6"/>
+      <c r="ADG102" s="6"/>
+      <c r="ADH102" s="6"/>
+      <c r="ADI102" s="6"/>
+      <c r="ADJ102" s="6"/>
+      <c r="ADK102" s="6"/>
+      <c r="ADL102" s="6"/>
+      <c r="ADM102" s="6"/>
+      <c r="ADN102" s="6"/>
+      <c r="ADO102" s="6"/>
+      <c r="ADP102" s="6"/>
+      <c r="ADQ102" s="6"/>
+      <c r="ADR102" s="6"/>
+      <c r="ADS102" s="6"/>
+      <c r="ADT102" s="6"/>
+      <c r="ADU102" s="6"/>
+      <c r="ADV102" s="6"/>
+      <c r="ADW102" s="6"/>
+      <c r="ADX102" s="6"/>
+      <c r="ADY102" s="6"/>
+      <c r="ADZ102" s="6"/>
+      <c r="AEA102" s="6"/>
+      <c r="AEB102" s="6"/>
+      <c r="AEC102" s="6"/>
+      <c r="AED102" s="6"/>
+      <c r="AEE102" s="6"/>
+      <c r="AEF102" s="6"/>
+      <c r="AEG102" s="6"/>
+      <c r="AEH102" s="6"/>
+      <c r="AEI102" s="6"/>
+      <c r="AEJ102" s="6"/>
+      <c r="AEK102" s="6"/>
+      <c r="AEL102" s="6"/>
+      <c r="AEM102" s="6"/>
+      <c r="AEN102" s="6"/>
+      <c r="AEO102" s="6"/>
+      <c r="AEP102" s="6"/>
+      <c r="AEQ102" s="6"/>
+      <c r="AER102" s="6"/>
+      <c r="AES102" s="6"/>
+      <c r="AET102" s="6"/>
+      <c r="AEU102" s="6"/>
+      <c r="AEV102" s="6"/>
+      <c r="AEW102" s="6"/>
+      <c r="AEX102" s="6"/>
+      <c r="AEY102" s="6"/>
+      <c r="AEZ102" s="6"/>
+      <c r="AFA102" s="6"/>
+      <c r="AFB102" s="6"/>
+      <c r="AFC102" s="6"/>
+      <c r="AFD102" s="6"/>
+      <c r="AFE102" s="6"/>
+      <c r="AFF102" s="6"/>
+      <c r="AFG102" s="6"/>
+      <c r="AFH102" s="6"/>
+      <c r="AFI102" s="6"/>
+      <c r="AFJ102" s="6"/>
+      <c r="AFK102" s="6"/>
+      <c r="AFL102" s="6"/>
+      <c r="AFM102" s="6"/>
+      <c r="AFN102" s="6"/>
+      <c r="AFO102" s="6"/>
+      <c r="AFP102" s="6"/>
+      <c r="AFQ102" s="6"/>
+      <c r="AFR102" s="6"/>
+      <c r="AFS102" s="6"/>
+      <c r="AFT102" s="6"/>
+      <c r="AFU102" s="6"/>
+      <c r="AFV102" s="6"/>
+      <c r="AFW102" s="6"/>
+      <c r="AFX102" s="6"/>
+      <c r="AFY102" s="6"/>
+      <c r="AFZ102" s="6"/>
+      <c r="AGA102" s="6"/>
+      <c r="AGB102" s="6"/>
+      <c r="AGC102" s="6"/>
+      <c r="AGD102" s="6"/>
+      <c r="AGE102" s="6"/>
+      <c r="AGF102" s="6"/>
+      <c r="AGG102" s="6"/>
+      <c r="AGH102" s="6"/>
+      <c r="AGI102" s="6"/>
+      <c r="AGJ102" s="6"/>
+      <c r="AGK102" s="6"/>
+      <c r="AGL102" s="6"/>
+      <c r="AGM102" s="6"/>
+      <c r="AGN102" s="6"/>
+      <c r="AGO102" s="6"/>
+      <c r="AGP102" s="6"/>
+      <c r="AGQ102" s="6"/>
+      <c r="AGR102" s="6"/>
+      <c r="AGS102" s="6"/>
+      <c r="AGT102" s="6"/>
+      <c r="AGU102" s="6"/>
+      <c r="AGV102" s="6"/>
+      <c r="AGW102" s="6"/>
+      <c r="AGX102" s="6"/>
+      <c r="AGY102" s="6"/>
+      <c r="AGZ102" s="6"/>
+      <c r="AHA102" s="6"/>
+      <c r="AHB102" s="6"/>
+      <c r="AHC102" s="6"/>
+      <c r="AHD102" s="6"/>
+      <c r="AHE102" s="6"/>
+      <c r="AHF102" s="6"/>
+      <c r="AHG102" s="6"/>
+      <c r="AHH102" s="6"/>
+      <c r="AHI102" s="6"/>
+      <c r="AHJ102" s="6"/>
+      <c r="AHK102" s="6"/>
+      <c r="AHL102" s="6"/>
+      <c r="AHM102" s="6"/>
+      <c r="AHN102" s="6"/>
+      <c r="AHO102" s="6"/>
+      <c r="AHP102" s="6"/>
+      <c r="AHQ102" s="6"/>
+      <c r="AHR102" s="6"/>
+      <c r="AHS102" s="6"/>
+      <c r="AHT102" s="6"/>
+      <c r="AHU102" s="6"/>
+      <c r="AHV102" s="6"/>
+      <c r="AHW102" s="6"/>
+      <c r="AHX102" s="6"/>
+      <c r="AHY102" s="6"/>
+      <c r="AHZ102" s="6"/>
+      <c r="AIA102" s="6"/>
+      <c r="AIB102" s="6"/>
+      <c r="AIC102" s="6"/>
+      <c r="AID102" s="6"/>
+      <c r="AIE102" s="6"/>
+      <c r="AIF102" s="6"/>
+      <c r="AIG102" s="6"/>
+      <c r="AIH102" s="6"/>
+      <c r="AII102" s="6"/>
+      <c r="AIJ102" s="6"/>
+      <c r="AIK102" s="6"/>
+      <c r="AIL102" s="6"/>
+      <c r="AIM102" s="6"/>
+      <c r="AIN102" s="6"/>
+      <c r="AIO102" s="6"/>
+      <c r="AIP102" s="6"/>
+      <c r="AIQ102" s="6"/>
+      <c r="AIR102" s="6"/>
+      <c r="AIS102" s="6"/>
+      <c r="AIT102" s="6"/>
+      <c r="AIU102" s="6"/>
+      <c r="AIV102" s="6"/>
+      <c r="AIW102" s="6"/>
+      <c r="AIX102" s="6"/>
+      <c r="AIY102" s="6"/>
+      <c r="AIZ102" s="6"/>
+      <c r="AJA102" s="6"/>
+      <c r="AJB102" s="6"/>
+      <c r="AJC102" s="6"/>
+      <c r="AJD102" s="6"/>
+      <c r="AJE102" s="6"/>
+      <c r="AJF102" s="6"/>
+      <c r="AJG102" s="6"/>
+      <c r="AJH102" s="6"/>
+      <c r="AJI102" s="6"/>
+      <c r="AJJ102" s="6"/>
+      <c r="AJK102" s="6"/>
+      <c r="AJL102" s="6"/>
+      <c r="AJM102" s="6"/>
+      <c r="AJN102" s="6"/>
+      <c r="AJO102" s="6"/>
+      <c r="AJP102" s="6"/>
+      <c r="AJQ102" s="6"/>
+      <c r="AJR102" s="6"/>
+      <c r="AJS102" s="6"/>
+      <c r="AJT102" s="6"/>
+      <c r="AJU102" s="6"/>
+      <c r="AJV102" s="6"/>
+      <c r="AJW102" s="6"/>
+      <c r="AJX102" s="6"/>
+      <c r="AJY102" s="6"/>
+      <c r="AJZ102" s="6"/>
+      <c r="AKA102" s="6"/>
+      <c r="AKB102" s="6"/>
+      <c r="AKC102" s="6"/>
+      <c r="AKD102" s="6"/>
+      <c r="AKE102" s="6"/>
+      <c r="AKF102" s="6"/>
+      <c r="AKG102" s="6"/>
+      <c r="AKH102" s="6"/>
+      <c r="AKI102" s="6"/>
+      <c r="AKJ102" s="6"/>
+      <c r="AKK102" s="6"/>
+      <c r="AKL102" s="6"/>
+      <c r="AKM102" s="6"/>
+      <c r="AKN102" s="6"/>
+      <c r="AKO102" s="6"/>
+      <c r="AKP102" s="6"/>
+      <c r="AKQ102" s="6"/>
+      <c r="AKR102" s="6"/>
+      <c r="AKS102" s="6"/>
+      <c r="AKT102" s="6"/>
+      <c r="AKU102" s="6"/>
+      <c r="AKV102" s="6"/>
+      <c r="AKW102" s="6"/>
+      <c r="AKX102" s="6"/>
+      <c r="AKY102" s="6"/>
+      <c r="AKZ102" s="6"/>
+      <c r="ALA102" s="6"/>
+      <c r="ALB102" s="6"/>
+      <c r="ALC102" s="6"/>
+      <c r="ALD102" s="6"/>
+      <c r="ALE102" s="6"/>
+      <c r="ALF102" s="6"/>
+      <c r="ALG102" s="6"/>
+      <c r="ALH102" s="6"/>
+      <c r="ALI102" s="6"/>
+      <c r="ALJ102" s="6"/>
+      <c r="ALK102" s="6"/>
+      <c r="ALL102" s="6"/>
+      <c r="ALM102" s="6"/>
+      <c r="ALN102" s="6"/>
+      <c r="ALO102" s="6"/>
+      <c r="ALP102" s="6"/>
+      <c r="ALQ102" s="6"/>
+      <c r="ALR102" s="6"/>
+      <c r="ALS102" s="6"/>
+      <c r="ALT102" s="6"/>
+      <c r="ALU102" s="6"/>
+      <c r="ALV102" s="6"/>
+      <c r="ALW102" s="6"/>
+      <c r="ALX102" s="6"/>
+      <c r="ALY102" s="6"/>
+      <c r="ALZ102" s="6"/>
+      <c r="AMA102" s="6"/>
+      <c r="AMB102" s="6"/>
+      <c r="AMC102" s="6"/>
+      <c r="AMD102" s="6"/>
+      <c r="AME102" s="6"/>
+      <c r="AMF102" s="6"/>
+      <c r="AMG102" s="6"/>
+      <c r="AMH102" s="6"/>
+      <c r="AMI102" s="6"/>
+      <c r="AMJ102" s="6"/>
+      <c r="AMK102" s="6"/>
+      <c r="AML102" s="6"/>
+      <c r="AMM102" s="6"/>
     </row>
     <row r="103" spans="1:1027" ht="120">
       <c r="A103" s="14" t="s">

</xml_diff>

<commit_message>
added description of other
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0984A10-4D21-E047-A705-48FB44FC5D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6BBA42-633C-45E6-A9F1-52F8003BA4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4900" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -18662,32 +18662,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The tags with an </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> at the end and PP1, PP2 consist of aggregates of individual tags. To avoid false correlation, skew etc. in the data, they should not be used in combination with the respective individual tags.</t>
-    </r>
-  </si>
-  <si>
     <t>Superlatives</t>
   </si>
   <si>
@@ -19041,13 +19015,16 @@
       </rPr>
       <t>+ ADJ/ADV.</t>
     </r>
+  </si>
+  <si>
+    <t>Important: The following features consist of aggregates of individual tags. To avoid redundant correlations, undue skew etc. in the data, they should not be used in combination with the respective individual tags. E.g., either use PP1 counts or the counts of PP1S &amp; PP1P, but not all three!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -19204,6 +19181,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -19344,7 +19328,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -19498,6 +19482,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -20051,30 +20038,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="27" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="70.6640625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" style="4" customWidth="1"/>
-    <col min="13" max="1026" width="14.1640625" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="14.6640625" style="1" customWidth="1"/>
-    <col min="1028" max="16384" width="10.6640625" style="6"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="70.625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="33.625" style="4" customWidth="1"/>
+    <col min="13" max="1026" width="14.125" style="1" customWidth="1"/>
+    <col min="1027" max="1027" width="14.625" style="1" customWidth="1"/>
+    <col min="1028" max="16384" width="10.625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="24" customFormat="1" ht="30">
+    <row r="1" spans="1:7" s="24" customFormat="1" ht="25.5">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -20108,7 +20095,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A3" s="9" t="s">
         <v>284</v>
       </c>
@@ -20131,7 +20118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="4" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A4" s="9" t="s">
         <v>284</v>
       </c>
@@ -20154,7 +20141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A5" s="9" t="s">
         <v>284</v>
       </c>
@@ -20177,7 +20164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="45">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="51">
       <c r="A6" s="9" t="s">
         <v>284</v>
       </c>
@@ -20200,7 +20187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="120">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="114.75">
       <c r="A7" s="9" t="s">
         <v>284</v>
       </c>
@@ -20234,7 +20221,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="9" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A9" s="14" t="s">
         <v>223</v>
       </c>
@@ -20257,7 +20244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A10" s="14" t="s">
         <v>223</v>
       </c>
@@ -20280,7 +20267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="11" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A11" s="14" t="s">
         <v>221</v>
       </c>
@@ -20303,7 +20290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A12" s="14" t="s">
         <v>221</v>
       </c>
@@ -20326,7 +20313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A13" s="14" t="s">
         <v>221</v>
       </c>
@@ -20349,7 +20336,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="14" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A14" s="14" t="s">
         <v>221</v>
       </c>
@@ -20372,7 +20359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="15" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A15" s="14" t="s">
         <v>220</v>
       </c>
@@ -20395,7 +20382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="16" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A16" s="14" t="s">
         <v>220</v>
       </c>
@@ -20441,7 +20428,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="70.25" customHeight="1">
+    <row r="18" spans="1:7" s="6" customFormat="1" ht="70.349999999999994" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>220</v>
       </c>
@@ -20464,7 +20451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="19" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A19" s="14" t="s">
         <v>220</v>
       </c>
@@ -20487,7 +20474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="20" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A20" s="14" t="s">
         <v>224</v>
       </c>
@@ -20510,7 +20497,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="6" customFormat="1" ht="135">
+    <row r="21" spans="1:7" s="6" customFormat="1" ht="114.75">
       <c r="A21" s="14" t="s">
         <v>224</v>
       </c>
@@ -20533,7 +20520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="22" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A22" s="14" t="s">
         <v>224</v>
       </c>
@@ -20556,7 +20543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="23" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A23" s="14" t="s">
         <v>224</v>
       </c>
@@ -20579,7 +20566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" ht="30">
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="25.5">
       <c r="A24" s="14" t="s">
         <v>224</v>
       </c>
@@ -20602,7 +20589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="165">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="140.25">
       <c r="A25" s="14" t="s">
         <v>224</v>
       </c>
@@ -20625,7 +20612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A26" s="14" t="s">
         <v>224</v>
       </c>
@@ -20648,7 +20635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A27" s="14" t="s">
         <v>224</v>
       </c>
@@ -20671,7 +20658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A28" s="14" t="s">
         <v>224</v>
       </c>
@@ -20694,7 +20681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A29" s="14" t="s">
         <v>224</v>
       </c>
@@ -20717,7 +20704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A30" s="14" t="s">
         <v>224</v>
       </c>
@@ -20740,7 +20727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A31" s="14" t="s">
         <v>224</v>
       </c>
@@ -20763,7 +20750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A32" s="14" t="s">
         <v>224</v>
       </c>
@@ -20786,7 +20773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A33" s="14" t="s">
         <v>224</v>
       </c>
@@ -20809,7 +20796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="6" customFormat="1" ht="135">
+    <row r="34" spans="1:7" s="6" customFormat="1" ht="114.75">
       <c r="A34" s="14" t="s">
         <v>224</v>
       </c>
@@ -20832,7 +20819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="35" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A35" s="14" t="s">
         <v>224</v>
       </c>
@@ -20855,7 +20842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="36" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A36" s="14" t="s">
         <v>34</v>
       </c>
@@ -20878,7 +20865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="37" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A37" s="14" t="s">
         <v>34</v>
       </c>
@@ -20901,7 +20888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="38" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A38" s="14" t="s">
         <v>34</v>
       </c>
@@ -20924,7 +20911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1">
+    <row r="39" spans="1:7" s="6" customFormat="1" ht="25.5">
       <c r="A39" s="14" t="s">
         <v>34</v>
       </c>
@@ -20947,7 +20934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="40" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A40" s="14" t="s">
         <v>34</v>
       </c>
@@ -20970,7 +20957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="41" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A41" s="14" t="s">
         <v>71</v>
       </c>
@@ -20993,7 +20980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="42" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A42" s="14" t="s">
         <v>117</v>
       </c>
@@ -21016,7 +21003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="43" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A43" s="14" t="s">
         <v>60</v>
       </c>
@@ -21039,7 +21026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="44" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A44" s="14" t="s">
         <v>60</v>
       </c>
@@ -21062,7 +21049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="45" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A45" s="14" t="s">
         <v>60</v>
       </c>
@@ -21085,7 +21072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A46" s="14" t="s">
         <v>60</v>
       </c>
@@ -21108,7 +21095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="47" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A47" s="14" t="s">
         <v>60</v>
       </c>
@@ -21131,7 +21118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="48" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A48" s="14" t="s">
         <v>60</v>
       </c>
@@ -21154,7 +21141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="49" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A49" s="14" t="s">
         <v>60</v>
       </c>
@@ -21177,7 +21164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="6" customFormat="1" ht="30">
+    <row r="50" spans="1:7" s="6" customFormat="1" ht="25.5">
       <c r="A50" s="14" t="s">
         <v>60</v>
       </c>
@@ -21200,7 +21187,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="51" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A51" s="14" t="s">
         <v>227</v>
       </c>
@@ -21223,7 +21210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="52" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A52" s="14" t="s">
         <v>227</v>
       </c>
@@ -21246,7 +21233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="53" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A53" s="14" t="s">
         <v>227</v>
       </c>
@@ -21269,7 +21256,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="54" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A54" s="14" t="s">
         <v>227</v>
       </c>
@@ -21292,7 +21279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="6" customFormat="1" ht="105">
+    <row r="55" spans="1:7" s="6" customFormat="1" ht="89.25">
       <c r="A55" s="14" t="s">
         <v>227</v>
       </c>
@@ -21315,7 +21302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="56" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A56" s="14" t="s">
         <v>222</v>
       </c>
@@ -21338,7 +21325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="6" customFormat="1" ht="165">
+    <row r="57" spans="1:7" s="6" customFormat="1" ht="153">
       <c r="A57" s="14" t="s">
         <v>222</v>
       </c>
@@ -21361,7 +21348,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="58" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A58" s="14" t="s">
         <v>65</v>
       </c>
@@ -21407,7 +21394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="60" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A60" s="14" t="s">
         <v>228</v>
       </c>
@@ -21430,7 +21417,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="61" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A61" s="14" t="s">
         <v>228</v>
       </c>
@@ -21453,7 +21440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="6" customFormat="1" ht="120">
+    <row r="62" spans="1:7" s="6" customFormat="1" ht="102">
       <c r="A62" s="14" t="s">
         <v>228</v>
       </c>
@@ -21476,7 +21463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="63" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A63" s="14" t="s">
         <v>228</v>
       </c>
@@ -21499,7 +21486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="64" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A64" s="14" t="s">
         <v>228</v>
       </c>
@@ -21522,7 +21509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="65" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A65" s="14" t="s">
         <v>228</v>
       </c>
@@ -21545,7 +21532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="66" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A66" s="14" t="s">
         <v>228</v>
       </c>
@@ -21568,7 +21555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="67" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A67" s="14" t="s">
         <v>228</v>
       </c>
@@ -21591,7 +21578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="6" customFormat="1" ht="165">
+    <row r="68" spans="1:7" s="6" customFormat="1" ht="140.25">
       <c r="A68" s="14" t="s">
         <v>228</v>
       </c>
@@ -21614,7 +21601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="69" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A69" s="14" t="s">
         <v>228</v>
       </c>
@@ -21637,7 +21624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="6" customFormat="1" ht="120">
+    <row r="70" spans="1:7" s="6" customFormat="1" ht="102">
       <c r="A70" s="14" t="s">
         <v>228</v>
       </c>
@@ -21660,7 +21647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="71" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A71" s="14" t="s">
         <v>228</v>
       </c>
@@ -21683,7 +21670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="6" customFormat="1" ht="75">
+    <row r="72" spans="1:7" s="6" customFormat="1" ht="63.75">
       <c r="A72" s="14" t="s">
         <v>228</v>
       </c>
@@ -21706,7 +21693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="6" customFormat="1" ht="135">
+    <row r="73" spans="1:7" s="6" customFormat="1" ht="114.75">
       <c r="A73" s="14" t="s">
         <v>91</v>
       </c>
@@ -21729,7 +21716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="6" customFormat="1" ht="135">
+    <row r="74" spans="1:7" s="6" customFormat="1" ht="127.5">
       <c r="A74" s="14" t="s">
         <v>91</v>
       </c>
@@ -21752,7 +21739,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="6" customFormat="1" ht="30">
+    <row r="75" spans="1:7" s="6" customFormat="1" ht="25.5">
       <c r="A75" s="14" t="s">
         <v>91</v>
       </c>
@@ -21775,7 +21762,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="6" customFormat="1" ht="60">
+    <row r="76" spans="1:7" s="6" customFormat="1" ht="51">
       <c r="A76" s="14" t="s">
         <v>91</v>
       </c>
@@ -21798,7 +21785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="6" customFormat="1" ht="150">
+    <row r="77" spans="1:7" s="6" customFormat="1" ht="127.5">
       <c r="A77" s="14" t="s">
         <v>91</v>
       </c>
@@ -21821,7 +21808,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="6" customFormat="1" ht="90">
+    <row r="78" spans="1:7" s="6" customFormat="1" ht="76.5">
       <c r="A78" s="14" t="s">
         <v>91</v>
       </c>
@@ -21844,7 +21831,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="6" customFormat="1" ht="180">
+    <row r="79" spans="1:7" s="6" customFormat="1" ht="153">
       <c r="A79" s="14" t="s">
         <v>91</v>
       </c>
@@ -21867,7 +21854,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="6" customFormat="1" ht="45">
+    <row r="80" spans="1:7" s="6" customFormat="1" ht="38.25">
       <c r="A80" s="14" t="s">
         <v>91</v>
       </c>
@@ -21890,7 +21877,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:1022" s="6" customFormat="1" ht="75">
+    <row r="81" spans="1:1022" s="6" customFormat="1" ht="63.75">
       <c r="A81" s="14" t="s">
         <v>91</v>
       </c>
@@ -21913,7 +21900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:1022" s="6" customFormat="1" ht="30">
+    <row r="82" spans="1:1022" s="6" customFormat="1" ht="25.5">
       <c r="A82" s="14" t="s">
         <v>91</v>
       </c>
@@ -21936,7 +21923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:1022" s="6" customFormat="1" ht="60">
+    <row r="83" spans="1:1022" s="6" customFormat="1" ht="51">
       <c r="A83" s="14" t="s">
         <v>91</v>
       </c>
@@ -21959,7 +21946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:1022" s="6" customFormat="1" ht="30">
+    <row r="84" spans="1:1022" s="6" customFormat="1" ht="25.5">
       <c r="A84" s="14" t="s">
         <v>91</v>
       </c>
@@ -21982,7 +21969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:1022" s="6" customFormat="1" ht="30">
+    <row r="85" spans="1:1022" s="6" customFormat="1" ht="25.5">
       <c r="A85" s="14" t="s">
         <v>91</v>
       </c>
@@ -22005,7 +21992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:1022" s="6" customFormat="1" ht="60">
+    <row r="86" spans="1:1022" s="6" customFormat="1" ht="51">
       <c r="A86" s="14" t="s">
         <v>91</v>
       </c>
@@ -22028,7 +22015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:1022" s="6" customFormat="1" ht="45">
+    <row r="87" spans="1:1022" s="6" customFormat="1" ht="38.25">
       <c r="A87" s="14" t="s">
         <v>91</v>
       </c>
@@ -22062,7 +22049,7 @@
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
     </row>
-    <row r="89" spans="1:1022" s="6" customFormat="1" ht="60">
+    <row r="89" spans="1:1022" s="6" customFormat="1" ht="51">
       <c r="A89" s="9" t="s">
         <v>34</v>
       </c>
@@ -23100,7 +23087,7 @@
       <c r="AMG89" s="1"/>
       <c r="AMH89" s="1"/>
     </row>
-    <row r="90" spans="1:1022" s="6" customFormat="1" ht="45">
+    <row r="90" spans="1:1022" s="6" customFormat="1" ht="51">
       <c r="A90" s="9" t="s">
         <v>34</v>
       </c>
@@ -24138,7 +24125,7 @@
       <c r="AMG90" s="1"/>
       <c r="AMH90" s="1"/>
     </row>
-    <row r="91" spans="1:1022" s="6" customFormat="1" ht="75">
+    <row r="91" spans="1:1022" s="6" customFormat="1" ht="63.75">
       <c r="A91" s="9" t="s">
         <v>228</v>
       </c>
@@ -24161,7 +24148,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:1022" s="6" customFormat="1" ht="75">
+    <row r="92" spans="1:1022" s="6" customFormat="1" ht="63.75">
       <c r="A92" s="9" t="s">
         <v>228</v>
       </c>
@@ -24184,7 +24171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:1022" s="6" customFormat="1" ht="105">
+    <row r="93" spans="1:1022" s="6" customFormat="1" ht="89.25">
       <c r="A93" s="9" t="s">
         <v>91</v>
       </c>
@@ -24207,7 +24194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:1022" s="6" customFormat="1" ht="90">
+    <row r="94" spans="1:1022" s="6" customFormat="1" ht="76.5">
       <c r="A94" s="9" t="s">
         <v>91</v>
       </c>
@@ -24230,7 +24217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:1022" s="6" customFormat="1" ht="75">
+    <row r="95" spans="1:1022" s="6" customFormat="1" ht="63.75">
       <c r="A95" s="9" t="s">
         <v>91</v>
       </c>
@@ -24253,7 +24240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:1022" s="6" customFormat="1" ht="37.25" customHeight="1">
+    <row r="96" spans="1:1022" s="6" customFormat="1" ht="37.35" customHeight="1">
       <c r="A96" s="12"/>
       <c r="B96" s="20"/>
       <c r="C96" s="7"/>
@@ -24264,7 +24251,7 @@
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
     </row>
-    <row r="97" spans="1:1027" ht="60">
+    <row r="97" spans="1:1027" ht="51">
       <c r="A97" s="9" t="s">
         <v>91</v>
       </c>
@@ -25307,7 +25294,7 @@
       <c r="AML97" s="6"/>
       <c r="AMM97" s="6"/>
     </row>
-    <row r="98" spans="1:1027" ht="45">
+    <row r="98" spans="1:1027" ht="38.25">
       <c r="A98" s="9" t="s">
         <v>228</v>
       </c>
@@ -26350,7 +26337,7 @@
       <c r="AML98" s="6"/>
       <c r="AMM98" s="6"/>
     </row>
-    <row r="99" spans="1:1027" ht="60">
+    <row r="99" spans="1:1027" ht="51">
       <c r="A99" s="9" t="s">
         <v>224</v>
       </c>
@@ -27393,7 +27380,7 @@
       <c r="AML99" s="6"/>
       <c r="AMM99" s="6"/>
     </row>
-    <row r="100" spans="1:1027" ht="37.25" customHeight="1">
+    <row r="100" spans="1:1027" ht="37.35" customHeight="1">
       <c r="A100" s="31"/>
       <c r="B100" s="32"/>
       <c r="C100" s="33"/>
@@ -28424,21 +28411,21 @@
       <c r="AML100" s="6"/>
       <c r="AMM100" s="6"/>
     </row>
-    <row r="101" spans="1:1027" ht="37.25" customHeight="1">
+    <row r="101" spans="1:1027" ht="37.35" customHeight="1">
       <c r="A101" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B101" s="43" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C101" s="44" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D101" s="45" t="s">
+        <v>654</v>
+      </c>
+      <c r="E101" s="14" t="s">
         <v>655</v>
-      </c>
-      <c r="E101" s="14" t="s">
-        <v>656</v>
       </c>
       <c r="F101" s="43" t="s">
         <v>8</v>
@@ -29467,21 +29454,21 @@
       <c r="AML101" s="6"/>
       <c r="AMM101" s="6"/>
     </row>
-    <row r="102" spans="1:1027" ht="37.25" customHeight="1">
+    <row r="102" spans="1:1027" ht="37.35" customHeight="1">
       <c r="A102" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B102" s="43" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C102" s="44" t="s">
+        <v>652</v>
+      </c>
+      <c r="D102" s="45" t="s">
         <v>653</v>
       </c>
-      <c r="D102" s="45" t="s">
-        <v>654</v>
-      </c>
       <c r="E102" s="14" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F102" s="43" t="s">
         <v>8</v>
@@ -30510,7 +30497,7 @@
       <c r="AML102" s="6"/>
       <c r="AMM102" s="6"/>
     </row>
-    <row r="103" spans="1:1027" ht="120">
+    <row r="103" spans="1:1027" ht="102">
       <c r="A103" s="14" t="s">
         <v>65</v>
       </c>
@@ -30531,7 +30518,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="104" spans="1:1027" ht="120">
+    <row r="104" spans="1:1027" ht="102">
       <c r="A104" s="14" t="s">
         <v>65</v>
       </c>
@@ -30552,7 +30539,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="105" spans="1:1027" ht="120">
+    <row r="105" spans="1:1027" ht="102">
       <c r="A105" s="14" t="s">
         <v>65</v>
       </c>
@@ -30572,7 +30559,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="106" spans="1:1027" ht="120">
+    <row r="106" spans="1:1027" ht="102">
       <c r="A106" s="14" t="s">
         <v>65</v>
       </c>
@@ -30592,7 +30579,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="107" spans="1:1027" ht="120">
+    <row r="107" spans="1:1027" ht="102">
       <c r="A107" s="14" t="s">
         <v>65</v>
       </c>
@@ -30612,7 +30599,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="108" spans="1:1027" ht="105">
+    <row r="108" spans="1:1027" ht="102">
       <c r="A108" s="14" t="s">
         <v>65</v>
       </c>
@@ -30632,7 +30619,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="109" spans="1:1027" ht="120">
+    <row r="109" spans="1:1027" ht="102">
       <c r="A109" s="14" t="s">
         <v>65</v>
       </c>
@@ -30652,7 +30639,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="110" spans="1:1027" ht="120">
+    <row r="110" spans="1:1027" ht="102">
       <c r="A110" s="14" t="s">
         <v>65</v>
       </c>
@@ -30672,7 +30659,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="111" spans="1:1027" ht="120">
+    <row r="111" spans="1:1027" ht="102">
       <c r="A111" s="14" t="s">
         <v>65</v>
       </c>
@@ -30692,7 +30679,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="112" spans="1:1027" ht="409.6">
+    <row r="112" spans="1:1027" ht="382.5">
       <c r="A112" s="14" t="s">
         <v>65</v>
       </c>
@@ -30712,7 +30699,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="135">
+    <row r="113" spans="1:7" ht="127.5">
       <c r="A113" s="14" t="s">
         <v>65</v>
       </c>
@@ -30732,7 +30719,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="120">
+    <row r="114" spans="1:7" ht="114.75">
       <c r="A114" s="14" t="s">
         <v>65</v>
       </c>
@@ -30752,7 +30739,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="120">
+    <row r="115" spans="1:7" ht="102">
       <c r="A115" s="14"/>
       <c r="B115" s="30" t="s">
         <v>567</v>
@@ -30770,7 +30757,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="409.6">
+    <row r="116" spans="1:7" ht="395.25">
       <c r="A116" s="14" t="s">
         <v>91</v>
       </c>
@@ -30790,7 +30777,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="150">
+    <row r="117" spans="1:7" ht="127.5">
       <c r="A117" s="14" t="s">
         <v>91</v>
       </c>
@@ -30810,7 +30797,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="135">
+    <row r="118" spans="1:7" ht="127.5">
       <c r="A118" s="14" t="s">
         <v>91</v>
       </c>
@@ -30830,7 +30817,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="75">
+    <row r="119" spans="1:7" ht="51.75">
       <c r="A119" s="14" t="s">
         <v>65</v>
       </c>
@@ -30851,7 +30838,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="75">
+    <row r="120" spans="1:7" ht="51.75">
       <c r="A120" s="14" t="s">
         <v>65</v>
       </c>
@@ -30872,7 +30859,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="75">
+    <row r="121" spans="1:7" ht="51.75">
       <c r="A121" s="14" t="s">
         <v>65</v>
       </c>
@@ -30893,7 +30880,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="75">
+    <row r="122" spans="1:7" ht="51.75">
       <c r="A122" s="14" t="s">
         <v>65</v>
       </c>
@@ -30914,7 +30901,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="75">
+    <row r="123" spans="1:7" ht="51.75">
       <c r="A123" s="14" t="s">
         <v>65</v>
       </c>
@@ -30935,7 +30922,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="105">
+    <row r="124" spans="1:7" ht="90">
       <c r="A124" s="14" t="s">
         <v>65</v>
       </c>
@@ -30956,7 +30943,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="135">
+    <row r="125" spans="1:7" ht="115.5">
       <c r="A125" s="14" t="s">
         <v>65</v>
       </c>
@@ -30977,7 +30964,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="105">
+    <row r="126" spans="1:7" ht="90">
       <c r="A126" s="14" t="s">
         <v>65</v>
       </c>
@@ -30998,7 +30985,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="75">
+    <row r="127" spans="1:7" ht="51.75">
       <c r="A127" s="14" t="s">
         <v>65</v>
       </c>
@@ -31019,7 +31006,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="75">
+    <row r="128" spans="1:7" ht="64.5">
       <c r="A128" s="14" t="s">
         <v>65</v>
       </c>
@@ -31040,7 +31027,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="105">
+    <row r="129" spans="1:7" ht="90">
       <c r="A129" s="14" t="s">
         <v>65</v>
       </c>
@@ -31061,7 +31048,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="409.6">
+    <row r="130" spans="1:7" ht="383.25">
       <c r="A130" s="14" t="s">
         <v>65</v>
       </c>
@@ -31082,7 +31069,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="135">
+    <row r="131" spans="1:7" ht="115.5">
       <c r="A131" s="14" t="s">
         <v>65</v>
       </c>
@@ -31103,7 +31090,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="120">
+    <row r="132" spans="1:7" ht="102.75">
       <c r="A132" s="14" t="s">
         <v>65</v>
       </c>
@@ -31124,7 +31111,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="75">
+    <row r="133" spans="1:7" ht="64.5">
       <c r="A133" s="14" t="s">
         <v>65</v>
       </c>
@@ -31144,7 +31131,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="180">
+    <row r="134" spans="1:7" ht="166.5">
       <c r="A134" s="14" t="s">
         <v>65</v>
       </c>
@@ -31164,7 +31151,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="75">
+    <row r="135" spans="1:7" ht="64.5">
       <c r="A135" s="14" t="s">
         <v>536</v>
       </c>
@@ -31184,7 +31171,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="75">
+    <row r="136" spans="1:7" ht="51">
       <c r="A136" s="14" t="s">
         <v>536</v>
       </c>
@@ -31204,7 +31191,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="75">
+    <row r="137" spans="1:7" ht="64.5">
       <c r="A137" s="14" t="s">
         <v>536</v>
       </c>
@@ -31224,7 +31211,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="75">
+    <row r="138" spans="1:7" ht="51">
       <c r="A138" s="14" t="s">
         <v>536</v>
       </c>
@@ -31244,7 +31231,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="75">
+    <row r="139" spans="1:7" ht="51.75">
       <c r="A139" s="14" t="s">
         <v>536</v>
       </c>
@@ -31264,7 +31251,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="75">
+    <row r="140" spans="1:7" ht="51">
       <c r="A140" s="14" t="s">
         <v>536</v>
       </c>
@@ -31284,7 +31271,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="75">
+    <row r="141" spans="1:7" ht="51">
       <c r="A141" s="14" t="s">
         <v>536</v>
       </c>
@@ -31304,7 +31291,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="75">
+    <row r="142" spans="1:7" ht="51">
       <c r="A142" s="14" t="s">
         <v>536</v>
       </c>
@@ -31345,7 +31332,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="180">
+    <row r="144" spans="1:7" ht="153.75">
       <c r="A144" s="1" t="s">
         <v>537</v>
       </c>
@@ -31387,7 +31374,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="146" spans="1:1027" ht="90">
+    <row r="146" spans="1:1027" ht="77.25">
       <c r="A146" s="1" t="s">
         <v>537</v>
       </c>
@@ -31408,7 +31395,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="147" spans="1:1027" ht="409.6">
+    <row r="147" spans="1:1027" ht="383.25">
       <c r="A147" s="1" t="s">
         <v>537</v>
       </c>
@@ -31429,7 +31416,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:1027" ht="240">
+    <row r="148" spans="1:1027" ht="204.75">
       <c r="A148" s="1" t="s">
         <v>537</v>
       </c>
@@ -31450,7 +31437,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="149" spans="1:1027" ht="135">
+    <row r="149" spans="1:1027" ht="115.5">
       <c r="A149" s="1" t="s">
         <v>537</v>
       </c>
@@ -31471,7 +31458,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="150" spans="1:1027" ht="195">
+    <row r="150" spans="1:1027" ht="166.5">
       <c r="A150" s="1" t="s">
         <v>537</v>
       </c>
@@ -31492,7 +31479,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="151" spans="1:1027" ht="105">
+    <row r="151" spans="1:1027" ht="76.5">
       <c r="A151" s="1" t="s">
         <v>537</v>
       </c>
@@ -31513,7 +31500,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="152" spans="1:1027" ht="45">
+    <row r="152" spans="1:1027" ht="38.25">
       <c r="A152" s="1" t="s">
         <v>537</v>
       </c>
@@ -31534,7 +31521,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="153" spans="1:1027" ht="180">
+    <row r="153" spans="1:1027" ht="166.5">
       <c r="A153" s="1" t="s">
         <v>537</v>
       </c>
@@ -31555,7 +31542,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="154" spans="1:1027" ht="75">
+    <row r="154" spans="1:1027" ht="51">
       <c r="A154" s="1" t="s">
         <v>538</v>
       </c>
@@ -31575,7 +31562,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="155" spans="1:1027" ht="75">
+    <row r="155" spans="1:1027" ht="51">
       <c r="A155" s="1" t="s">
         <v>538</v>
       </c>
@@ -31595,7 +31582,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="156" spans="1:1027" ht="75">
+    <row r="156" spans="1:1027" ht="51">
       <c r="A156" s="1" t="s">
         <v>538</v>
       </c>
@@ -31615,7 +31602,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="157" spans="1:1027" ht="75">
+    <row r="157" spans="1:1027" ht="51">
       <c r="A157" s="1" t="s">
         <v>538</v>
       </c>
@@ -31635,15 +31622,15 @@
         <v>522</v>
       </c>
     </row>
-    <row r="158" spans="1:1027" s="42" customFormat="1" ht="45">
+    <row r="158" spans="1:1027" s="42" customFormat="1" ht="39">
       <c r="A158" s="36"/>
       <c r="B158" s="37"/>
       <c r="C158" s="36"/>
       <c r="D158" s="38" t="s">
         <v>593</v>
       </c>
-      <c r="E158" s="36" t="s">
-        <v>649</v>
+      <c r="E158" s="46" t="s">
+        <v>657</v>
       </c>
       <c r="F158" s="36"/>
       <c r="G158" s="39"/>
@@ -32668,7 +32655,7 @@
       <c r="AML158" s="36"/>
       <c r="AMM158" s="36"/>
     </row>
-    <row r="159" spans="1:1027" ht="75">
+    <row r="159" spans="1:1027" ht="51.75">
       <c r="A159" s="1" t="s">
         <v>60</v>
       </c>
@@ -32688,7 +32675,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="160" spans="1:1027" ht="75">
+    <row r="160" spans="1:1027" ht="51.75">
       <c r="A160" s="1" t="s">
         <v>60</v>
       </c>
@@ -32708,7 +32695,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="30">
+    <row r="161" spans="1:7" ht="26.25">
       <c r="A161" s="1" t="s">
         <v>91</v>
       </c>
@@ -32728,7 +32715,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="30">
+    <row r="162" spans="1:7" ht="26.25">
       <c r="A162" s="1" t="s">
         <v>91</v>
       </c>
@@ -32748,7 +32735,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="30">
+    <row r="163" spans="1:7" ht="26.25">
       <c r="A163" s="14" t="s">
         <v>228</v>
       </c>
@@ -32768,7 +32755,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="75">
+    <row r="164" spans="1:7" ht="51">
       <c r="A164" s="1" t="s">
         <v>538</v>
       </c>
@@ -32788,7 +32775,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="120">
+    <row r="165" spans="1:7" ht="102.75">
       <c r="A165" s="1" t="s">
         <v>65</v>
       </c>
@@ -32808,7 +32795,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="75">
+    <row r="166" spans="1:7" ht="64.5">
       <c r="A166" s="1" t="s">
         <v>65</v>
       </c>
@@ -32828,7 +32815,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="120">
+    <row r="167" spans="1:7" ht="102.75">
       <c r="A167" s="1" t="s">
         <v>65</v>
       </c>
@@ -32848,7 +32835,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="75">
+    <row r="168" spans="1:7" ht="64.5">
       <c r="A168" s="1" t="s">
         <v>65</v>
       </c>
@@ -32868,7 +32855,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="90">
+    <row r="169" spans="1:7" ht="77.25">
       <c r="A169" s="1" t="s">
         <v>65</v>
       </c>
@@ -32888,7 +32875,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="120">
+    <row r="170" spans="1:7" ht="102.75">
       <c r="A170" s="1" t="s">
         <v>65</v>
       </c>
@@ -32908,7 +32895,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="75">
+    <row r="171" spans="1:7" ht="64.5">
       <c r="A171" s="1" t="s">
         <v>65</v>
       </c>
@@ -32928,7 +32915,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="75">
+    <row r="172" spans="1:7" ht="64.5">
       <c r="A172" s="1" t="s">
         <v>65</v>
       </c>
@@ -32948,7 +32935,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="60">
+    <row r="173" spans="1:7" ht="51.75">
       <c r="A173" s="1" t="s">
         <v>117</v>
       </c>
@@ -32968,7 +32955,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="75">
+    <row r="174" spans="1:7" ht="64.5">
       <c r="A174" s="1" t="s">
         <v>223</v>
       </c>
@@ -32988,7 +32975,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="75">
+    <row r="175" spans="1:7" ht="64.5">
       <c r="A175" s="1" t="s">
         <v>223</v>
       </c>
@@ -33008,7 +32995,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="60">
+    <row r="176" spans="1:7" ht="51.75">
       <c r="A176" s="1" t="s">
         <v>17</v>
       </c>
@@ -33028,7 +33015,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="60">
+    <row r="177" spans="1:7" ht="51.75">
       <c r="A177" s="1" t="s">
         <v>587</v>
       </c>
@@ -33048,7 +33035,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="75">
+    <row r="178" spans="1:7" ht="64.5">
       <c r="A178" s="1" t="s">
         <v>588</v>
       </c>
@@ -33068,7 +33055,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="105">
+    <row r="179" spans="1:7" ht="90">
       <c r="A179" s="1" t="s">
         <v>588</v>
       </c>
@@ -33088,7 +33075,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="75">
+    <row r="180" spans="1:7" ht="64.5">
       <c r="A180" s="1" t="s">
         <v>588</v>
       </c>

</xml_diff>

<commit_message>
ToJCRTN feature description corrected
</commit_message>
<xml_diff>
--- a/List_Features_MFTE_python_1.0.xlsx
+++ b/List_Features_MFTE_python_1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Related\PythonCode\MFTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6BBA42-633C-45E6-A9F1-52F8003BA4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E78056-6D54-4F4A-9B1A-48F409708458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="659">
   <si>
     <t>Feature</t>
   </si>
@@ -19018,6 +19018,29 @@
   </si>
   <si>
     <t>Important: The following features consist of aggregates of individual tags. To avoid redundant correlations, undue skew etc. in the data, they should not be used in combination with the respective individual tags. E.g., either use PP1 counts or the counts of PP1S &amp; PP1P, but not all three!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> clauses preceded by certainty adjectives</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -20038,8 +20061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="188" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15"/>
@@ -20187,7 +20210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" ht="114.75">
+    <row r="7" spans="1:7" s="6" customFormat="1" ht="102">
       <c r="A7" s="9" t="s">
         <v>284</v>
       </c>
@@ -30843,7 +30866,7 @@
         <v>65</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>431</v>
+        <v>658</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>421</v>

</xml_diff>